<commit_message>
upload latest data files as of 2019-01-07
upload latest data files as of 2019-01-07 - for Fences and Scaffold
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases BEMSST.xlsx
+++ b/src/com/data/Test Cases BEMSST.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="22545" windowHeight="10125" tabRatio="152" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="3825" yWindow="3375" windowWidth="22290" windowHeight="7515" tabRatio="152" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K21"/>
+  <oleSize ref="A1:K14"/>
 </workbook>
 </file>
 
@@ -2099,8 +2099,8 @@
   <dimension ref="A1:CX262"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F16" sqref="F16"/>
+      <pane xSplit="2" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -5045,7 +5045,7 @@
       <c r="BP33" s="9"/>
       <c r="BQ33" s="9"/>
     </row>
-    <row r="34" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="34" spans="1:102" s="10" customFormat="1">
       <c r="A34" s="9"/>
       <c r="B34" s="17"/>
       <c r="E34" s="9"/>
@@ -5096,7 +5096,7 @@
       <c r="BP34" s="9"/>
       <c r="BQ34" s="9"/>
     </row>
-    <row r="35" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="35" spans="1:102" s="10" customFormat="1">
       <c r="A35" s="9"/>
       <c r="B35" s="17"/>
       <c r="E35" s="9"/>
@@ -5147,7 +5147,7 @@
       <c r="BP35" s="9"/>
       <c r="BQ35" s="9"/>
     </row>
-    <row r="36" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="36" spans="1:102" s="10" customFormat="1">
       <c r="A36" s="9"/>
       <c r="B36" s="17"/>
       <c r="E36" s="9"/>
@@ -5198,7 +5198,7 @@
       <c r="BP36" s="9"/>
       <c r="BQ36" s="9"/>
     </row>
-    <row r="37" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="37" spans="1:102" s="10" customFormat="1">
       <c r="A37" s="9"/>
       <c r="B37" s="17"/>
       <c r="E37" s="9"/>
@@ -5249,7 +5249,7 @@
       <c r="BP37" s="9"/>
       <c r="BQ37" s="9"/>
     </row>
-    <row r="38" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="38" spans="1:102" s="10" customFormat="1">
       <c r="A38" s="9"/>
       <c r="B38" s="17"/>
       <c r="E38" s="9"/>
@@ -5300,7 +5300,7 @@
       <c r="BP38" s="9"/>
       <c r="BQ38" s="9"/>
     </row>
-    <row r="39" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="39" spans="1:102" s="10" customFormat="1">
       <c r="A39" s="9"/>
       <c r="B39" s="17"/>
       <c r="E39" s="9"/>
@@ -5351,7 +5351,7 @@
       <c r="BP39" s="9"/>
       <c r="BQ39" s="9"/>
     </row>
-    <row r="40" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="40" spans="1:102" s="10" customFormat="1">
       <c r="A40" s="9"/>
       <c r="B40" s="17"/>
       <c r="E40" s="9"/>
@@ -5402,7 +5402,7 @@
       <c r="BP40" s="9"/>
       <c r="BQ40" s="9"/>
     </row>
-    <row r="41" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="41" spans="1:102" s="10" customFormat="1">
       <c r="A41" s="9"/>
       <c r="B41" s="17"/>
       <c r="E41" s="9"/>
@@ -5453,7 +5453,7 @@
       <c r="BP41" s="9"/>
       <c r="BQ41" s="9"/>
     </row>
-    <row r="42" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="42" spans="1:102" s="10" customFormat="1">
       <c r="A42" s="9"/>
       <c r="B42" s="17"/>
       <c r="E42" s="9"/>
@@ -5504,7 +5504,7 @@
       <c r="BP42" s="9"/>
       <c r="BQ42" s="9"/>
     </row>
-    <row r="43" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="43" spans="1:102" s="10" customFormat="1">
       <c r="A43" s="9"/>
       <c r="B43" s="17"/>
       <c r="E43" s="9"/>
@@ -5555,7 +5555,7 @@
       <c r="BP43" s="9"/>
       <c r="BQ43" s="9"/>
     </row>
-    <row r="44" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="44" spans="1:102" s="10" customFormat="1">
       <c r="A44" s="9"/>
       <c r="B44" s="17"/>
       <c r="E44" s="9"/>
@@ -5606,7 +5606,7 @@
       <c r="BP44" s="9"/>
       <c r="BQ44" s="9"/>
     </row>
-    <row r="45" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="45" spans="1:102" s="10" customFormat="1">
       <c r="A45" s="9"/>
       <c r="B45" s="17"/>
       <c r="E45" s="9"/>
@@ -5657,7 +5657,7 @@
       <c r="BP45" s="9"/>
       <c r="BQ45" s="9"/>
     </row>
-    <row r="46" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="46" spans="1:102" s="10" customFormat="1">
       <c r="A46" s="9"/>
       <c r="B46" s="17"/>
       <c r="E46" s="9"/>

</xml_diff>

<commit_message>
Data changes as of 2019-01-10
Data changes as of 2019-01-10 - "Test Cases BEMSST.xlsx" "Test Cases Fab4.xlsx"
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases BEMSST.xlsx
+++ b/src/com/data/Test Cases BEMSST.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="3375" windowWidth="22290" windowHeight="7515" tabRatio="152" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1185" windowWidth="23115" windowHeight="11370" tabRatio="152" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="145">
   <si>
     <t>TCID</t>
   </si>
@@ -378,9 +378,6 @@
     <t>Standard Plan Examination or Review</t>
   </si>
   <si>
-    <t>1 :: Electrical Motors :: DOBTESTING123@GMAIL.COM :: Professional Engineer</t>
-  </si>
-  <si>
     <t>StNew</t>
   </si>
   <si>
@@ -444,13 +441,16 @@
     <t>Mechanical Work Boiler Equipment New</t>
   </si>
   <si>
-    <t>111 :: FIRST AVENUE :: MANHATTAN :: 448 :: 28 :: BE1</t>
-  </si>
-  <si>
     <t>111 :: FIRST AVENUE :: MANHATTAN :: 448 :: 28 :: MS1</t>
   </si>
   <si>
     <t>111 :: FIRST AVENUE :: MANHATTAN :: 448 :: 28 :: ST1</t>
+  </si>
+  <si>
+    <t>280 :: BROADWAY :: MANHATTAN :: 153 :: 1 :: BE1</t>
+  </si>
+  <si>
+    <t>1 :: 2 :: N :: N :: N :: N :: N :: N :: N :: N :: N :: N</t>
   </si>
 </sst>
 </file>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1">
       <c r="A2" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="32" t="s">
@@ -1707,7 +1707,7 @@
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1">
       <c r="A3" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="32" t="s">
@@ -1716,7 +1716,7 @@
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1">
       <c r="A4" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="30"/>
       <c r="C4" s="32" t="s">
@@ -2099,8 +2099,8 @@
   <dimension ref="A1:CX262"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U7" sqref="U7"/>
+      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="5" spans="1:102" s="7" customFormat="1">
       <c r="A5" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5" s="6"/>
       <c r="E5" s="6"/>
@@ -2797,7 +2797,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>119</v>
@@ -2806,16 +2806,16 @@
         <v>116</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>109</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>3</v>
@@ -2824,10 +2824,10 @@
         <v>118</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M7" s="11" t="s">
         <v>111</v>
@@ -2850,18 +2850,18 @@
         <v>108</v>
       </c>
       <c r="U7" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="W7" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="V7" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="W7" s="11" t="s">
-        <v>135</v>
       </c>
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
       <c r="Z7" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA7" s="11" t="s">
         <v>27</v>
@@ -3018,7 +3018,7 @@
     </row>
     <row r="9" spans="1:102" s="7" customFormat="1">
       <c r="A9" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B9" s="6"/>
       <c r="E9" s="6"/>
@@ -3351,7 +3351,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>119</v>
@@ -3360,16 +3360,16 @@
         <v>116</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>109</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>3</v>
@@ -3378,10 +3378,10 @@
         <v>118</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>111</v>
@@ -3404,13 +3404,13 @@
         <v>108</v>
       </c>
       <c r="U11" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="V11" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="V11" s="4" t="s">
+      <c r="W11" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="W11" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="X11" s="11"/>
       <c r="Y11" s="11"/>
@@ -3572,7 +3572,7 @@
     </row>
     <row r="13" spans="1:102" s="7" customFormat="1">
       <c r="A13" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B13" s="6"/>
       <c r="E13" s="6"/>
@@ -3905,7 +3905,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>119</v>
@@ -3914,16 +3914,16 @@
         <v>116</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>109</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>3</v>
@@ -3932,10 +3932,10 @@
         <v>118</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M15" s="11" t="s">
         <v>111</v>
@@ -3955,17 +3955,15 @@
         <v>3</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V15" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="W15" s="11" t="s">
-        <v>120</v>
-      </c>
+      <c r="W15" s="11"/>
       <c r="X15" s="11"/>
       <c r="Y15" s="11"/>
       <c r="Z15" s="11" t="s">
@@ -4994,7 +4992,7 @@
       <c r="BP32" s="9"/>
       <c r="BQ32" s="9"/>
     </row>
-    <row r="33" spans="1:102" s="10" customFormat="1">
+    <row r="33" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A33" s="9"/>
       <c r="B33" s="17"/>
       <c r="E33" s="9"/>
@@ -5045,7 +5043,7 @@
       <c r="BP33" s="9"/>
       <c r="BQ33" s="9"/>
     </row>
-    <row r="34" spans="1:102" s="10" customFormat="1">
+    <row r="34" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A34" s="9"/>
       <c r="B34" s="17"/>
       <c r="E34" s="9"/>
@@ -5096,7 +5094,7 @@
       <c r="BP34" s="9"/>
       <c r="BQ34" s="9"/>
     </row>
-    <row r="35" spans="1:102" s="10" customFormat="1">
+    <row r="35" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A35" s="9"/>
       <c r="B35" s="17"/>
       <c r="E35" s="9"/>
@@ -5147,7 +5145,7 @@
       <c r="BP35" s="9"/>
       <c r="BQ35" s="9"/>
     </row>
-    <row r="36" spans="1:102" s="10" customFormat="1">
+    <row r="36" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A36" s="9"/>
       <c r="B36" s="17"/>
       <c r="E36" s="9"/>
@@ -5198,7 +5196,7 @@
       <c r="BP36" s="9"/>
       <c r="BQ36" s="9"/>
     </row>
-    <row r="37" spans="1:102" s="10" customFormat="1">
+    <row r="37" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A37" s="9"/>
       <c r="B37" s="17"/>
       <c r="E37" s="9"/>
@@ -5249,7 +5247,7 @@
       <c r="BP37" s="9"/>
       <c r="BQ37" s="9"/>
     </row>
-    <row r="38" spans="1:102" s="10" customFormat="1">
+    <row r="38" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A38" s="9"/>
       <c r="B38" s="17"/>
       <c r="E38" s="9"/>
@@ -5300,7 +5298,7 @@
       <c r="BP38" s="9"/>
       <c r="BQ38" s="9"/>
     </row>
-    <row r="39" spans="1:102" s="10" customFormat="1">
+    <row r="39" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A39" s="9"/>
       <c r="B39" s="17"/>
       <c r="E39" s="9"/>
@@ -5351,7 +5349,7 @@
       <c r="BP39" s="9"/>
       <c r="BQ39" s="9"/>
     </row>
-    <row r="40" spans="1:102" s="10" customFormat="1">
+    <row r="40" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A40" s="9"/>
       <c r="B40" s="17"/>
       <c r="E40" s="9"/>
@@ -5402,7 +5400,7 @@
       <c r="BP40" s="9"/>
       <c r="BQ40" s="9"/>
     </row>
-    <row r="41" spans="1:102" s="10" customFormat="1">
+    <row r="41" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A41" s="9"/>
       <c r="B41" s="17"/>
       <c r="E41" s="9"/>
@@ -5453,7 +5451,7 @@
       <c r="BP41" s="9"/>
       <c r="BQ41" s="9"/>
     </row>
-    <row r="42" spans="1:102" s="10" customFormat="1">
+    <row r="42" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A42" s="9"/>
       <c r="B42" s="17"/>
       <c r="E42" s="9"/>
@@ -5504,7 +5502,7 @@
       <c r="BP42" s="9"/>
       <c r="BQ42" s="9"/>
     </row>
-    <row r="43" spans="1:102" s="10" customFormat="1">
+    <row r="43" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A43" s="9"/>
       <c r="B43" s="17"/>
       <c r="E43" s="9"/>
@@ -5555,7 +5553,7 @@
       <c r="BP43" s="9"/>
       <c r="BQ43" s="9"/>
     </row>
-    <row r="44" spans="1:102" s="10" customFormat="1">
+    <row r="44" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A44" s="9"/>
       <c r="B44" s="17"/>
       <c r="E44" s="9"/>
@@ -5606,7 +5604,7 @@
       <c r="BP44" s="9"/>
       <c r="BQ44" s="9"/>
     </row>
-    <row r="45" spans="1:102" s="10" customFormat="1">
+    <row r="45" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A45" s="9"/>
       <c r="B45" s="17"/>
       <c r="E45" s="9"/>
@@ -5657,7 +5655,7 @@
       <c r="BP45" s="9"/>
       <c r="BQ45" s="9"/>
     </row>
-    <row r="46" spans="1:102" s="10" customFormat="1">
+    <row r="46" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A46" s="9"/>
       <c r="B46" s="17"/>
       <c r="E46" s="9"/>

</xml_diff>

<commit_message>
data changes as of 2019-01-11
data changes as of 2019-01-11 - bemsst
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases BEMSST.xlsx
+++ b/src/com/data/Test Cases BEMSST.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1185" windowWidth="23115" windowHeight="11370" tabRatio="152" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1185" windowWidth="18090" windowHeight="11145" tabRatio="152" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K14"/>
+  <oleSize ref="A1:K24"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="150">
   <si>
     <t>TCID</t>
   </si>
@@ -381,9 +381,6 @@
     <t>StNew</t>
   </si>
   <si>
-    <t>Structural - New</t>
-  </si>
-  <si>
     <t>Structural</t>
   </si>
   <si>
@@ -394,9 +391,6 @@
   </si>
   <si>
     <t>Structural :: 1111 :: 1.00 :: 3333</t>
-  </si>
-  <si>
-    <t>Mechanical Systems - New</t>
   </si>
   <si>
     <t>Mechanical Work Mechanical Systems</t>
@@ -412,9 +406,6 @@
   </si>
   <si>
     <t>BeNew</t>
-  </si>
-  <si>
-    <t>Boiler Equipment - New</t>
   </si>
   <si>
     <t>Boiler Equipment :: 1111 :: 1.00 :: 3333</t>
@@ -452,12 +443,36 @@
   <si>
     <t>1 :: 2 :: N :: N :: N :: N :: N :: N :: N :: N :: N :: N</t>
   </si>
+  <si>
+    <t>Professional Certification</t>
+  </si>
+  <si>
+    <t>BeProfCertPw2</t>
+  </si>
+  <si>
+    <t>1 :: 1 :: N :: N :: N :: N :: N :: N :: N :: N :: N :: N</t>
+  </si>
+  <si>
+    <t>Boiler Equipment - Standard</t>
+  </si>
+  <si>
+    <t>Mechanical Systems - Standard</t>
+  </si>
+  <si>
+    <t>Structural - Standard</t>
+  </si>
+  <si>
+    <t>Boiler Equipment - Prof Cert - PW2</t>
+  </si>
+  <si>
+    <t>BOILERPLUMBER@GMAIL.COM :: Master Plumber :: THE PLUMBING COMPANY INC :: APPLEROME16@GMAIL.COM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,6 +659,14 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1003,7 +1026,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="128">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1132,8 +1155,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1243,8 +1267,11 @@
     <xf numFmtId="49" fontId="24" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="1" xfId="128" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="128">
+  <cellStyles count="129">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1362,6 +1389,7 @@
     <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1674,7 +1702,7 @@
   <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="12.75"/>
@@ -1698,7 +1726,7 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1">
       <c r="A2" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="32" t="s">
@@ -1707,7 +1735,7 @@
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1">
       <c r="A3" s="34" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="32" t="s">
@@ -1724,9 +1752,13 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">
-      <c r="A5" s="30"/>
+      <c r="A5" s="34" t="s">
+        <v>143</v>
+      </c>
       <c r="B5" s="30"/>
-      <c r="C5" s="33"/>
+      <c r="C5" s="32" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1">
       <c r="A6" s="30"/>
@@ -2096,11 +2128,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CX262"/>
+  <dimension ref="A1:CX266"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W15" sqref="W15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -2128,7 +2160,7 @@
     <col min="21" max="21" width="18" style="9" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="45.7109375" style="9" customWidth="1"/>
     <col min="23" max="23" width="43.28515625" style="9" customWidth="1"/>
-    <col min="24" max="24" width="4.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.7109375" style="9" customWidth="1"/>
     <col min="25" max="25" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" style="9" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="21.7109375" style="9" bestFit="1" customWidth="1"/>
@@ -2464,7 +2496,7 @@
     </row>
     <row r="5" spans="1:102" s="7" customFormat="1">
       <c r="A5" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B5" s="6"/>
       <c r="E5" s="6"/>
@@ -2797,7 +2829,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>119</v>
@@ -2806,16 +2838,16 @@
         <v>116</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>109</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>3</v>
@@ -2824,10 +2856,10 @@
         <v>118</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="M7" s="11" t="s">
         <v>111</v>
@@ -2850,18 +2882,18 @@
         <v>108</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="W7" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
       <c r="Z7" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AA7" s="11" t="s">
         <v>27</v>
@@ -3018,7 +3050,7 @@
     </row>
     <row r="9" spans="1:102" s="7" customFormat="1">
       <c r="A9" s="34" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B9" s="6"/>
       <c r="E9" s="6"/>
@@ -3351,7 +3383,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>119</v>
@@ -3360,16 +3392,16 @@
         <v>116</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>109</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>3</v>
@@ -3378,10 +3410,10 @@
         <v>118</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>111</v>
@@ -3404,13 +3436,13 @@
         <v>108</v>
       </c>
       <c r="U11" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="W11" s="11" t="s">
         <v>128</v>
-      </c>
-      <c r="V11" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="W11" s="11" t="s">
-        <v>130</v>
       </c>
       <c r="X11" s="11"/>
       <c r="Y11" s="11"/>
@@ -3905,7 +3937,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>119</v>
@@ -3914,16 +3946,16 @@
         <v>116</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>109</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>3</v>
@@ -3932,10 +3964,10 @@
         <v>118</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="M15" s="11" t="s">
         <v>111</v>
@@ -3955,10 +3987,10 @@
         <v>3</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="V15" s="4" t="s">
         <v>117</v>
@@ -4122,212 +4154,510 @@
       <c r="BP16" s="9"/>
       <c r="BQ16" s="9"/>
     </row>
-    <row r="17" spans="1:102" s="25" customFormat="1">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="24"/>
-      <c r="AC17" s="24"/>
-      <c r="AD17" s="24"/>
-      <c r="AE17" s="24"/>
-      <c r="AF17" s="24"/>
-      <c r="AG17" s="24"/>
-      <c r="AH17" s="24"/>
-      <c r="AJ17" s="22"/>
-      <c r="AK17" s="22"/>
-      <c r="AL17" s="22"/>
-      <c r="AM17" s="22"/>
-      <c r="AN17" s="22"/>
-      <c r="AO17" s="24"/>
-      <c r="AP17" s="22"/>
-      <c r="AR17" s="22"/>
-      <c r="AS17" s="22"/>
-      <c r="AT17" s="24"/>
-      <c r="AU17" s="22"/>
-      <c r="AV17" s="22"/>
-      <c r="AW17" s="22"/>
-      <c r="AX17" s="22"/>
-      <c r="AY17" s="22"/>
-      <c r="AZ17" s="22"/>
-      <c r="BA17" s="22"/>
-      <c r="BB17" s="24"/>
-      <c r="BC17" s="24"/>
-      <c r="BD17" s="24"/>
-      <c r="BE17" s="22"/>
-      <c r="BF17" s="22"/>
-      <c r="BG17" s="22"/>
-      <c r="BH17" s="22"/>
-      <c r="BI17" s="22"/>
-      <c r="BJ17" s="22"/>
-      <c r="BK17" s="22"/>
-      <c r="BL17" s="22"/>
-      <c r="BM17" s="22"/>
-      <c r="BN17" s="22"/>
-      <c r="BO17" s="22"/>
-      <c r="BP17" s="24"/>
-      <c r="BQ17" s="24"/>
-    </row>
-    <row r="18" spans="1:102" s="25" customFormat="1">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
-      <c r="AB18" s="24"/>
-      <c r="AC18" s="24"/>
-      <c r="AD18" s="24"/>
-      <c r="AE18" s="24"/>
-      <c r="AF18" s="24"/>
-      <c r="AG18" s="24"/>
-      <c r="AH18" s="24"/>
-      <c r="AJ18" s="22"/>
-      <c r="AK18" s="22"/>
-      <c r="AL18" s="22"/>
-      <c r="AM18" s="22"/>
-      <c r="AN18" s="22"/>
-      <c r="AO18" s="24"/>
-      <c r="AP18" s="22"/>
-      <c r="AR18" s="22"/>
-      <c r="AS18" s="22"/>
-      <c r="AT18" s="24"/>
-      <c r="AU18" s="22"/>
-      <c r="AV18" s="22"/>
-      <c r="AW18" s="22"/>
-      <c r="AX18" s="22"/>
-      <c r="AY18" s="22"/>
-      <c r="AZ18" s="22"/>
-      <c r="BA18" s="22"/>
-      <c r="BB18" s="24"/>
-      <c r="BC18" s="24"/>
-      <c r="BD18" s="24"/>
-      <c r="BE18" s="22"/>
-      <c r="BF18" s="22"/>
-      <c r="BG18" s="22"/>
-      <c r="BH18" s="22"/>
-      <c r="BI18" s="22"/>
-      <c r="BJ18" s="22"/>
-      <c r="BK18" s="22"/>
-      <c r="BL18" s="22"/>
-      <c r="BM18" s="22"/>
-      <c r="BN18" s="22"/>
-      <c r="BO18" s="22"/>
-      <c r="BP18" s="24"/>
-      <c r="BQ18" s="24"/>
-    </row>
-    <row r="19" spans="1:102" s="25" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
-      <c r="U19" s="24"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="24"/>
-      <c r="AA19" s="24"/>
-      <c r="AB19" s="24"/>
-      <c r="AC19" s="24"/>
-      <c r="AD19" s="24"/>
-      <c r="AE19" s="24"/>
-      <c r="AF19" s="24"/>
-      <c r="AG19" s="24"/>
-      <c r="AH19" s="24"/>
-      <c r="AJ19" s="22"/>
-      <c r="AK19" s="22"/>
-      <c r="AL19" s="22"/>
-      <c r="AM19" s="22"/>
-      <c r="AN19" s="22"/>
-      <c r="AO19" s="24"/>
-      <c r="AP19" s="22"/>
-      <c r="AR19" s="22"/>
-      <c r="AS19" s="22"/>
-      <c r="AT19" s="24"/>
-      <c r="AU19" s="22"/>
-      <c r="AV19" s="22"/>
-      <c r="AW19" s="22"/>
-      <c r="AX19" s="22"/>
-      <c r="AY19" s="22"/>
-      <c r="AZ19" s="22"/>
-      <c r="BA19" s="22"/>
-      <c r="BB19" s="24"/>
-      <c r="BC19" s="24"/>
-      <c r="BD19" s="24"/>
-      <c r="BE19" s="22"/>
-      <c r="BF19" s="22"/>
-      <c r="BG19" s="22"/>
-      <c r="BH19" s="22"/>
-      <c r="BI19" s="22"/>
-      <c r="BJ19" s="22"/>
-      <c r="BK19" s="22"/>
-      <c r="BL19" s="22"/>
-      <c r="BM19" s="22"/>
-      <c r="BN19" s="22"/>
-      <c r="BO19" s="22"/>
-      <c r="BP19" s="24"/>
-      <c r="BQ19" s="24"/>
+    <row r="17" spans="1:102" s="7" customFormat="1">
+      <c r="A17" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="6"/>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="6"/>
+      <c r="AJ17" s="6"/>
+      <c r="AK17" s="6"/>
+      <c r="AL17" s="6"/>
+      <c r="AM17" s="6"/>
+      <c r="AN17" s="6"/>
+      <c r="AO17" s="6"/>
+      <c r="AP17" s="6"/>
+      <c r="AR17" s="6"/>
+      <c r="AT17" s="6"/>
+      <c r="AU17" s="6"/>
+      <c r="AV17" s="6"/>
+      <c r="AW17" s="6"/>
+      <c r="AX17" s="6"/>
+      <c r="BH17" s="6"/>
+      <c r="BJ17" s="6"/>
+      <c r="BK17" s="6"/>
+      <c r="BL17" s="6"/>
+      <c r="BM17" s="6"/>
+      <c r="BN17" s="6"/>
+      <c r="BO17" s="6"/>
+      <c r="BP17" s="6"/>
+      <c r="BQ17" s="6"/>
+    </row>
+    <row r="18" spans="1:102" s="8" customFormat="1" ht="38.25">
+      <c r="A18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="S18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="T18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="U18" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="V18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="W18" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="X18" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y18" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF18" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG18" s="5"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ18" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK18" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL18" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM18" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN18" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP18" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ18" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR18" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT18" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AU18" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV18" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="AW18" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="AX18" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AY18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="BA18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB18" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="BC18" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="BD18" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF18" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG18" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="BH18" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="BI18" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ18" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="BK18" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="BL18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="BM18" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="BN18" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="BO18" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="BP18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="BQ18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="BR18" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="BS18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BT18" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="BU18" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="BV18" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BW18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BX18" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="BY18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="BZ18" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="CA18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="CB18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CC18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="CD18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="CE18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="CF18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CG18" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="CH18" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="CI18" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="CJ18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="CK18" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="CL18" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="CM18" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="CN18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="CO18" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:102" s="4" customFormat="1" ht="105">
+      <c r="A19" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="R19" s="11"/>
+      <c r="S19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="W19" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="X19" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD19" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE19" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="11"/>
+      <c r="AJ19" s="3"/>
+      <c r="AK19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL19" s="3"/>
+      <c r="AM19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN19" s="3"/>
+      <c r="AO19" s="11"/>
+      <c r="AP19" s="3"/>
+      <c r="AR19" s="3"/>
+      <c r="AS19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT19" s="11"/>
+      <c r="AU19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AV19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AW19" s="3"/>
+      <c r="AX19" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY19" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA19" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB19" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="BC19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="BD19" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="BE19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="BF19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="BG19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="BH19" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="BI19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BJ19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK19" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="BL19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="BM19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="BN19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BO19" s="3"/>
+      <c r="BP19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BQ19" s="18" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20" spans="1:102" s="10" customFormat="1">
       <c r="A20" s="9"/>
@@ -4380,158 +4710,212 @@
       <c r="BP20" s="9"/>
       <c r="BQ20" s="9"/>
     </row>
-    <row r="21" spans="1:102" s="10" customFormat="1">
-      <c r="A21" s="9"/>
-      <c r="B21" s="17"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="9"/>
-      <c r="AJ21" s="9"/>
-      <c r="AK21" s="9"/>
-      <c r="AL21" s="9"/>
-      <c r="AM21" s="9"/>
-      <c r="AN21" s="9"/>
-      <c r="AO21" s="9"/>
-      <c r="AP21" s="9"/>
-      <c r="AR21" s="9"/>
-      <c r="AT21" s="9"/>
-      <c r="AU21" s="9"/>
-      <c r="AV21" s="9"/>
-      <c r="AW21" s="9"/>
-      <c r="AX21" s="9"/>
-      <c r="BH21" s="9"/>
-      <c r="BJ21" s="9"/>
-      <c r="BK21" s="9"/>
-      <c r="BL21" s="9"/>
-      <c r="BM21" s="9"/>
-      <c r="BN21" s="9"/>
-      <c r="BO21" s="9"/>
-      <c r="BP21" s="9"/>
-      <c r="BQ21" s="9"/>
-    </row>
-    <row r="22" spans="1:102" s="10" customFormat="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="17"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="29"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
-      <c r="AB22" s="9"/>
-      <c r="AC22" s="9"/>
-      <c r="AD22" s="9"/>
-      <c r="AE22" s="9"/>
-      <c r="AF22" s="9"/>
-      <c r="AG22" s="9"/>
-      <c r="AH22" s="9"/>
-      <c r="AJ22" s="9"/>
-      <c r="AK22" s="9"/>
-      <c r="AL22" s="9"/>
-      <c r="AM22" s="9"/>
-      <c r="AN22" s="9"/>
-      <c r="AO22" s="9"/>
-      <c r="AP22" s="9"/>
-      <c r="AR22" s="9"/>
-      <c r="AT22" s="9"/>
-      <c r="AU22" s="9"/>
-      <c r="AV22" s="9"/>
-      <c r="AW22" s="9"/>
-      <c r="AX22" s="9"/>
-      <c r="BH22" s="9"/>
-      <c r="BJ22" s="9"/>
-      <c r="BK22" s="9"/>
-      <c r="BL22" s="9"/>
-      <c r="BM22" s="9"/>
-      <c r="BN22" s="9"/>
-      <c r="BO22" s="9"/>
-      <c r="BP22" s="9"/>
-      <c r="BQ22" s="9"/>
-    </row>
-    <row r="23" spans="1:102" s="10" customFormat="1">
-      <c r="A23" s="9"/>
-      <c r="B23" s="17"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="29"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="9"/>
-      <c r="Z23" s="9"/>
-      <c r="AA23" s="9"/>
-      <c r="AB23" s="9"/>
-      <c r="AC23" s="9"/>
-      <c r="AD23" s="9"/>
-      <c r="AE23" s="9"/>
-      <c r="AF23" s="9"/>
-      <c r="AG23" s="9"/>
-      <c r="AH23" s="9"/>
-      <c r="AJ23" s="9"/>
-      <c r="AK23" s="9"/>
-      <c r="AL23" s="9"/>
-      <c r="AM23" s="9"/>
-      <c r="AN23" s="9"/>
-      <c r="AO23" s="9"/>
-      <c r="AP23" s="9"/>
-      <c r="AR23" s="9"/>
-      <c r="AT23" s="9"/>
-      <c r="AU23" s="9"/>
-      <c r="AV23" s="9"/>
-      <c r="AW23" s="9"/>
-      <c r="AX23" s="9"/>
-      <c r="BH23" s="9"/>
-      <c r="BJ23" s="9"/>
-      <c r="BK23" s="9"/>
-      <c r="BL23" s="9"/>
-      <c r="BM23" s="9"/>
-      <c r="BN23" s="9"/>
-      <c r="BO23" s="9"/>
-      <c r="BP23" s="9"/>
-      <c r="BQ23" s="9"/>
+    <row r="21" spans="1:102" s="25" customFormat="1">
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="24"/>
+      <c r="AA21" s="24"/>
+      <c r="AB21" s="24"/>
+      <c r="AC21" s="24"/>
+      <c r="AD21" s="24"/>
+      <c r="AE21" s="24"/>
+      <c r="AF21" s="24"/>
+      <c r="AG21" s="24"/>
+      <c r="AH21" s="24"/>
+      <c r="AJ21" s="22"/>
+      <c r="AK21" s="22"/>
+      <c r="AL21" s="22"/>
+      <c r="AM21" s="22"/>
+      <c r="AN21" s="22"/>
+      <c r="AO21" s="24"/>
+      <c r="AP21" s="22"/>
+      <c r="AR21" s="22"/>
+      <c r="AS21" s="22"/>
+      <c r="AT21" s="24"/>
+      <c r="AU21" s="22"/>
+      <c r="AV21" s="22"/>
+      <c r="AW21" s="22"/>
+      <c r="AX21" s="22"/>
+      <c r="AY21" s="22"/>
+      <c r="AZ21" s="22"/>
+      <c r="BA21" s="22"/>
+      <c r="BB21" s="24"/>
+      <c r="BC21" s="24"/>
+      <c r="BD21" s="24"/>
+      <c r="BE21" s="22"/>
+      <c r="BF21" s="22"/>
+      <c r="BG21" s="22"/>
+      <c r="BH21" s="22"/>
+      <c r="BI21" s="22"/>
+      <c r="BJ21" s="22"/>
+      <c r="BK21" s="22"/>
+      <c r="BL21" s="22"/>
+      <c r="BM21" s="22"/>
+      <c r="BN21" s="22"/>
+      <c r="BO21" s="22"/>
+      <c r="BP21" s="24"/>
+      <c r="BQ21" s="24"/>
+    </row>
+    <row r="22" spans="1:102" s="25" customFormat="1">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="24"/>
+      <c r="Z22" s="24"/>
+      <c r="AA22" s="24"/>
+      <c r="AB22" s="24"/>
+      <c r="AC22" s="24"/>
+      <c r="AD22" s="24"/>
+      <c r="AE22" s="24"/>
+      <c r="AF22" s="24"/>
+      <c r="AG22" s="24"/>
+      <c r="AH22" s="24"/>
+      <c r="AJ22" s="22"/>
+      <c r="AK22" s="22"/>
+      <c r="AL22" s="22"/>
+      <c r="AM22" s="22"/>
+      <c r="AN22" s="22"/>
+      <c r="AO22" s="24"/>
+      <c r="AP22" s="22"/>
+      <c r="AR22" s="22"/>
+      <c r="AS22" s="22"/>
+      <c r="AT22" s="24"/>
+      <c r="AU22" s="22"/>
+      <c r="AV22" s="22"/>
+      <c r="AW22" s="22"/>
+      <c r="AX22" s="22"/>
+      <c r="AY22" s="22"/>
+      <c r="AZ22" s="22"/>
+      <c r="BA22" s="22"/>
+      <c r="BB22" s="24"/>
+      <c r="BC22" s="24"/>
+      <c r="BD22" s="24"/>
+      <c r="BE22" s="22"/>
+      <c r="BF22" s="22"/>
+      <c r="BG22" s="22"/>
+      <c r="BH22" s="22"/>
+      <c r="BI22" s="22"/>
+      <c r="BJ22" s="22"/>
+      <c r="BK22" s="22"/>
+      <c r="BL22" s="22"/>
+      <c r="BM22" s="22"/>
+      <c r="BN22" s="22"/>
+      <c r="BO22" s="22"/>
+      <c r="BP22" s="24"/>
+      <c r="BQ22" s="24"/>
+    </row>
+    <row r="23" spans="1:102" s="25" customFormat="1">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="24"/>
+      <c r="W23" s="24"/>
+      <c r="X23" s="24"/>
+      <c r="Y23" s="24"/>
+      <c r="Z23" s="24"/>
+      <c r="AA23" s="24"/>
+      <c r="AB23" s="24"/>
+      <c r="AC23" s="24"/>
+      <c r="AD23" s="24"/>
+      <c r="AE23" s="24"/>
+      <c r="AF23" s="24"/>
+      <c r="AG23" s="24"/>
+      <c r="AH23" s="24"/>
+      <c r="AJ23" s="22"/>
+      <c r="AK23" s="22"/>
+      <c r="AL23" s="22"/>
+      <c r="AM23" s="22"/>
+      <c r="AN23" s="22"/>
+      <c r="AO23" s="24"/>
+      <c r="AP23" s="22"/>
+      <c r="AR23" s="22"/>
+      <c r="AS23" s="22"/>
+      <c r="AT23" s="24"/>
+      <c r="AU23" s="22"/>
+      <c r="AV23" s="22"/>
+      <c r="AW23" s="22"/>
+      <c r="AX23" s="22"/>
+      <c r="AY23" s="22"/>
+      <c r="AZ23" s="22"/>
+      <c r="BA23" s="22"/>
+      <c r="BB23" s="24"/>
+      <c r="BC23" s="24"/>
+      <c r="BD23" s="24"/>
+      <c r="BE23" s="22"/>
+      <c r="BF23" s="22"/>
+      <c r="BG23" s="22"/>
+      <c r="BH23" s="22"/>
+      <c r="BI23" s="22"/>
+      <c r="BJ23" s="22"/>
+      <c r="BK23" s="22"/>
+      <c r="BL23" s="22"/>
+      <c r="BM23" s="22"/>
+      <c r="BN23" s="22"/>
+      <c r="BO23" s="22"/>
+      <c r="BP23" s="24"/>
+      <c r="BQ23" s="24"/>
     </row>
     <row r="24" spans="1:102" s="10" customFormat="1">
       <c r="A24" s="9"/>
@@ -4992,7 +5376,7 @@
       <c r="BP32" s="9"/>
       <c r="BQ32" s="9"/>
     </row>
-    <row r="33" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="33" spans="1:102" s="10" customFormat="1">
       <c r="A33" s="9"/>
       <c r="B33" s="17"/>
       <c r="E33" s="9"/>
@@ -5043,7 +5427,7 @@
       <c r="BP33" s="9"/>
       <c r="BQ33" s="9"/>
     </row>
-    <row r="34" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="34" spans="1:102" s="10" customFormat="1">
       <c r="A34" s="9"/>
       <c r="B34" s="17"/>
       <c r="E34" s="9"/>
@@ -5094,7 +5478,7 @@
       <c r="BP34" s="9"/>
       <c r="BQ34" s="9"/>
     </row>
-    <row r="35" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="35" spans="1:102" s="10" customFormat="1">
       <c r="A35" s="9"/>
       <c r="B35" s="17"/>
       <c r="E35" s="9"/>
@@ -5145,7 +5529,7 @@
       <c r="BP35" s="9"/>
       <c r="BQ35" s="9"/>
     </row>
-    <row r="36" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="36" spans="1:102" s="10" customFormat="1">
       <c r="A36" s="9"/>
       <c r="B36" s="17"/>
       <c r="E36" s="9"/>
@@ -5196,7 +5580,7 @@
       <c r="BP36" s="9"/>
       <c r="BQ36" s="9"/>
     </row>
-    <row r="37" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="37" spans="1:102" s="10" customFormat="1">
       <c r="A37" s="9"/>
       <c r="B37" s="17"/>
       <c r="E37" s="9"/>
@@ -5247,7 +5631,7 @@
       <c r="BP37" s="9"/>
       <c r="BQ37" s="9"/>
     </row>
-    <row r="38" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="38" spans="1:102" s="10" customFormat="1">
       <c r="A38" s="9"/>
       <c r="B38" s="17"/>
       <c r="E38" s="9"/>
@@ -16722,8 +17106,215 @@
       <c r="BP262" s="9"/>
       <c r="BQ262" s="9"/>
     </row>
+    <row r="263" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A263" s="9"/>
+      <c r="B263" s="17"/>
+      <c r="E263" s="9"/>
+      <c r="F263" s="9"/>
+      <c r="G263" s="9"/>
+      <c r="K263" s="28"/>
+      <c r="L263" s="9"/>
+      <c r="M263" s="9"/>
+      <c r="N263" s="9"/>
+      <c r="O263" s="9"/>
+      <c r="P263" s="9"/>
+      <c r="Q263" s="29"/>
+      <c r="R263" s="29"/>
+      <c r="U263" s="9"/>
+      <c r="V263" s="9"/>
+      <c r="W263" s="9"/>
+      <c r="X263" s="9"/>
+      <c r="Y263" s="9"/>
+      <c r="Z263" s="9"/>
+      <c r="AA263" s="9"/>
+      <c r="AB263" s="9"/>
+      <c r="AC263" s="9"/>
+      <c r="AD263" s="9"/>
+      <c r="AE263" s="9"/>
+      <c r="AF263" s="9"/>
+      <c r="AG263" s="9"/>
+      <c r="AH263" s="9"/>
+      <c r="AJ263" s="9"/>
+      <c r="AK263" s="9"/>
+      <c r="AL263" s="9"/>
+      <c r="AM263" s="9"/>
+      <c r="AN263" s="9"/>
+      <c r="AO263" s="9"/>
+      <c r="AP263" s="9"/>
+      <c r="AR263" s="9"/>
+      <c r="AT263" s="9"/>
+      <c r="AU263" s="9"/>
+      <c r="AV263" s="9"/>
+      <c r="AW263" s="9"/>
+      <c r="AX263" s="9"/>
+      <c r="BH263" s="9"/>
+      <c r="BJ263" s="9"/>
+      <c r="BK263" s="9"/>
+      <c r="BL263" s="9"/>
+      <c r="BM263" s="9"/>
+      <c r="BN263" s="9"/>
+      <c r="BO263" s="9"/>
+      <c r="BP263" s="9"/>
+      <c r="BQ263" s="9"/>
+    </row>
+    <row r="264" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A264" s="9"/>
+      <c r="B264" s="17"/>
+      <c r="E264" s="9"/>
+      <c r="F264" s="9"/>
+      <c r="G264" s="9"/>
+      <c r="K264" s="28"/>
+      <c r="L264" s="9"/>
+      <c r="M264" s="9"/>
+      <c r="N264" s="9"/>
+      <c r="O264" s="9"/>
+      <c r="P264" s="9"/>
+      <c r="Q264" s="29"/>
+      <c r="R264" s="29"/>
+      <c r="U264" s="9"/>
+      <c r="V264" s="9"/>
+      <c r="W264" s="9"/>
+      <c r="X264" s="9"/>
+      <c r="Y264" s="9"/>
+      <c r="Z264" s="9"/>
+      <c r="AA264" s="9"/>
+      <c r="AB264" s="9"/>
+      <c r="AC264" s="9"/>
+      <c r="AD264" s="9"/>
+      <c r="AE264" s="9"/>
+      <c r="AF264" s="9"/>
+      <c r="AG264" s="9"/>
+      <c r="AH264" s="9"/>
+      <c r="AJ264" s="9"/>
+      <c r="AK264" s="9"/>
+      <c r="AL264" s="9"/>
+      <c r="AM264" s="9"/>
+      <c r="AN264" s="9"/>
+      <c r="AO264" s="9"/>
+      <c r="AP264" s="9"/>
+      <c r="AR264" s="9"/>
+      <c r="AT264" s="9"/>
+      <c r="AU264" s="9"/>
+      <c r="AV264" s="9"/>
+      <c r="AW264" s="9"/>
+      <c r="AX264" s="9"/>
+      <c r="BH264" s="9"/>
+      <c r="BJ264" s="9"/>
+      <c r="BK264" s="9"/>
+      <c r="BL264" s="9"/>
+      <c r="BM264" s="9"/>
+      <c r="BN264" s="9"/>
+      <c r="BO264" s="9"/>
+      <c r="BP264" s="9"/>
+      <c r="BQ264" s="9"/>
+    </row>
+    <row r="265" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A265" s="9"/>
+      <c r="B265" s="17"/>
+      <c r="E265" s="9"/>
+      <c r="F265" s="9"/>
+      <c r="G265" s="9"/>
+      <c r="K265" s="28"/>
+      <c r="L265" s="9"/>
+      <c r="M265" s="9"/>
+      <c r="N265" s="9"/>
+      <c r="O265" s="9"/>
+      <c r="P265" s="9"/>
+      <c r="Q265" s="29"/>
+      <c r="R265" s="29"/>
+      <c r="U265" s="9"/>
+      <c r="V265" s="9"/>
+      <c r="W265" s="9"/>
+      <c r="X265" s="9"/>
+      <c r="Y265" s="9"/>
+      <c r="Z265" s="9"/>
+      <c r="AA265" s="9"/>
+      <c r="AB265" s="9"/>
+      <c r="AC265" s="9"/>
+      <c r="AD265" s="9"/>
+      <c r="AE265" s="9"/>
+      <c r="AF265" s="9"/>
+      <c r="AG265" s="9"/>
+      <c r="AH265" s="9"/>
+      <c r="AJ265" s="9"/>
+      <c r="AK265" s="9"/>
+      <c r="AL265" s="9"/>
+      <c r="AM265" s="9"/>
+      <c r="AN265" s="9"/>
+      <c r="AO265" s="9"/>
+      <c r="AP265" s="9"/>
+      <c r="AR265" s="9"/>
+      <c r="AT265" s="9"/>
+      <c r="AU265" s="9"/>
+      <c r="AV265" s="9"/>
+      <c r="AW265" s="9"/>
+      <c r="AX265" s="9"/>
+      <c r="BH265" s="9"/>
+      <c r="BJ265" s="9"/>
+      <c r="BK265" s="9"/>
+      <c r="BL265" s="9"/>
+      <c r="BM265" s="9"/>
+      <c r="BN265" s="9"/>
+      <c r="BO265" s="9"/>
+      <c r="BP265" s="9"/>
+      <c r="BQ265" s="9"/>
+    </row>
+    <row r="266" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A266" s="9"/>
+      <c r="B266" s="17"/>
+      <c r="E266" s="9"/>
+      <c r="F266" s="9"/>
+      <c r="G266" s="9"/>
+      <c r="K266" s="28"/>
+      <c r="L266" s="9"/>
+      <c r="M266" s="9"/>
+      <c r="N266" s="9"/>
+      <c r="O266" s="9"/>
+      <c r="P266" s="9"/>
+      <c r="Q266" s="29"/>
+      <c r="R266" s="29"/>
+      <c r="U266" s="9"/>
+      <c r="V266" s="9"/>
+      <c r="W266" s="9"/>
+      <c r="X266" s="9"/>
+      <c r="Y266" s="9"/>
+      <c r="Z266" s="9"/>
+      <c r="AA266" s="9"/>
+      <c r="AB266" s="9"/>
+      <c r="AC266" s="9"/>
+      <c r="AD266" s="9"/>
+      <c r="AE266" s="9"/>
+      <c r="AF266" s="9"/>
+      <c r="AG266" s="9"/>
+      <c r="AH266" s="9"/>
+      <c r="AJ266" s="9"/>
+      <c r="AK266" s="9"/>
+      <c r="AL266" s="9"/>
+      <c r="AM266" s="9"/>
+      <c r="AN266" s="9"/>
+      <c r="AO266" s="9"/>
+      <c r="AP266" s="9"/>
+      <c r="AR266" s="9"/>
+      <c r="AT266" s="9"/>
+      <c r="AU266" s="9"/>
+      <c r="AV266" s="9"/>
+      <c r="AW266" s="9"/>
+      <c r="AX266" s="9"/>
+      <c r="BH266" s="9"/>
+      <c r="BJ266" s="9"/>
+      <c r="BK266" s="9"/>
+      <c r="BL266" s="9"/>
+      <c r="BM266" s="9"/>
+      <c r="BN266" s="9"/>
+      <c r="BO266" s="9"/>
+      <c r="BP266" s="9"/>
+      <c r="BQ266" s="9"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="X19" r:id="rId1" display="BOILERSOIL@GMAIL.COM :: Oil Burner Installer :: CONTROLLED PLBG CO., INC"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
latest data files as of 2019-01-15
latest data files as of 2019-01-15 - bemsst, fab4
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases BEMSST.xlsx
+++ b/src/com/data/Test Cases BEMSST.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1185" windowWidth="18090" windowHeight="11145" tabRatio="152" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="33330" yWindow="2715" windowWidth="21645" windowHeight="7155" tabRatio="152" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K24"/>
+  <oleSize ref="A13:J23"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="162">
   <si>
     <t>TCID</t>
   </si>
@@ -366,9 +366,6 @@
     <t>user_info</t>
   </si>
   <si>
-    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2</t>
-  </si>
-  <si>
     <t>1 :: DOBTESTING123@GMAIL.COM :: Professional Engineer :: 005551 :: Fuel-Oil Storage and Fuel-Oil Piping Systems</t>
   </si>
   <si>
@@ -426,9 +423,6 @@
     <t>1 :: N :: Y :: N :: N :: N :: N :: N :: N :: N :: N</t>
   </si>
   <si>
-    <t>boiler</t>
-  </si>
-  <si>
     <t>Mechanical Work Boiler Equipment New</t>
   </si>
   <si>
@@ -447,9 +441,6 @@
     <t>Professional Certification</t>
   </si>
   <si>
-    <t>BeProfCertPw2</t>
-  </si>
-  <si>
     <t>1 :: 1 :: N :: N :: N :: N :: N :: N :: N :: N :: N :: N</t>
   </si>
   <si>
@@ -466,6 +457,51 @@
   </si>
   <si>
     <t>BOILERPLUMBER@GMAIL.COM :: Master Plumber :: THE PLUMBING COMPANY INC :: APPLEROME16@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>Boiler Equipment - New - Standard</t>
+  </si>
+  <si>
+    <t>AJOETEST@GMAIL.COM :: Mechanical Work :: 2 :: 1 :: 1</t>
+  </si>
+  <si>
+    <t>AJOETEST@GMAIL.COM :: Professional Engineer :: JA&amp; LLC</t>
+  </si>
+  <si>
+    <t>a :: AJOETEST@GMAIL.COM :: Professional Engineer :: 005546 :: Lowest Floor Elevation</t>
+  </si>
+  <si>
+    <t>q :: Maintenance information :: AJOETEST@GMAIL.COM :: Professional Engineer</t>
+  </si>
+  <si>
+    <t>AJOETEST@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>AJOETEST@GMAIL.COM :: Professional Engineer :: JA&amp; LLC :: APPLEROME16@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2 :: APPLEROME16@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>boiler :: AJOETEST@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>boiler :: APPLEROME18@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>Y :: APPLEROME18@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: JA&amp; LLC</t>
+  </si>
+  <si>
+    <t>a :: DOBTESTING123@GMAIL.COM :: Professional Engineer :: 005546 :: Fuel-Oil Storage and Fuel-Oil Piping Systems</t>
+  </si>
+  <si>
+    <t>BeNewStd</t>
+  </si>
+  <si>
+    <t>BeNewProPw2</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1193,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1268,6 +1304,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="26" fillId="0" borderId="1" xfId="128" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="1" xfId="128" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="128" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1726,7 +1768,7 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1">
       <c r="A2" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="32" t="s">
@@ -1735,7 +1777,7 @@
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1">
       <c r="A3" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="32" t="s">
@@ -1744,7 +1786,7 @@
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1">
       <c r="A4" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="30"/>
       <c r="C4" s="32" t="s">
@@ -1753,7 +1795,7 @@
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">
       <c r="A5" s="34" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="32" t="s">
@@ -1761,9 +1803,13 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1">
-      <c r="A6" s="30"/>
+      <c r="A6" s="34" t="s">
+        <v>160</v>
+      </c>
       <c r="B6" s="30"/>
-      <c r="C6" s="33"/>
+      <c r="C6" s="32" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1">
       <c r="A7" s="30"/>
@@ -2128,11 +2174,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CX266"/>
+  <dimension ref="A1:CX271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X20" sqref="X20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -2141,7 +2187,7 @@
     <col min="2" max="2" width="33.140625" style="17" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="9" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" style="9" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" style="9" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" style="10" customWidth="1"/>
@@ -2496,7 +2542,7 @@
     </row>
     <row r="5" spans="1:102" s="7" customFormat="1">
       <c r="A5" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="6"/>
       <c r="E5" s="6"/>
@@ -2824,42 +2870,42 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:102" s="4" customFormat="1" ht="51">
+    <row r="7" spans="1:102" s="4" customFormat="1" ht="63.75">
       <c r="A7" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>109</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M7" s="11" t="s">
         <v>111</v>
@@ -2878,22 +2924,22 @@
       <c r="S7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="T7" s="4" t="s">
-        <v>108</v>
+      <c r="T7" s="39" t="s">
+        <v>158</v>
       </c>
       <c r="U7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="W7" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="V7" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="W7" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
       <c r="Z7" s="11" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="AA7" s="11" t="s">
         <v>27</v>
@@ -3050,7 +3096,7 @@
     </row>
     <row r="9" spans="1:102" s="7" customFormat="1">
       <c r="A9" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B9" s="6"/>
       <c r="E9" s="6"/>
@@ -3378,42 +3424,42 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:102" s="4" customFormat="1" ht="51">
+    <row r="11" spans="1:102" s="4" customFormat="1" ht="63.75">
       <c r="A11" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>109</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>111</v>
@@ -3436,18 +3482,18 @@
         <v>108</v>
       </c>
       <c r="U11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="V11" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="V11" s="4" t="s">
+      <c r="W11" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="W11" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="X11" s="11"/>
       <c r="Y11" s="11"/>
       <c r="Z11" s="11" t="s">
-        <v>3</v>
+        <v>157</v>
       </c>
       <c r="AA11" s="11" t="s">
         <v>27</v>
@@ -3604,7 +3650,7 @@
     </row>
     <row r="13" spans="1:102" s="7" customFormat="1">
       <c r="A13" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B13" s="6"/>
       <c r="E13" s="6"/>
@@ -3932,42 +3978,42 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:102" s="4" customFormat="1" ht="38.25">
+    <row r="15" spans="1:102" s="4" customFormat="1" ht="63.75">
       <c r="A15" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>109</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M15" s="11" t="s">
         <v>111</v>
@@ -3987,19 +4033,19 @@
         <v>3</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V15" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
       <c r="Y15" s="11"/>
       <c r="Z15" s="11" t="s">
-        <v>3</v>
+        <v>157</v>
       </c>
       <c r="AA15" s="11" t="s">
         <v>27</v>
@@ -4156,7 +4202,7 @@
     </row>
     <row r="17" spans="1:102" s="7" customFormat="1">
       <c r="A17" s="34" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="B17" s="6"/>
       <c r="E17" s="6"/>
@@ -4489,37 +4535,37 @@
         <v>3</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>109</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M19" s="11" t="s">
         <v>111</v>
@@ -4538,24 +4584,24 @@
       <c r="S19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="T19" s="4" t="s">
-        <v>108</v>
+      <c r="T19" s="39" t="s">
+        <v>158</v>
       </c>
       <c r="U19" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="W19" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="V19" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="W19" s="11" t="s">
-        <v>131</v>
-      </c>
       <c r="X19" s="39" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="Y19" s="11"/>
       <c r="Z19" s="11" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="AA19" s="11" t="s">
         <v>27</v>
@@ -4710,212 +4756,510 @@
       <c r="BP20" s="9"/>
       <c r="BQ20" s="9"/>
     </row>
-    <row r="21" spans="1:102" s="25" customFormat="1">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="22"/>
-      <c r="T21" s="22"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="24"/>
-      <c r="Z21" s="24"/>
-      <c r="AA21" s="24"/>
-      <c r="AB21" s="24"/>
-      <c r="AC21" s="24"/>
-      <c r="AD21" s="24"/>
-      <c r="AE21" s="24"/>
-      <c r="AF21" s="24"/>
-      <c r="AG21" s="24"/>
-      <c r="AH21" s="24"/>
-      <c r="AJ21" s="22"/>
-      <c r="AK21" s="22"/>
-      <c r="AL21" s="22"/>
-      <c r="AM21" s="22"/>
-      <c r="AN21" s="22"/>
-      <c r="AO21" s="24"/>
-      <c r="AP21" s="22"/>
-      <c r="AR21" s="22"/>
-      <c r="AS21" s="22"/>
-      <c r="AT21" s="24"/>
-      <c r="AU21" s="22"/>
-      <c r="AV21" s="22"/>
-      <c r="AW21" s="22"/>
-      <c r="AX21" s="22"/>
-      <c r="AY21" s="22"/>
-      <c r="AZ21" s="22"/>
-      <c r="BA21" s="22"/>
-      <c r="BB21" s="24"/>
-      <c r="BC21" s="24"/>
-      <c r="BD21" s="24"/>
-      <c r="BE21" s="22"/>
-      <c r="BF21" s="22"/>
-      <c r="BG21" s="22"/>
-      <c r="BH21" s="22"/>
-      <c r="BI21" s="22"/>
-      <c r="BJ21" s="22"/>
-      <c r="BK21" s="22"/>
-      <c r="BL21" s="22"/>
-      <c r="BM21" s="22"/>
-      <c r="BN21" s="22"/>
-      <c r="BO21" s="22"/>
-      <c r="BP21" s="24"/>
-      <c r="BQ21" s="24"/>
-    </row>
-    <row r="22" spans="1:102" s="25" customFormat="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="22"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="24"/>
-      <c r="Z22" s="24"/>
-      <c r="AA22" s="24"/>
-      <c r="AB22" s="24"/>
-      <c r="AC22" s="24"/>
-      <c r="AD22" s="24"/>
-      <c r="AE22" s="24"/>
-      <c r="AF22" s="24"/>
-      <c r="AG22" s="24"/>
-      <c r="AH22" s="24"/>
-      <c r="AJ22" s="22"/>
-      <c r="AK22" s="22"/>
-      <c r="AL22" s="22"/>
-      <c r="AM22" s="22"/>
-      <c r="AN22" s="22"/>
-      <c r="AO22" s="24"/>
-      <c r="AP22" s="22"/>
-      <c r="AR22" s="22"/>
-      <c r="AS22" s="22"/>
-      <c r="AT22" s="24"/>
-      <c r="AU22" s="22"/>
-      <c r="AV22" s="22"/>
-      <c r="AW22" s="22"/>
-      <c r="AX22" s="22"/>
-      <c r="AY22" s="22"/>
-      <c r="AZ22" s="22"/>
-      <c r="BA22" s="22"/>
-      <c r="BB22" s="24"/>
-      <c r="BC22" s="24"/>
-      <c r="BD22" s="24"/>
-      <c r="BE22" s="22"/>
-      <c r="BF22" s="22"/>
-      <c r="BG22" s="22"/>
-      <c r="BH22" s="22"/>
-      <c r="BI22" s="22"/>
-      <c r="BJ22" s="22"/>
-      <c r="BK22" s="22"/>
-      <c r="BL22" s="22"/>
-      <c r="BM22" s="22"/>
-      <c r="BN22" s="22"/>
-      <c r="BO22" s="22"/>
-      <c r="BP22" s="24"/>
-      <c r="BQ22" s="24"/>
-    </row>
-    <row r="23" spans="1:102" s="25" customFormat="1">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="22"/>
-      <c r="T23" s="22"/>
-      <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="24"/>
-      <c r="Z23" s="24"/>
-      <c r="AA23" s="24"/>
-      <c r="AB23" s="24"/>
-      <c r="AC23" s="24"/>
-      <c r="AD23" s="24"/>
-      <c r="AE23" s="24"/>
-      <c r="AF23" s="24"/>
-      <c r="AG23" s="24"/>
-      <c r="AH23" s="24"/>
-      <c r="AJ23" s="22"/>
-      <c r="AK23" s="22"/>
-      <c r="AL23" s="22"/>
-      <c r="AM23" s="22"/>
-      <c r="AN23" s="22"/>
-      <c r="AO23" s="24"/>
-      <c r="AP23" s="22"/>
-      <c r="AR23" s="22"/>
-      <c r="AS23" s="22"/>
-      <c r="AT23" s="24"/>
-      <c r="AU23" s="22"/>
-      <c r="AV23" s="22"/>
-      <c r="AW23" s="22"/>
-      <c r="AX23" s="22"/>
-      <c r="AY23" s="22"/>
-      <c r="AZ23" s="22"/>
-      <c r="BA23" s="22"/>
-      <c r="BB23" s="24"/>
-      <c r="BC23" s="24"/>
-      <c r="BD23" s="24"/>
-      <c r="BE23" s="22"/>
-      <c r="BF23" s="22"/>
-      <c r="BG23" s="22"/>
-      <c r="BH23" s="22"/>
-      <c r="BI23" s="22"/>
-      <c r="BJ23" s="22"/>
-      <c r="BK23" s="22"/>
-      <c r="BL23" s="22"/>
-      <c r="BM23" s="22"/>
-      <c r="BN23" s="22"/>
-      <c r="BO23" s="22"/>
-      <c r="BP23" s="24"/>
-      <c r="BQ23" s="24"/>
+    <row r="21" spans="1:102" s="7" customFormat="1">
+      <c r="A21" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6"/>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="6"/>
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="6"/>
+      <c r="AJ21" s="6"/>
+      <c r="AK21" s="6"/>
+      <c r="AL21" s="6"/>
+      <c r="AM21" s="6"/>
+      <c r="AN21" s="6"/>
+      <c r="AO21" s="6"/>
+      <c r="AP21" s="6"/>
+      <c r="AR21" s="6"/>
+      <c r="AT21" s="6"/>
+      <c r="AU21" s="6"/>
+      <c r="AV21" s="6"/>
+      <c r="AW21" s="6"/>
+      <c r="AX21" s="6"/>
+      <c r="BH21" s="6"/>
+      <c r="BJ21" s="6"/>
+      <c r="BK21" s="6"/>
+      <c r="BL21" s="6"/>
+      <c r="BM21" s="6"/>
+      <c r="BN21" s="6"/>
+      <c r="BO21" s="6"/>
+      <c r="BP21" s="6"/>
+      <c r="BQ21" s="6"/>
+    </row>
+    <row r="22" spans="1:102" s="8" customFormat="1" ht="38.25">
+      <c r="A22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="S22" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="T22" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="U22" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="V22" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="W22" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="X22" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y22" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z22" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE22" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF22" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG22" s="5"/>
+      <c r="AH22" s="5"/>
+      <c r="AI22" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK22" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL22" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM22" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP22" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ22" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR22" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS22" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AU22" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV22" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="AW22" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="AX22" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AY22" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="BA22" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB22" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="BC22" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="BD22" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE22" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF22" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG22" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="BH22" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="BI22" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ22" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="BK22" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="BL22" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="BM22" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="BN22" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="BO22" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="BP22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="BQ22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="BR22" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="BS22" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BT22" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="BU22" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="BV22" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BW22" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BX22" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="BY22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="BZ22" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="CA22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="CB22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CC22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="CD22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="CE22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="CF22" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CG22" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="CH22" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="CI22" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="CJ22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="CK22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="CL22" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="CM22" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="CN22" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="CO22" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:102" s="4" customFormat="1" ht="105">
+      <c r="A23" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q23" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="R23" s="11"/>
+      <c r="S23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T23" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="W23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="X23" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA23" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB23" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC23" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD23" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE23" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF23" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG23" s="11"/>
+      <c r="AH23" s="11"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN23" s="3"/>
+      <c r="AO23" s="11"/>
+      <c r="AP23" s="3"/>
+      <c r="AR23" s="3"/>
+      <c r="AS23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT23" s="11"/>
+      <c r="AU23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AV23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AW23" s="3"/>
+      <c r="AX23" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA23" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB23" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="BC23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="BD23" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="BE23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="BF23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="BG23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="BH23" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="BI23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BJ23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK23" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="BL23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="BM23" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="BN23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BO23" s="3"/>
+      <c r="BP23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BQ23" s="18" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" spans="1:102" s="10" customFormat="1">
       <c r="A24" s="9"/>
@@ -5019,158 +5363,212 @@
       <c r="BP25" s="9"/>
       <c r="BQ25" s="9"/>
     </row>
-    <row r="26" spans="1:102" s="10" customFormat="1">
-      <c r="A26" s="9"/>
-      <c r="B26" s="17"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="29"/>
-      <c r="R26" s="29"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
-      <c r="X26" s="9"/>
-      <c r="Y26" s="9"/>
-      <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
-      <c r="AB26" s="9"/>
-      <c r="AC26" s="9"/>
-      <c r="AD26" s="9"/>
-      <c r="AE26" s="9"/>
-      <c r="AF26" s="9"/>
-      <c r="AG26" s="9"/>
-      <c r="AH26" s="9"/>
-      <c r="AJ26" s="9"/>
-      <c r="AK26" s="9"/>
-      <c r="AL26" s="9"/>
-      <c r="AM26" s="9"/>
-      <c r="AN26" s="9"/>
-      <c r="AO26" s="9"/>
-      <c r="AP26" s="9"/>
-      <c r="AR26" s="9"/>
-      <c r="AT26" s="9"/>
-      <c r="AU26" s="9"/>
-      <c r="AV26" s="9"/>
-      <c r="AW26" s="9"/>
-      <c r="AX26" s="9"/>
-      <c r="BH26" s="9"/>
-      <c r="BJ26" s="9"/>
-      <c r="BK26" s="9"/>
-      <c r="BL26" s="9"/>
-      <c r="BM26" s="9"/>
-      <c r="BN26" s="9"/>
-      <c r="BO26" s="9"/>
-      <c r="BP26" s="9"/>
-      <c r="BQ26" s="9"/>
-    </row>
-    <row r="27" spans="1:102" s="10" customFormat="1">
-      <c r="A27" s="9"/>
-      <c r="B27" s="17"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="29"/>
-      <c r="R27" s="29"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="9"/>
-      <c r="AA27" s="9"/>
-      <c r="AB27" s="9"/>
-      <c r="AC27" s="9"/>
-      <c r="AD27" s="9"/>
-      <c r="AE27" s="9"/>
-      <c r="AF27" s="9"/>
-      <c r="AG27" s="9"/>
-      <c r="AH27" s="9"/>
-      <c r="AJ27" s="9"/>
-      <c r="AK27" s="9"/>
-      <c r="AL27" s="9"/>
-      <c r="AM27" s="9"/>
-      <c r="AN27" s="9"/>
-      <c r="AO27" s="9"/>
-      <c r="AP27" s="9"/>
-      <c r="AR27" s="9"/>
-      <c r="AT27" s="9"/>
-      <c r="AU27" s="9"/>
-      <c r="AV27" s="9"/>
-      <c r="AW27" s="9"/>
-      <c r="AX27" s="9"/>
-      <c r="BH27" s="9"/>
-      <c r="BJ27" s="9"/>
-      <c r="BK27" s="9"/>
-      <c r="BL27" s="9"/>
-      <c r="BM27" s="9"/>
-      <c r="BN27" s="9"/>
-      <c r="BO27" s="9"/>
-      <c r="BP27" s="9"/>
-      <c r="BQ27" s="9"/>
-    </row>
-    <row r="28" spans="1:102" s="10" customFormat="1">
-      <c r="A28" s="9"/>
-      <c r="B28" s="17"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="29"/>
-      <c r="R28" s="29"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9"/>
-      <c r="W28" s="9"/>
-      <c r="X28" s="9"/>
-      <c r="Y28" s="9"/>
-      <c r="Z28" s="9"/>
-      <c r="AA28" s="9"/>
-      <c r="AB28" s="9"/>
-      <c r="AC28" s="9"/>
-      <c r="AD28" s="9"/>
-      <c r="AE28" s="9"/>
-      <c r="AF28" s="9"/>
-      <c r="AG28" s="9"/>
-      <c r="AH28" s="9"/>
-      <c r="AJ28" s="9"/>
-      <c r="AK28" s="9"/>
-      <c r="AL28" s="9"/>
-      <c r="AM28" s="9"/>
-      <c r="AN28" s="9"/>
-      <c r="AO28" s="9"/>
-      <c r="AP28" s="9"/>
-      <c r="AR28" s="9"/>
-      <c r="AT28" s="9"/>
-      <c r="AU28" s="9"/>
-      <c r="AV28" s="9"/>
-      <c r="AW28" s="9"/>
-      <c r="AX28" s="9"/>
-      <c r="BH28" s="9"/>
-      <c r="BJ28" s="9"/>
-      <c r="BK28" s="9"/>
-      <c r="BL28" s="9"/>
-      <c r="BM28" s="9"/>
-      <c r="BN28" s="9"/>
-      <c r="BO28" s="9"/>
-      <c r="BP28" s="9"/>
-      <c r="BQ28" s="9"/>
+    <row r="26" spans="1:102" s="25" customFormat="1">
+      <c r="A26" s="22"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
+      <c r="U26" s="24"/>
+      <c r="V26" s="24"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="24"/>
+      <c r="Y26" s="24"/>
+      <c r="Z26" s="24"/>
+      <c r="AA26" s="24"/>
+      <c r="AB26" s="24"/>
+      <c r="AC26" s="24"/>
+      <c r="AD26" s="24"/>
+      <c r="AE26" s="24"/>
+      <c r="AF26" s="24"/>
+      <c r="AG26" s="24"/>
+      <c r="AH26" s="24"/>
+      <c r="AJ26" s="22"/>
+      <c r="AK26" s="22"/>
+      <c r="AL26" s="22"/>
+      <c r="AM26" s="22"/>
+      <c r="AN26" s="22"/>
+      <c r="AO26" s="24"/>
+      <c r="AP26" s="22"/>
+      <c r="AR26" s="22"/>
+      <c r="AS26" s="22"/>
+      <c r="AT26" s="24"/>
+      <c r="AU26" s="22"/>
+      <c r="AV26" s="22"/>
+      <c r="AW26" s="22"/>
+      <c r="AX26" s="22"/>
+      <c r="AY26" s="22"/>
+      <c r="AZ26" s="22"/>
+      <c r="BA26" s="22"/>
+      <c r="BB26" s="24"/>
+      <c r="BC26" s="24"/>
+      <c r="BD26" s="24"/>
+      <c r="BE26" s="22"/>
+      <c r="BF26" s="22"/>
+      <c r="BG26" s="22"/>
+      <c r="BH26" s="22"/>
+      <c r="BI26" s="22"/>
+      <c r="BJ26" s="22"/>
+      <c r="BK26" s="22"/>
+      <c r="BL26" s="22"/>
+      <c r="BM26" s="22"/>
+      <c r="BN26" s="22"/>
+      <c r="BO26" s="22"/>
+      <c r="BP26" s="24"/>
+      <c r="BQ26" s="24"/>
+    </row>
+    <row r="27" spans="1:102" s="25" customFormat="1">
+      <c r="A27" s="22"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="24"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="24"/>
+      <c r="V27" s="24"/>
+      <c r="W27" s="24"/>
+      <c r="X27" s="24"/>
+      <c r="Y27" s="24"/>
+      <c r="Z27" s="24"/>
+      <c r="AA27" s="24"/>
+      <c r="AB27" s="24"/>
+      <c r="AC27" s="24"/>
+      <c r="AD27" s="24"/>
+      <c r="AE27" s="24"/>
+      <c r="AF27" s="24"/>
+      <c r="AG27" s="24"/>
+      <c r="AH27" s="24"/>
+      <c r="AJ27" s="22"/>
+      <c r="AK27" s="22"/>
+      <c r="AL27" s="22"/>
+      <c r="AM27" s="22"/>
+      <c r="AN27" s="22"/>
+      <c r="AO27" s="24"/>
+      <c r="AP27" s="22"/>
+      <c r="AR27" s="22"/>
+      <c r="AS27" s="22"/>
+      <c r="AT27" s="24"/>
+      <c r="AU27" s="22"/>
+      <c r="AV27" s="22"/>
+      <c r="AW27" s="22"/>
+      <c r="AX27" s="22"/>
+      <c r="AY27" s="22"/>
+      <c r="AZ27" s="22"/>
+      <c r="BA27" s="22"/>
+      <c r="BB27" s="24"/>
+      <c r="BC27" s="24"/>
+      <c r="BD27" s="24"/>
+      <c r="BE27" s="22"/>
+      <c r="BF27" s="22"/>
+      <c r="BG27" s="22"/>
+      <c r="BH27" s="22"/>
+      <c r="BI27" s="22"/>
+      <c r="BJ27" s="22"/>
+      <c r="BK27" s="22"/>
+      <c r="BL27" s="22"/>
+      <c r="BM27" s="22"/>
+      <c r="BN27" s="22"/>
+      <c r="BO27" s="22"/>
+      <c r="BP27" s="24"/>
+      <c r="BQ27" s="24"/>
+    </row>
+    <row r="28" spans="1:102" s="25" customFormat="1">
+      <c r="A28" s="22"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="24"/>
+      <c r="V28" s="24"/>
+      <c r="W28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="24"/>
+      <c r="Z28" s="24"/>
+      <c r="AA28" s="24"/>
+      <c r="AB28" s="24"/>
+      <c r="AC28" s="24"/>
+      <c r="AD28" s="24"/>
+      <c r="AE28" s="24"/>
+      <c r="AF28" s="24"/>
+      <c r="AG28" s="24"/>
+      <c r="AH28" s="24"/>
+      <c r="AJ28" s="22"/>
+      <c r="AK28" s="22"/>
+      <c r="AL28" s="22"/>
+      <c r="AM28" s="22"/>
+      <c r="AN28" s="22"/>
+      <c r="AO28" s="24"/>
+      <c r="AP28" s="22"/>
+      <c r="AR28" s="22"/>
+      <c r="AS28" s="22"/>
+      <c r="AT28" s="24"/>
+      <c r="AU28" s="22"/>
+      <c r="AV28" s="22"/>
+      <c r="AW28" s="22"/>
+      <c r="AX28" s="22"/>
+      <c r="AY28" s="22"/>
+      <c r="AZ28" s="22"/>
+      <c r="BA28" s="22"/>
+      <c r="BB28" s="24"/>
+      <c r="BC28" s="24"/>
+      <c r="BD28" s="24"/>
+      <c r="BE28" s="22"/>
+      <c r="BF28" s="22"/>
+      <c r="BG28" s="22"/>
+      <c r="BH28" s="22"/>
+      <c r="BI28" s="22"/>
+      <c r="BJ28" s="22"/>
+      <c r="BK28" s="22"/>
+      <c r="BL28" s="22"/>
+      <c r="BM28" s="22"/>
+      <c r="BN28" s="22"/>
+      <c r="BO28" s="22"/>
+      <c r="BP28" s="24"/>
+      <c r="BQ28" s="24"/>
     </row>
     <row r="29" spans="1:102" s="10" customFormat="1">
       <c r="A29" s="9"/>
@@ -5682,7 +6080,7 @@
       <c r="BP38" s="9"/>
       <c r="BQ38" s="9"/>
     </row>
-    <row r="39" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="39" spans="1:102" s="10" customFormat="1">
       <c r="A39" s="9"/>
       <c r="B39" s="17"/>
       <c r="E39" s="9"/>
@@ -5733,7 +6131,7 @@
       <c r="BP39" s="9"/>
       <c r="BQ39" s="9"/>
     </row>
-    <row r="40" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="40" spans="1:102" s="10" customFormat="1">
       <c r="A40" s="9"/>
       <c r="B40" s="17"/>
       <c r="E40" s="9"/>
@@ -5784,7 +6182,7 @@
       <c r="BP40" s="9"/>
       <c r="BQ40" s="9"/>
     </row>
-    <row r="41" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="41" spans="1:102" s="10" customFormat="1">
       <c r="A41" s="9"/>
       <c r="B41" s="17"/>
       <c r="E41" s="9"/>
@@ -17310,11 +17708,274 @@
       <c r="BP266" s="9"/>
       <c r="BQ266" s="9"/>
     </row>
+    <row r="267" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A267" s="9"/>
+      <c r="B267" s="17"/>
+      <c r="E267" s="9"/>
+      <c r="F267" s="9"/>
+      <c r="G267" s="9"/>
+      <c r="K267" s="28"/>
+      <c r="L267" s="9"/>
+      <c r="M267" s="9"/>
+      <c r="N267" s="9"/>
+      <c r="O267" s="9"/>
+      <c r="P267" s="9"/>
+      <c r="Q267" s="29"/>
+      <c r="R267" s="29"/>
+      <c r="U267" s="9"/>
+      <c r="V267" s="9"/>
+      <c r="W267" s="9"/>
+      <c r="X267" s="9"/>
+      <c r="Y267" s="9"/>
+      <c r="Z267" s="9"/>
+      <c r="AA267" s="9"/>
+      <c r="AB267" s="9"/>
+      <c r="AC267" s="9"/>
+      <c r="AD267" s="9"/>
+      <c r="AE267" s="9"/>
+      <c r="AF267" s="9"/>
+      <c r="AG267" s="9"/>
+      <c r="AH267" s="9"/>
+      <c r="AJ267" s="9"/>
+      <c r="AK267" s="9"/>
+      <c r="AL267" s="9"/>
+      <c r="AM267" s="9"/>
+      <c r="AN267" s="9"/>
+      <c r="AO267" s="9"/>
+      <c r="AP267" s="9"/>
+      <c r="AR267" s="9"/>
+      <c r="AT267" s="9"/>
+      <c r="AU267" s="9"/>
+      <c r="AV267" s="9"/>
+      <c r="AW267" s="9"/>
+      <c r="AX267" s="9"/>
+      <c r="BH267" s="9"/>
+      <c r="BJ267" s="9"/>
+      <c r="BK267" s="9"/>
+      <c r="BL267" s="9"/>
+      <c r="BM267" s="9"/>
+      <c r="BN267" s="9"/>
+      <c r="BO267" s="9"/>
+      <c r="BP267" s="9"/>
+      <c r="BQ267" s="9"/>
+    </row>
+    <row r="268" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A268" s="9"/>
+      <c r="B268" s="17"/>
+      <c r="E268" s="9"/>
+      <c r="F268" s="9"/>
+      <c r="G268" s="9"/>
+      <c r="K268" s="28"/>
+      <c r="L268" s="9"/>
+      <c r="M268" s="9"/>
+      <c r="N268" s="9"/>
+      <c r="O268" s="9"/>
+      <c r="P268" s="9"/>
+      <c r="Q268" s="29"/>
+      <c r="R268" s="29"/>
+      <c r="U268" s="9"/>
+      <c r="V268" s="9"/>
+      <c r="W268" s="9"/>
+      <c r="X268" s="9"/>
+      <c r="Y268" s="9"/>
+      <c r="Z268" s="9"/>
+      <c r="AA268" s="9"/>
+      <c r="AB268" s="9"/>
+      <c r="AC268" s="9"/>
+      <c r="AD268" s="9"/>
+      <c r="AE268" s="9"/>
+      <c r="AF268" s="9"/>
+      <c r="AG268" s="9"/>
+      <c r="AH268" s="9"/>
+      <c r="AJ268" s="9"/>
+      <c r="AK268" s="9"/>
+      <c r="AL268" s="9"/>
+      <c r="AM268" s="9"/>
+      <c r="AN268" s="9"/>
+      <c r="AO268" s="9"/>
+      <c r="AP268" s="9"/>
+      <c r="AR268" s="9"/>
+      <c r="AT268" s="9"/>
+      <c r="AU268" s="9"/>
+      <c r="AV268" s="9"/>
+      <c r="AW268" s="9"/>
+      <c r="AX268" s="9"/>
+      <c r="BH268" s="9"/>
+      <c r="BJ268" s="9"/>
+      <c r="BK268" s="9"/>
+      <c r="BL268" s="9"/>
+      <c r="BM268" s="9"/>
+      <c r="BN268" s="9"/>
+      <c r="BO268" s="9"/>
+      <c r="BP268" s="9"/>
+      <c r="BQ268" s="9"/>
+    </row>
+    <row r="269" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A269" s="9"/>
+      <c r="B269" s="17"/>
+      <c r="E269" s="9"/>
+      <c r="F269" s="9"/>
+      <c r="G269" s="9"/>
+      <c r="K269" s="28"/>
+      <c r="L269" s="9"/>
+      <c r="M269" s="9"/>
+      <c r="N269" s="9"/>
+      <c r="O269" s="9"/>
+      <c r="P269" s="9"/>
+      <c r="Q269" s="29"/>
+      <c r="R269" s="29"/>
+      <c r="U269" s="9"/>
+      <c r="V269" s="9"/>
+      <c r="W269" s="9"/>
+      <c r="X269" s="9"/>
+      <c r="Y269" s="9"/>
+      <c r="Z269" s="9"/>
+      <c r="AA269" s="9"/>
+      <c r="AB269" s="9"/>
+      <c r="AC269" s="9"/>
+      <c r="AD269" s="9"/>
+      <c r="AE269" s="9"/>
+      <c r="AF269" s="9"/>
+      <c r="AG269" s="9"/>
+      <c r="AH269" s="9"/>
+      <c r="AJ269" s="9"/>
+      <c r="AK269" s="9"/>
+      <c r="AL269" s="9"/>
+      <c r="AM269" s="9"/>
+      <c r="AN269" s="9"/>
+      <c r="AO269" s="9"/>
+      <c r="AP269" s="9"/>
+      <c r="AR269" s="9"/>
+      <c r="AT269" s="9"/>
+      <c r="AU269" s="9"/>
+      <c r="AV269" s="9"/>
+      <c r="AW269" s="9"/>
+      <c r="AX269" s="9"/>
+      <c r="BH269" s="9"/>
+      <c r="BJ269" s="9"/>
+      <c r="BK269" s="9"/>
+      <c r="BL269" s="9"/>
+      <c r="BM269" s="9"/>
+      <c r="BN269" s="9"/>
+      <c r="BO269" s="9"/>
+      <c r="BP269" s="9"/>
+      <c r="BQ269" s="9"/>
+    </row>
+    <row r="270" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A270" s="9"/>
+      <c r="B270" s="17"/>
+      <c r="E270" s="9"/>
+      <c r="F270" s="9"/>
+      <c r="G270" s="9"/>
+      <c r="K270" s="28"/>
+      <c r="L270" s="9"/>
+      <c r="M270" s="9"/>
+      <c r="N270" s="9"/>
+      <c r="O270" s="9"/>
+      <c r="P270" s="9"/>
+      <c r="Q270" s="29"/>
+      <c r="R270" s="29"/>
+      <c r="U270" s="9"/>
+      <c r="V270" s="9"/>
+      <c r="W270" s="9"/>
+      <c r="X270" s="9"/>
+      <c r="Y270" s="9"/>
+      <c r="Z270" s="9"/>
+      <c r="AA270" s="9"/>
+      <c r="AB270" s="9"/>
+      <c r="AC270" s="9"/>
+      <c r="AD270" s="9"/>
+      <c r="AE270" s="9"/>
+      <c r="AF270" s="9"/>
+      <c r="AG270" s="9"/>
+      <c r="AH270" s="9"/>
+      <c r="AJ270" s="9"/>
+      <c r="AK270" s="9"/>
+      <c r="AL270" s="9"/>
+      <c r="AM270" s="9"/>
+      <c r="AN270" s="9"/>
+      <c r="AO270" s="9"/>
+      <c r="AP270" s="9"/>
+      <c r="AR270" s="9"/>
+      <c r="AT270" s="9"/>
+      <c r="AU270" s="9"/>
+      <c r="AV270" s="9"/>
+      <c r="AW270" s="9"/>
+      <c r="AX270" s="9"/>
+      <c r="BH270" s="9"/>
+      <c r="BJ270" s="9"/>
+      <c r="BK270" s="9"/>
+      <c r="BL270" s="9"/>
+      <c r="BM270" s="9"/>
+      <c r="BN270" s="9"/>
+      <c r="BO270" s="9"/>
+      <c r="BP270" s="9"/>
+      <c r="BQ270" s="9"/>
+    </row>
+    <row r="271" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A271" s="9"/>
+      <c r="B271" s="17"/>
+      <c r="E271" s="9"/>
+      <c r="F271" s="9"/>
+      <c r="G271" s="9"/>
+      <c r="K271" s="28"/>
+      <c r="L271" s="9"/>
+      <c r="M271" s="9"/>
+      <c r="N271" s="9"/>
+      <c r="O271" s="9"/>
+      <c r="P271" s="9"/>
+      <c r="Q271" s="29"/>
+      <c r="R271" s="29"/>
+      <c r="U271" s="9"/>
+      <c r="V271" s="9"/>
+      <c r="W271" s="9"/>
+      <c r="X271" s="9"/>
+      <c r="Y271" s="9"/>
+      <c r="Z271" s="9"/>
+      <c r="AA271" s="9"/>
+      <c r="AB271" s="9"/>
+      <c r="AC271" s="9"/>
+      <c r="AD271" s="9"/>
+      <c r="AE271" s="9"/>
+      <c r="AF271" s="9"/>
+      <c r="AG271" s="9"/>
+      <c r="AH271" s="9"/>
+      <c r="AJ271" s="9"/>
+      <c r="AK271" s="9"/>
+      <c r="AL271" s="9"/>
+      <c r="AM271" s="9"/>
+      <c r="AN271" s="9"/>
+      <c r="AO271" s="9"/>
+      <c r="AP271" s="9"/>
+      <c r="AR271" s="9"/>
+      <c r="AT271" s="9"/>
+      <c r="AU271" s="9"/>
+      <c r="AV271" s="9"/>
+      <c r="AW271" s="9"/>
+      <c r="AX271" s="9"/>
+      <c r="BH271" s="9"/>
+      <c r="BJ271" s="9"/>
+      <c r="BK271" s="9"/>
+      <c r="BL271" s="9"/>
+      <c r="BM271" s="9"/>
+      <c r="BN271" s="9"/>
+      <c r="BO271" s="9"/>
+      <c r="BP271" s="9"/>
+      <c r="BQ271" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="X19" r:id="rId1" display="BOILERSOIL@GMAIL.COM :: Oil Burner Installer :: CONTROLLED PLBG CO., INC"/>
+    <hyperlink ref="X23" r:id="rId2" display="BOILERSOIL@GMAIL.COM :: Oil Burner Installer :: CONTROLLED PLBG CO., INC"/>
+    <hyperlink ref="E23" r:id="rId3"/>
+    <hyperlink ref="D23" r:id="rId4" display="AJOETEST@GMAIL.COM :: Professional Engineer :: JA&amp; LLC"/>
+    <hyperlink ref="T23" r:id="rId5"/>
+    <hyperlink ref="AA23" r:id="rId6"/>
+    <hyperlink ref="AB23" r:id="rId7"/>
+    <hyperlink ref="T7" r:id="rId8"/>
+    <hyperlink ref="T19" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
latest data files as of 2019-01-17
latest data files as of 2019-01-17 - 3 files: bemsst, fab4 and base
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases BEMSST.xlsx
+++ b/src/com/data/Test Cases BEMSST.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="33330" yWindow="2715" windowWidth="21645" windowHeight="7155" tabRatio="152" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1185" windowWidth="22095" windowHeight="10605" tabRatio="152" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A13:J23"/>
+  <oleSize ref="A5:J23"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="157">
   <si>
     <t>TCID</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>tr8</t>
-  </si>
-  <si>
-    <t>APPLEROME18@GMAIL.COM</t>
   </si>
   <si>
     <t>BUILD002</t>
@@ -366,19 +363,10 @@
     <t>user_info</t>
   </si>
   <si>
-    <t>1 :: DOBTESTING123@GMAIL.COM :: Professional Engineer :: 005551 :: Fuel-Oil Storage and Fuel-Oil Piping Systems</t>
-  </si>
-  <si>
     <t>1111 :: 700 :: Other :: 1111</t>
   </si>
   <si>
     <t>Standard Plan Examination or Review</t>
-  </si>
-  <si>
-    <t>StNew</t>
-  </si>
-  <si>
-    <t>Structural</t>
   </si>
   <si>
     <t>1 :: false :: false :: 1 :: 1 :: 1 :: false :: false :: false :: false</t>
@@ -390,9 +378,6 @@
     <t>Structural :: 1111 :: 1.00 :: 3333</t>
   </si>
   <si>
-    <t>Mechanical Work Mechanical Systems</t>
-  </si>
-  <si>
     <t>Mechanical Systems :: 1111 :: 1.00 :: 3333</t>
   </si>
   <si>
@@ -402,13 +387,7 @@
     <t>1 :: Electrical Motors :: AJOETEST@GMAIL.COM :: Professional Engineer</t>
   </si>
   <si>
-    <t>BeNew</t>
-  </si>
-  <si>
     <t>Boiler Equipment :: 1111 :: 1.00 :: 3333</t>
-  </si>
-  <si>
-    <t>q :: Electrical Motors :: DOBTESTING123@GMAIL.COM :: Professional Engineer</t>
   </si>
   <si>
     <t>NYCECC :: Tabular Analysis :: N</t>
@@ -417,22 +396,7 @@
     <t>NYCECC :: Tabular Analysis :: Y</t>
   </si>
   <si>
-    <t>MsNew</t>
-  </si>
-  <si>
     <t>1 :: N :: Y :: N :: N :: N :: N :: N :: N :: N :: N</t>
-  </si>
-  <si>
-    <t>Mechanical Work Boiler Equipment New</t>
-  </si>
-  <si>
-    <t>111 :: FIRST AVENUE :: MANHATTAN :: 448 :: 28 :: MS1</t>
-  </si>
-  <si>
-    <t>111 :: FIRST AVENUE :: MANHATTAN :: 448 :: 28 :: ST1</t>
-  </si>
-  <si>
-    <t>280 :: BROADWAY :: MANHATTAN :: 153 :: 1 :: BE1</t>
   </si>
   <si>
     <t>1 :: 2 :: N :: N :: N :: N :: N :: N :: N :: N :: N :: N</t>
@@ -441,25 +405,13 @@
     <t>Professional Certification</t>
   </si>
   <si>
-    <t>1 :: 1 :: N :: N :: N :: N :: N :: N :: N :: N :: N :: N</t>
-  </si>
-  <si>
-    <t>Boiler Equipment - Standard</t>
-  </si>
-  <si>
     <t>Mechanical Systems - Standard</t>
   </si>
   <si>
     <t>Structural - Standard</t>
   </si>
   <si>
-    <t>Boiler Equipment - Prof Cert - PW2</t>
-  </si>
-  <si>
     <t>BOILERPLUMBER@GMAIL.COM :: Master Plumber :: THE PLUMBING COMPANY INC :: APPLEROME16@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>Boiler Equipment - New - Standard</t>
   </si>
   <si>
     <t>AJOETEST@GMAIL.COM :: Mechanical Work :: 2 :: 1 :: 1</t>
@@ -480,28 +432,61 @@
     <t>AJOETEST@GMAIL.COM :: Professional Engineer :: JA&amp; LLC :: APPLEROME16@GMAIL.COM</t>
   </si>
   <si>
-    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2 :: APPLEROME16@GMAIL.COM</t>
-  </si>
-  <si>
     <t>boiler :: AJOETEST@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>boiler :: APPLEROME18@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>Y :: APPLEROME18@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: JA&amp; LLC</t>
-  </si>
-  <si>
-    <t>a :: DOBTESTING123@GMAIL.COM :: Professional Engineer :: 005546 :: Fuel-Oil Storage and Fuel-Oil Piping Systems</t>
   </si>
   <si>
     <t>BeNewStd</t>
   </si>
   <si>
     <t>BeNewProPw2</t>
+  </si>
+  <si>
+    <t>BeNewPro</t>
+  </si>
+  <si>
+    <t>AJOETEST@GMAIL.COM :: Mechanical Work :: 2 :: 1 :: 2</t>
+  </si>
+  <si>
+    <t>Boiler Equipment - New Install - Prof Cert - No PW2</t>
+  </si>
+  <si>
+    <t>Boiler Equipment - New Install - Prof Cert - PW2</t>
+  </si>
+  <si>
+    <t>Boiler Equipment - New Install - Standard</t>
+  </si>
+  <si>
+    <t>MsNewStd</t>
+  </si>
+  <si>
+    <t>StNewStd</t>
+  </si>
+  <si>
+    <t>AJOETEST@GMAIL.COM :: Structural :: 0 :: 0 :: 1</t>
+  </si>
+  <si>
+    <t>280 :: BROADWAY :: MANHATTAN :: 153 :: 1 :: BES</t>
+  </si>
+  <si>
+    <t>280 :: BROADWAY :: MANHATTAN :: 153 :: 1 :: BEP</t>
+  </si>
+  <si>
+    <t>111 :: FIRST AVENUE :: MANHATTAN :: 448 :: 28 :: STS</t>
+  </si>
+  <si>
+    <t>111 :: FIRST AVENUE :: MANHATTAN :: 448 :: 28 :: MSS</t>
+  </si>
+  <si>
+    <t>Y :: AJOETEST@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>AJOETEST@GMAIL.COM :: Mechanical Work :: 1 :: 0 :: 1</t>
+  </si>
+  <si>
+    <t>1 :: AJOETEST@GMAIL.COM :: Professional Engineer :: 005551 :: Fuel-Oil Storage and Fuel-Oil Piping Systems</t>
+  </si>
+  <si>
+    <t>BOILERSTEST1@GMAIL.COM :: Master Plumber :: SAMUEL &amp; SONS P &amp; H INC :: APPLEROME16@GMAIL.COM :: AJOETEST@GMAIL.COM</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1178,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1306,10 +1291,16 @@
     <xf numFmtId="49" fontId="26" fillId="0" borderId="1" xfId="128" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="1" xfId="128" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="128" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="128" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="1" xfId="128" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1768,7 +1759,7 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1">
       <c r="A2" s="34" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="32" t="s">
@@ -1777,7 +1768,7 @@
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1">
       <c r="A3" s="34" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="32" t="s">
@@ -1786,7 +1777,7 @@
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1">
       <c r="A4" s="34" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="B4" s="30"/>
       <c r="C4" s="32" t="s">
@@ -1795,7 +1786,7 @@
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">
       <c r="A5" s="34" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="32" t="s">
@@ -1804,7 +1795,7 @@
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1">
       <c r="A6" s="34" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="32" t="s">
@@ -2176,9 +2167,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="T1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -2186,8 +2177,8 @@
     <col min="1" max="1" width="25.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.140625" style="17" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="19" style="9" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" style="9" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" style="9" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" style="10" customWidth="1"/>
@@ -2206,11 +2197,11 @@
     <col min="21" max="21" width="18" style="9" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="45.7109375" style="9" customWidth="1"/>
     <col min="23" max="23" width="43.28515625" style="9" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" style="9" customWidth="1"/>
+    <col min="24" max="24" width="49" style="9" customWidth="1"/>
     <col min="25" max="25" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="9" customWidth="1"/>
     <col min="27" max="27" width="21.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" style="9" customWidth="1"/>
+    <col min="28" max="28" width="11.85546875" style="9" customWidth="1"/>
     <col min="29" max="29" width="8.28515625" style="9" customWidth="1"/>
     <col min="30" max="30" width="15.28515625" style="9" customWidth="1"/>
     <col min="31" max="31" width="10.28515625" style="9" customWidth="1"/>
@@ -2542,7 +2533,7 @@
     </row>
     <row r="5" spans="1:102" s="7" customFormat="1">
       <c r="A5" s="34" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="B5" s="6"/>
       <c r="E5" s="6"/>
@@ -2604,25 +2595,25 @@
         <v>15</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>14</v>
@@ -2631,13 +2622,13 @@
         <v>7</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>11</v>
@@ -2646,7 +2637,7 @@
         <v>10</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S6" s="12" t="s">
         <v>6</v>
@@ -2670,7 +2661,7 @@
         <v>18</v>
       </c>
       <c r="Z6" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA6" s="5" t="s">
         <v>22</v>
@@ -2682,7 +2673,7 @@
         <v>24</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AE6" s="15" t="s">
         <v>17</v>
@@ -2693,229 +2684,229 @@
       <c r="AG6" s="5"/>
       <c r="AH6" s="5"/>
       <c r="AI6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ6" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN6" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP6" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ6" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR6" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS6" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU6" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV6" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW6" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AZ6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="BA6" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC6" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="BD6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE6" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG6" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="BH6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="BJ6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK6" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="BL6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="BM6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="BN6" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="AJ6" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL6" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN6" s="13" t="s">
+      <c r="BO6" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BP6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BQ6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AO6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP6" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ6" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR6" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AS6" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT6" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU6" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="AV6" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="AW6" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="AX6" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="AY6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AZ6" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="BA6" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="BB6" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="BC6" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="BD6" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE6" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF6" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="BG6" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="BH6" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="BI6" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="BJ6" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="BK6" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="BL6" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="BM6" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="BN6" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="BO6" s="14" t="s">
+      <c r="BR6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="BS6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BT6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="BU6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="BV6" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BW6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BX6" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BY6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BZ6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CA6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="CB6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="CC6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CD6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="CE6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="CF6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CG6" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="CH6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="CI6" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="CJ6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CL6" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="CM6" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CO6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="BP6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="BQ6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="BR6" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="BS6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="BT6" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="BU6" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="BV6" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="BW6" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="BX6" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="BY6" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BZ6" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="CA6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="CB6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="CC6" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="CD6" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="CE6" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="CF6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="CG6" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="CH6" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="CI6" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="CJ6" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="CK6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="CL6" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="CM6" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="CN6" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="CO6" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:102" s="4" customFormat="1" ht="63.75">
+    </row>
+    <row r="7" spans="1:102" s="4" customFormat="1" ht="45">
       <c r="A7" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>135</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="L7" s="11" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N7" s="11" t="s">
         <v>3</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q7" s="11" t="s">
         <v>3</v>
@@ -2925,49 +2916,49 @@
         <v>3</v>
       </c>
       <c r="T7" s="39" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="W7" s="11" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
       <c r="Z7" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="AA7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB7" s="11" t="s">
-        <v>3</v>
+        <v>138</v>
+      </c>
+      <c r="AA7" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB7" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="AC7" s="11" t="s">
         <v>3</v>
       </c>
       <c r="AD7" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE7" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG7" s="11"/>
       <c r="AH7" s="11"/>
       <c r="AJ7" s="3"/>
       <c r="AK7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AL7" s="3"/>
       <c r="AM7" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN7" s="3"/>
       <c r="AO7" s="11"/>
@@ -2978,44 +2969,44 @@
       </c>
       <c r="AT7" s="11"/>
       <c r="AU7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV7" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="AV7" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="AW7" s="3"/>
       <c r="AX7" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AY7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ7" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="AZ7" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="BA7" s="18" t="s">
         <v>13</v>
       </c>
       <c r="BB7" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BC7" s="11" t="s">
         <v>20</v>
       </c>
       <c r="BD7" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BE7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="BF7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH7" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BI7" s="3" t="s">
         <v>3</v>
@@ -3024,13 +3015,13 @@
         <v>3</v>
       </c>
       <c r="BK7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BL7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BM7" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BN7" s="3" t="s">
         <v>3</v>
@@ -3096,7 +3087,7 @@
     </row>
     <row r="9" spans="1:102" s="7" customFormat="1">
       <c r="A9" s="34" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="B9" s="6"/>
       <c r="E9" s="6"/>
@@ -3158,25 +3149,25 @@
         <v>15</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>14</v>
@@ -3185,13 +3176,13 @@
         <v>7</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>11</v>
@@ -3200,7 +3191,7 @@
         <v>10</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S10" s="12" t="s">
         <v>6</v>
@@ -3224,7 +3215,7 @@
         <v>18</v>
       </c>
       <c r="Z10" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA10" s="5" t="s">
         <v>22</v>
@@ -3236,7 +3227,7 @@
         <v>24</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AE10" s="15" t="s">
         <v>17</v>
@@ -3247,229 +3238,229 @@
       <c r="AG10" s="5"/>
       <c r="AH10" s="5"/>
       <c r="AI10" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL10" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN10" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP10" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR10" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS10" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU10" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV10" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW10" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AZ10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="BA10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC10" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="BD10" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG10" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="BH10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI10" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="BJ10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK10" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="BL10" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="BM10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="BN10" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="AJ10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK10" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL10" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM10" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN10" s="13" t="s">
+      <c r="BO10" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BP10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BQ10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AO10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP10" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ10" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR10" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AS10" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT10" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU10" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="AV10" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="AW10" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="AX10" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="AY10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AZ10" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="BA10" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="BB10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="BC10" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="BD10" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE10" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF10" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="BG10" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="BH10" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="BI10" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="BJ10" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="BK10" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="BL10" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="BM10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="BN10" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="BO10" s="14" t="s">
+      <c r="BR10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="BS10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BT10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="BU10" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="BV10" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BW10" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BX10" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BY10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BZ10" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CA10" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="CB10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="CC10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CD10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="CE10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="CF10" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CG10" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="CH10" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="CI10" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="CJ10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CL10" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="CM10" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CO10" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="BP10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="BQ10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="BR10" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="BS10" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="BT10" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="BU10" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="BV10" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="BW10" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="BX10" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="BY10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BZ10" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="CA10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="CB10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="CC10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="CD10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="CE10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="CF10" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="CG10" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="CH10" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="CI10" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="CJ10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="CK10" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="CL10" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="CM10" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="CN10" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="CO10" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:102" s="4" customFormat="1" ht="63.75">
+    </row>
+    <row r="11" spans="1:102" s="4" customFormat="1" ht="45">
       <c r="A11" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C11" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="L11" s="11" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N11" s="11" t="s">
         <v>3</v>
       </c>
       <c r="O11" s="11"/>
       <c r="P11" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q11" s="11" t="s">
         <v>3</v>
@@ -3479,49 +3470,49 @@
         <v>3</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="V11" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="W11" s="11" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="X11" s="11"/>
       <c r="Y11" s="11"/>
       <c r="Z11" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB11" s="11" t="s">
-        <v>3</v>
+        <v>153</v>
+      </c>
+      <c r="AA11" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB11" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="AC11" s="11" t="s">
         <v>3</v>
       </c>
       <c r="AD11" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE11" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AF11" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG11" s="11"/>
       <c r="AH11" s="11"/>
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AL11" s="3"/>
       <c r="AM11" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN11" s="3"/>
       <c r="AO11" s="11"/>
@@ -3532,44 +3523,44 @@
       </c>
       <c r="AT11" s="11"/>
       <c r="AU11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV11" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="AV11" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="AW11" s="3"/>
       <c r="AX11" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AY11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ11" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="AZ11" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="BA11" s="18" t="s">
         <v>13</v>
       </c>
       <c r="BB11" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BC11" s="11" t="s">
         <v>20</v>
       </c>
       <c r="BD11" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BE11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="BF11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH11" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BI11" s="3" t="s">
         <v>3</v>
@@ -3578,13 +3569,13 @@
         <v>3</v>
       </c>
       <c r="BK11" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BL11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BM11" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BN11" s="3" t="s">
         <v>3</v>
@@ -3650,7 +3641,7 @@
     </row>
     <row r="13" spans="1:102" s="7" customFormat="1">
       <c r="A13" s="34" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="B13" s="6"/>
       <c r="E13" s="6"/>
@@ -3712,25 +3703,25 @@
         <v>15</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>14</v>
@@ -3739,13 +3730,13 @@
         <v>7</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N14" s="5" t="s">
         <v>9</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P14" s="5" t="s">
         <v>11</v>
@@ -3754,7 +3745,7 @@
         <v>10</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S14" s="12" t="s">
         <v>6</v>
@@ -3778,7 +3769,7 @@
         <v>18</v>
       </c>
       <c r="Z14" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA14" s="5" t="s">
         <v>22</v>
@@ -3790,7 +3781,7 @@
         <v>24</v>
       </c>
       <c r="AD14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AE14" s="15" t="s">
         <v>17</v>
@@ -3801,229 +3792,229 @@
       <c r="AG14" s="5"/>
       <c r="AH14" s="5"/>
       <c r="AI14" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ14" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL14" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP14" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ14" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR14" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS14" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU14" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV14" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW14" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AZ14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="BA14" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="BD14" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF14" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG14" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="BH14" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="BJ14" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK14" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="BL14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="BM14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="BN14" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="AJ14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK14" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL14" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN14" s="13" t="s">
+      <c r="BO14" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BP14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BQ14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AO14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP14" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ14" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR14" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AS14" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT14" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU14" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="AV14" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="AW14" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="AX14" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="AY14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AZ14" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="BA14" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="BB14" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="BC14" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="BD14" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE14" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF14" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="BG14" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="BH14" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="BI14" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="BJ14" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="BK14" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="BL14" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="BM14" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="BN14" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="BO14" s="14" t="s">
+      <c r="BR14" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="BS14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BT14" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="BU14" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="BV14" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BW14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BX14" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BY14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BZ14" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CA14" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="CB14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="CC14" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CD14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="CE14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="CF14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CG14" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="CH14" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="CI14" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="CJ14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK14" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CL14" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="CM14" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CO14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="BP14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="BQ14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="BR14" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="BS14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="BT14" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="BU14" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="BV14" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="BW14" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="BX14" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="BY14" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BZ14" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="CA14" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="CB14" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="CC14" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="CD14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="CE14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="CF14" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="CG14" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="CH14" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="CI14" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="CJ14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="CK14" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="CL14" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="CM14" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="CN14" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="CO14" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:102" s="4" customFormat="1" ht="63.75">
+    </row>
+    <row r="15" spans="1:102" s="4" customFormat="1" ht="45">
       <c r="A15" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C15" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="K15" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="L15" s="11" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N15" s="11" t="s">
         <v>3</v>
       </c>
       <c r="O15" s="11"/>
       <c r="P15" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q15" s="11" t="s">
         <v>3</v>
@@ -4033,47 +4024,47 @@
         <v>3</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="V15" s="4" t="s">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
       <c r="Y15" s="11"/>
       <c r="Z15" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB15" s="11" t="s">
-        <v>3</v>
+        <v>153</v>
+      </c>
+      <c r="AA15" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB15" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="AC15" s="11" t="s">
         <v>3</v>
       </c>
       <c r="AD15" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE15" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AF15" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG15" s="11"/>
       <c r="AH15" s="11"/>
       <c r="AJ15" s="3"/>
       <c r="AK15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AL15" s="3"/>
       <c r="AM15" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN15" s="3"/>
       <c r="AO15" s="11"/>
@@ -4084,44 +4075,44 @@
       </c>
       <c r="AT15" s="11"/>
       <c r="AU15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV15" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="AV15" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="AW15" s="3"/>
       <c r="AX15" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AY15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ15" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="AZ15" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="BA15" s="18" t="s">
         <v>13</v>
       </c>
       <c r="BB15" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BC15" s="11" t="s">
         <v>20</v>
       </c>
       <c r="BD15" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BE15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="BF15" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG15" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH15" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BI15" s="3" t="s">
         <v>3</v>
@@ -4130,13 +4121,13 @@
         <v>3</v>
       </c>
       <c r="BK15" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BL15" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BM15" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BN15" s="3" t="s">
         <v>3</v>
@@ -4202,7 +4193,7 @@
     </row>
     <row r="17" spans="1:102" s="7" customFormat="1">
       <c r="A17" s="34" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="B17" s="6"/>
       <c r="E17" s="6"/>
@@ -4264,25 +4255,25 @@
         <v>15</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>14</v>
@@ -4291,13 +4282,13 @@
         <v>7</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N18" s="5" t="s">
         <v>9</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P18" s="5" t="s">
         <v>11</v>
@@ -4306,7 +4297,7 @@
         <v>10</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S18" s="12" t="s">
         <v>6</v>
@@ -4330,7 +4321,7 @@
         <v>18</v>
       </c>
       <c r="Z18" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA18" s="5" t="s">
         <v>22</v>
@@ -4342,7 +4333,7 @@
         <v>24</v>
       </c>
       <c r="AD18" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AE18" s="15" t="s">
         <v>17</v>
@@ -4353,229 +4344,229 @@
       <c r="AG18" s="5"/>
       <c r="AH18" s="5"/>
       <c r="AI18" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ18" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK18" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL18" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM18" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN18" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP18" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ18" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR18" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS18" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU18" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV18" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW18" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX18" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AZ18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="BA18" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB18" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC18" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="BD18" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG18" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="BH18" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="BJ18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK18" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="BL18" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="BM18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="BN18" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="AJ18" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK18" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL18" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM18" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN18" s="13" t="s">
+      <c r="BO18" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BP18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BQ18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AO18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP18" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ18" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR18" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AS18" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT18" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU18" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="AV18" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="AW18" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="AX18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="AY18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AZ18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="BA18" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="BB18" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="BC18" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="BD18" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE18" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF18" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="BG18" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="BH18" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="BI18" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="BJ18" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="BK18" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="BL18" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="BM18" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="BN18" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="BO18" s="14" t="s">
+      <c r="BR18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="BS18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BT18" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="BU18" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="BV18" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BW18" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BX18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BY18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BZ18" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CA18" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="CB18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="CC18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CD18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="CE18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="CF18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CG18" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="CH18" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="CI18" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="CJ18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK18" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CL18" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="CM18" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CO18" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="BP18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="BQ18" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="BR18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="BS18" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="BT18" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="BU18" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="BV18" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="BW18" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="BX18" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="BY18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BZ18" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="CA18" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="CB18" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="CC18" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="CD18" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="CE18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="CF18" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="CG18" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="CH18" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="CI18" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="CJ18" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="CK18" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="CL18" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="CM18" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="CN18" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="CO18" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:102" s="4" customFormat="1" ht="105">
+    </row>
+    <row r="19" spans="1:102" s="4" customFormat="1" ht="60">
       <c r="A19" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>142</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J19" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K19" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="K19" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="L19" s="11" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N19" s="11" t="s">
         <v>3</v>
       </c>
       <c r="O19" s="11"/>
       <c r="P19" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q19" s="11" t="s">
         <v>3</v>
@@ -4585,51 +4576,51 @@
         <v>3</v>
       </c>
       <c r="T19" s="39" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="U19" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="V19" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="W19" s="11" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="X19" s="39" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="Y19" s="11"/>
       <c r="Z19" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="AA19" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB19" s="11" t="s">
-        <v>3</v>
+        <v>138</v>
+      </c>
+      <c r="AA19" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB19" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="AC19" s="11" t="s">
         <v>3</v>
       </c>
       <c r="AD19" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE19" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AF19" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG19" s="11"/>
       <c r="AH19" s="11"/>
       <c r="AJ19" s="3"/>
       <c r="AK19" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AL19" s="3"/>
       <c r="AM19" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN19" s="3"/>
       <c r="AO19" s="11"/>
@@ -4640,44 +4631,44 @@
       </c>
       <c r="AT19" s="11"/>
       <c r="AU19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV19" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="AV19" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="AW19" s="3"/>
       <c r="AX19" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AY19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ19" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="AZ19" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="BA19" s="18" t="s">
         <v>13</v>
       </c>
       <c r="BB19" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BC19" s="11" t="s">
         <v>20</v>
       </c>
       <c r="BD19" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BE19" s="4" t="s">
         <v>3</v>
       </c>
       <c r="BF19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH19" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BI19" s="3" t="s">
         <v>3</v>
@@ -4686,13 +4677,13 @@
         <v>3</v>
       </c>
       <c r="BK19" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BL19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BM19" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BN19" s="3" t="s">
         <v>3</v>
@@ -4758,7 +4749,7 @@
     </row>
     <row r="21" spans="1:102" s="7" customFormat="1">
       <c r="A21" s="34" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="B21" s="6"/>
       <c r="E21" s="6"/>
@@ -4820,25 +4811,25 @@
         <v>15</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>14</v>
@@ -4847,13 +4838,13 @@
         <v>7</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>11</v>
@@ -4862,7 +4853,7 @@
         <v>10</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S22" s="12" t="s">
         <v>6</v>
@@ -4886,7 +4877,7 @@
         <v>18</v>
       </c>
       <c r="Z22" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA22" s="5" t="s">
         <v>22</v>
@@ -4898,7 +4889,7 @@
         <v>24</v>
       </c>
       <c r="AD22" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AE22" s="15" t="s">
         <v>17</v>
@@ -4909,229 +4900,229 @@
       <c r="AG22" s="5"/>
       <c r="AH22" s="5"/>
       <c r="AI22" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ22" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK22" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL22" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM22" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN22" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP22" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR22" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS22" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT22" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU22" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV22" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW22" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AZ22" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="BA22" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB22" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC22" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="BD22" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE22" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF22" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG22" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="BH22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI22" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="BJ22" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK22" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="BL22" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="BM22" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="BN22" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="AJ22" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK22" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL22" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM22" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN22" s="13" t="s">
+      <c r="BO22" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BP22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BQ22" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AO22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP22" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ22" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR22" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AS22" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT22" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU22" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="AV22" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="AW22" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="AX22" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="AY22" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AZ22" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="BA22" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="BB22" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="BC22" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="BD22" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE22" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF22" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="BG22" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="BH22" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="BI22" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="BJ22" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="BK22" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="BL22" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="BM22" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="BN22" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="BO22" s="14" t="s">
+      <c r="BR22" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="BS22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BT22" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="BU22" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="BV22" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BW22" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BX22" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BY22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BZ22" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CA22" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="CB22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="CC22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CD22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="CE22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="CF22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CG22" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="CH22" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="CI22" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="CJ22" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CL22" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="CM22" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN22" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CO22" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="BP22" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="BQ22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="BR22" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="BS22" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="BT22" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="BU22" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="BV22" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="BW22" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="BX22" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="BY22" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BZ22" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="CA22" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="CB22" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="CC22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="CD22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="CE22" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="CF22" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="CG22" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="CH22" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="CI22" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="CJ22" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="CK22" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="CL22" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="CM22" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="CN22" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="CO22" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:102" s="4" customFormat="1" ht="105">
+    </row>
+    <row r="23" spans="1:102" s="4" customFormat="1" ht="45">
       <c r="A23" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>148</v>
+        <v>116</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>132</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J23" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K23" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="K23" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="L23" s="11" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N23" s="11" t="s">
         <v>3</v>
       </c>
       <c r="O23" s="11"/>
       <c r="P23" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q23" s="11" t="s">
         <v>3</v>
@@ -5141,51 +5132,51 @@
         <v>3</v>
       </c>
       <c r="T23" s="39" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="U23" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="V23" s="4" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="W23" s="11" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="X23" s="39" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="Y23" s="11"/>
       <c r="Z23" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA23" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="AB23" s="41" t="s">
-        <v>152</v>
+        <v>138</v>
+      </c>
+      <c r="AA23" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB23" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="AC23" s="11" t="s">
         <v>3</v>
       </c>
       <c r="AD23" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE23" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AF23" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG23" s="11"/>
       <c r="AH23" s="11"/>
       <c r="AJ23" s="3"/>
       <c r="AK23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AL23" s="3"/>
       <c r="AM23" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN23" s="3"/>
       <c r="AO23" s="11"/>
@@ -5196,44 +5187,44 @@
       </c>
       <c r="AT23" s="11"/>
       <c r="AU23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV23" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="AV23" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="AW23" s="3"/>
       <c r="AX23" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AY23" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ23" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="AZ23" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="BA23" s="18" t="s">
         <v>13</v>
       </c>
       <c r="BB23" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BC23" s="11" t="s">
         <v>20</v>
       </c>
       <c r="BD23" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BE23" s="4" t="s">
         <v>3</v>
       </c>
       <c r="BF23" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG23" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH23" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BI23" s="3" t="s">
         <v>3</v>
@@ -5242,13 +5233,13 @@
         <v>3</v>
       </c>
       <c r="BK23" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BL23" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BM23" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BN23" s="3" t="s">
         <v>3</v>
@@ -5363,7 +5354,7 @@
       <c r="BP25" s="9"/>
       <c r="BQ25" s="9"/>
     </row>
-    <row r="26" spans="1:102" s="25" customFormat="1">
+    <row r="26" spans="1:102" s="25" customFormat="1" ht="409.6">
       <c r="A26" s="22"/>
       <c r="B26" s="23"/>
       <c r="C26" s="22"/>
@@ -5432,7 +5423,7 @@
       <c r="BP26" s="24"/>
       <c r="BQ26" s="24"/>
     </row>
-    <row r="27" spans="1:102" s="25" customFormat="1">
+    <row r="27" spans="1:102" s="25" customFormat="1" ht="409.6">
       <c r="A27" s="22"/>
       <c r="B27" s="23"/>
       <c r="C27" s="22"/>
@@ -5501,7 +5492,7 @@
       <c r="BP27" s="24"/>
       <c r="BQ27" s="24"/>
     </row>
-    <row r="28" spans="1:102" s="25" customFormat="1">
+    <row r="28" spans="1:102" s="25" customFormat="1" ht="409.6">
       <c r="A28" s="22"/>
       <c r="B28" s="23"/>
       <c r="C28" s="22"/>
@@ -5570,7 +5561,7 @@
       <c r="BP28" s="24"/>
       <c r="BQ28" s="24"/>
     </row>
-    <row r="29" spans="1:102" s="10" customFormat="1">
+    <row r="29" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A29" s="9"/>
       <c r="B29" s="17"/>
       <c r="E29" s="9"/>
@@ -5621,7 +5612,7 @@
       <c r="BP29" s="9"/>
       <c r="BQ29" s="9"/>
     </row>
-    <row r="30" spans="1:102" s="10" customFormat="1">
+    <row r="30" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A30" s="9"/>
       <c r="B30" s="17"/>
       <c r="E30" s="9"/>
@@ -5672,7 +5663,7 @@
       <c r="BP30" s="9"/>
       <c r="BQ30" s="9"/>
     </row>
-    <row r="31" spans="1:102" s="10" customFormat="1">
+    <row r="31" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A31" s="9"/>
       <c r="B31" s="17"/>
       <c r="E31" s="9"/>
@@ -5723,7 +5714,7 @@
       <c r="BP31" s="9"/>
       <c r="BQ31" s="9"/>
     </row>
-    <row r="32" spans="1:102" s="10" customFormat="1">
+    <row r="32" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A32" s="9"/>
       <c r="B32" s="17"/>
       <c r="E32" s="9"/>
@@ -5774,7 +5765,7 @@
       <c r="BP32" s="9"/>
       <c r="BQ32" s="9"/>
     </row>
-    <row r="33" spans="1:102" s="10" customFormat="1">
+    <row r="33" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A33" s="9"/>
       <c r="B33" s="17"/>
       <c r="E33" s="9"/>
@@ -5825,7 +5816,7 @@
       <c r="BP33" s="9"/>
       <c r="BQ33" s="9"/>
     </row>
-    <row r="34" spans="1:102" s="10" customFormat="1">
+    <row r="34" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A34" s="9"/>
       <c r="B34" s="17"/>
       <c r="E34" s="9"/>
@@ -5876,7 +5867,7 @@
       <c r="BP34" s="9"/>
       <c r="BQ34" s="9"/>
     </row>
-    <row r="35" spans="1:102" s="10" customFormat="1">
+    <row r="35" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A35" s="9"/>
       <c r="B35" s="17"/>
       <c r="E35" s="9"/>
@@ -5927,7 +5918,7 @@
       <c r="BP35" s="9"/>
       <c r="BQ35" s="9"/>
     </row>
-    <row r="36" spans="1:102" s="10" customFormat="1">
+    <row r="36" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A36" s="9"/>
       <c r="B36" s="17"/>
       <c r="E36" s="9"/>
@@ -5978,7 +5969,7 @@
       <c r="BP36" s="9"/>
       <c r="BQ36" s="9"/>
     </row>
-    <row r="37" spans="1:102" s="10" customFormat="1">
+    <row r="37" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A37" s="9"/>
       <c r="B37" s="17"/>
       <c r="E37" s="9"/>
@@ -6029,7 +6020,7 @@
       <c r="BP37" s="9"/>
       <c r="BQ37" s="9"/>
     </row>
-    <row r="38" spans="1:102" s="10" customFormat="1">
+    <row r="38" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A38" s="9"/>
       <c r="B38" s="17"/>
       <c r="E38" s="9"/>
@@ -6080,7 +6071,7 @@
       <c r="BP38" s="9"/>
       <c r="BQ38" s="9"/>
     </row>
-    <row r="39" spans="1:102" s="10" customFormat="1">
+    <row r="39" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A39" s="9"/>
       <c r="B39" s="17"/>
       <c r="E39" s="9"/>
@@ -6131,7 +6122,7 @@
       <c r="BP39" s="9"/>
       <c r="BQ39" s="9"/>
     </row>
-    <row r="40" spans="1:102" s="10" customFormat="1">
+    <row r="40" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A40" s="9"/>
       <c r="B40" s="17"/>
       <c r="E40" s="9"/>
@@ -6182,7 +6173,7 @@
       <c r="BP40" s="9"/>
       <c r="BQ40" s="9"/>
     </row>
-    <row r="41" spans="1:102" s="10" customFormat="1">
+    <row r="41" spans="1:102" s="10" customFormat="1" ht="409.6">
       <c r="A41" s="9"/>
       <c r="B41" s="17"/>
       <c r="E41" s="9"/>
@@ -17967,15 +17958,22 @@
   <hyperlinks>
     <hyperlink ref="X19" r:id="rId1" display="BOILERSOIL@GMAIL.COM :: Oil Burner Installer :: CONTROLLED PLBG CO., INC"/>
     <hyperlink ref="X23" r:id="rId2" display="BOILERSOIL@GMAIL.COM :: Oil Burner Installer :: CONTROLLED PLBG CO., INC"/>
-    <hyperlink ref="E23" r:id="rId3"/>
-    <hyperlink ref="D23" r:id="rId4" display="AJOETEST@GMAIL.COM :: Professional Engineer :: JA&amp; LLC"/>
-    <hyperlink ref="T23" r:id="rId5"/>
-    <hyperlink ref="AA23" r:id="rId6"/>
-    <hyperlink ref="AB23" r:id="rId7"/>
-    <hyperlink ref="T7" r:id="rId8"/>
-    <hyperlink ref="T19" r:id="rId9"/>
+    <hyperlink ref="T23" r:id="rId3"/>
+    <hyperlink ref="AA23" r:id="rId4"/>
+    <hyperlink ref="AB23" r:id="rId5"/>
+    <hyperlink ref="T19" r:id="rId6"/>
+    <hyperlink ref="T7" r:id="rId7"/>
+    <hyperlink ref="AA19" r:id="rId8"/>
+    <hyperlink ref="AA7" r:id="rId9"/>
+    <hyperlink ref="AB19" r:id="rId10"/>
+    <hyperlink ref="AB7" r:id="rId11"/>
+    <hyperlink ref="AA11" r:id="rId12"/>
+    <hyperlink ref="AB11" r:id="rId13"/>
+    <hyperlink ref="E11" r:id="rId14"/>
+    <hyperlink ref="AA15" r:id="rId15"/>
+    <hyperlink ref="AB15" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
latest data files as of 2019-01-17a
latest data files as of 2019-01-17a - 2 files
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases BEMSST.xlsx
+++ b/src/com/data/Test Cases BEMSST.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1185" windowWidth="22095" windowHeight="10605" tabRatio="152" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="22095" windowHeight="10200" tabRatio="152" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A5:J23"/>
+  <oleSize ref="A5:J22"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="160">
   <si>
     <t>TCID</t>
   </si>
@@ -483,10 +483,19 @@
     <t>AJOETEST@GMAIL.COM :: Mechanical Work :: 1 :: 0 :: 1</t>
   </si>
   <si>
-    <t>1 :: AJOETEST@GMAIL.COM :: Professional Engineer :: 005551 :: Fuel-Oil Storage and Fuel-Oil Piping Systems</t>
+    <t>BOILERSTEST1@GMAIL.COM :: Master Plumber :: SAMUEL &amp; SONS P &amp; H INC :: APPLEROME16@GMAIL.COM :: AJOETEST@GMAIL.COM</t>
   </si>
   <si>
-    <t>BOILERSTEST1@GMAIL.COM :: Master Plumber :: SAMUEL &amp; SONS P &amp; H INC :: APPLEROME16@GMAIL.COM :: AJOETEST@GMAIL.COM</t>
+    <t>1 :: AJOETEST@GMAIL.COM :: Professional Engineer :: 005546 :: Fuel-Oil Storage and Fuel-Oil Piping Systems</t>
+  </si>
+  <si>
+    <t>BeNewStdRep</t>
+  </si>
+  <si>
+    <t>AJOETEST@GMAIL.COM :: Mechanical Work :: 2 :: 2 :: 1</t>
+  </si>
+  <si>
+    <t>Boiler Equipment - Replacement - Standard</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1187,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1301,6 +1310,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="26" fillId="0" borderId="1" xfId="128" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="128" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1735,7 +1747,7 @@
   <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="12.75"/>
@@ -1803,9 +1815,13 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1">
-      <c r="A7" s="30"/>
+      <c r="A7" s="34" t="s">
+        <v>157</v>
+      </c>
       <c r="B7" s="30"/>
-      <c r="C7" s="33"/>
+      <c r="C7" s="32" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1">
       <c r="A8" s="30"/>
@@ -2165,11 +2181,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CX271"/>
+  <dimension ref="A1:CX276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -2197,7 +2213,7 @@
     <col min="21" max="21" width="18" style="9" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="45.7109375" style="9" customWidth="1"/>
     <col min="23" max="23" width="43.28515625" style="9" customWidth="1"/>
-    <col min="24" max="24" width="49" style="9" customWidth="1"/>
+    <col min="24" max="24" width="53.28515625" style="9" customWidth="1"/>
     <col min="25" max="25" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12.42578125" style="9" customWidth="1"/>
     <col min="27" max="27" width="21.7109375" style="9" bestFit="1" customWidth="1"/>
@@ -3450,7 +3466,7 @@
         <v>117</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>110</v>
@@ -4030,7 +4046,7 @@
         <v>119</v>
       </c>
       <c r="V15" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
@@ -4521,7 +4537,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:102" s="4" customFormat="1" ht="60">
+    <row r="19" spans="1:102" s="4" customFormat="1" ht="45">
       <c r="A19" s="26" t="s">
         <v>3</v>
       </c>
@@ -4588,7 +4604,7 @@
         <v>135</v>
       </c>
       <c r="X19" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Y19" s="11"/>
       <c r="Z19" s="11" t="s">
@@ -5303,265 +5319,563 @@
       <c r="BP24" s="9"/>
       <c r="BQ24" s="9"/>
     </row>
-    <row r="25" spans="1:102" s="10" customFormat="1">
-      <c r="A25" s="9"/>
-      <c r="B25" s="17"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="29"/>
-      <c r="R25" s="29"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="9"/>
-      <c r="X25" s="9"/>
-      <c r="Y25" s="9"/>
-      <c r="Z25" s="9"/>
-      <c r="AA25" s="9"/>
-      <c r="AB25" s="9"/>
-      <c r="AC25" s="9"/>
-      <c r="AD25" s="9"/>
-      <c r="AE25" s="9"/>
-      <c r="AF25" s="9"/>
-      <c r="AG25" s="9"/>
-      <c r="AH25" s="9"/>
-      <c r="AJ25" s="9"/>
-      <c r="AK25" s="9"/>
-      <c r="AL25" s="9"/>
-      <c r="AM25" s="9"/>
-      <c r="AN25" s="9"/>
-      <c r="AO25" s="9"/>
-      <c r="AP25" s="9"/>
-      <c r="AR25" s="9"/>
-      <c r="AT25" s="9"/>
-      <c r="AU25" s="9"/>
-      <c r="AV25" s="9"/>
-      <c r="AW25" s="9"/>
-      <c r="AX25" s="9"/>
-      <c r="BH25" s="9"/>
-      <c r="BJ25" s="9"/>
-      <c r="BK25" s="9"/>
-      <c r="BL25" s="9"/>
-      <c r="BM25" s="9"/>
-      <c r="BN25" s="9"/>
-      <c r="BO25" s="9"/>
-      <c r="BP25" s="9"/>
-      <c r="BQ25" s="9"/>
-    </row>
-    <row r="26" spans="1:102" s="25" customFormat="1" ht="409.6">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="22"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="24"/>
-      <c r="Z26" s="24"/>
-      <c r="AA26" s="24"/>
-      <c r="AB26" s="24"/>
-      <c r="AC26" s="24"/>
-      <c r="AD26" s="24"/>
-      <c r="AE26" s="24"/>
-      <c r="AF26" s="24"/>
-      <c r="AG26" s="24"/>
-      <c r="AH26" s="24"/>
-      <c r="AJ26" s="22"/>
-      <c r="AK26" s="22"/>
-      <c r="AL26" s="22"/>
-      <c r="AM26" s="22"/>
-      <c r="AN26" s="22"/>
-      <c r="AO26" s="24"/>
-      <c r="AP26" s="22"/>
-      <c r="AR26" s="22"/>
-      <c r="AS26" s="22"/>
-      <c r="AT26" s="24"/>
-      <c r="AU26" s="22"/>
-      <c r="AV26" s="22"/>
-      <c r="AW26" s="22"/>
-      <c r="AX26" s="22"/>
-      <c r="AY26" s="22"/>
-      <c r="AZ26" s="22"/>
-      <c r="BA26" s="22"/>
-      <c r="BB26" s="24"/>
-      <c r="BC26" s="24"/>
-      <c r="BD26" s="24"/>
-      <c r="BE26" s="22"/>
-      <c r="BF26" s="22"/>
-      <c r="BG26" s="22"/>
-      <c r="BH26" s="22"/>
-      <c r="BI26" s="22"/>
-      <c r="BJ26" s="22"/>
-      <c r="BK26" s="22"/>
-      <c r="BL26" s="22"/>
-      <c r="BM26" s="22"/>
-      <c r="BN26" s="22"/>
-      <c r="BO26" s="22"/>
-      <c r="BP26" s="24"/>
-      <c r="BQ26" s="24"/>
-    </row>
-    <row r="27" spans="1:102" s="25" customFormat="1" ht="409.6">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="22"/>
-      <c r="U27" s="24"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="24"/>
-      <c r="Z27" s="24"/>
-      <c r="AA27" s="24"/>
-      <c r="AB27" s="24"/>
-      <c r="AC27" s="24"/>
-      <c r="AD27" s="24"/>
-      <c r="AE27" s="24"/>
-      <c r="AF27" s="24"/>
-      <c r="AG27" s="24"/>
-      <c r="AH27" s="24"/>
-      <c r="AJ27" s="22"/>
-      <c r="AK27" s="22"/>
-      <c r="AL27" s="22"/>
-      <c r="AM27" s="22"/>
-      <c r="AN27" s="22"/>
-      <c r="AO27" s="24"/>
-      <c r="AP27" s="22"/>
-      <c r="AR27" s="22"/>
-      <c r="AS27" s="22"/>
-      <c r="AT27" s="24"/>
-      <c r="AU27" s="22"/>
-      <c r="AV27" s="22"/>
-      <c r="AW27" s="22"/>
-      <c r="AX27" s="22"/>
-      <c r="AY27" s="22"/>
-      <c r="AZ27" s="22"/>
-      <c r="BA27" s="22"/>
-      <c r="BB27" s="24"/>
-      <c r="BC27" s="24"/>
-      <c r="BD27" s="24"/>
-      <c r="BE27" s="22"/>
-      <c r="BF27" s="22"/>
-      <c r="BG27" s="22"/>
-      <c r="BH27" s="22"/>
-      <c r="BI27" s="22"/>
-      <c r="BJ27" s="22"/>
-      <c r="BK27" s="22"/>
-      <c r="BL27" s="22"/>
-      <c r="BM27" s="22"/>
-      <c r="BN27" s="22"/>
-      <c r="BO27" s="22"/>
-      <c r="BP27" s="24"/>
-      <c r="BQ27" s="24"/>
-    </row>
-    <row r="28" spans="1:102" s="25" customFormat="1" ht="409.6">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="24"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="24"/>
-      <c r="Z28" s="24"/>
-      <c r="AA28" s="24"/>
-      <c r="AB28" s="24"/>
-      <c r="AC28" s="24"/>
-      <c r="AD28" s="24"/>
-      <c r="AE28" s="24"/>
-      <c r="AF28" s="24"/>
-      <c r="AG28" s="24"/>
-      <c r="AH28" s="24"/>
-      <c r="AJ28" s="22"/>
-      <c r="AK28" s="22"/>
-      <c r="AL28" s="22"/>
-      <c r="AM28" s="22"/>
-      <c r="AN28" s="22"/>
-      <c r="AO28" s="24"/>
-      <c r="AP28" s="22"/>
-      <c r="AR28" s="22"/>
-      <c r="AS28" s="22"/>
-      <c r="AT28" s="24"/>
-      <c r="AU28" s="22"/>
-      <c r="AV28" s="22"/>
-      <c r="AW28" s="22"/>
-      <c r="AX28" s="22"/>
-      <c r="AY28" s="22"/>
-      <c r="AZ28" s="22"/>
-      <c r="BA28" s="22"/>
-      <c r="BB28" s="24"/>
-      <c r="BC28" s="24"/>
-      <c r="BD28" s="24"/>
-      <c r="BE28" s="22"/>
-      <c r="BF28" s="22"/>
-      <c r="BG28" s="22"/>
-      <c r="BH28" s="22"/>
-      <c r="BI28" s="22"/>
-      <c r="BJ28" s="22"/>
-      <c r="BK28" s="22"/>
-      <c r="BL28" s="22"/>
-      <c r="BM28" s="22"/>
-      <c r="BN28" s="22"/>
-      <c r="BO28" s="22"/>
-      <c r="BP28" s="24"/>
-      <c r="BQ28" s="24"/>
-    </row>
-    <row r="29" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="25" spans="1:102" s="7" customFormat="1">
+      <c r="A25" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="6"/>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="6"/>
+      <c r="AG25" s="6"/>
+      <c r="AH25" s="6"/>
+      <c r="AJ25" s="6"/>
+      <c r="AK25" s="6"/>
+      <c r="AL25" s="6"/>
+      <c r="AM25" s="6"/>
+      <c r="AN25" s="6"/>
+      <c r="AO25" s="6"/>
+      <c r="AP25" s="6"/>
+      <c r="AR25" s="6"/>
+      <c r="AT25" s="6"/>
+      <c r="AU25" s="6"/>
+      <c r="AV25" s="6"/>
+      <c r="AW25" s="6"/>
+      <c r="AX25" s="6"/>
+      <c r="BH25" s="6"/>
+      <c r="BJ25" s="6"/>
+      <c r="BK25" s="6"/>
+      <c r="BL25" s="6"/>
+      <c r="BM25" s="6"/>
+      <c r="BN25" s="6"/>
+      <c r="BO25" s="6"/>
+      <c r="BP25" s="6"/>
+      <c r="BQ25" s="6"/>
+    </row>
+    <row r="26" spans="1:102" s="8" customFormat="1" ht="38.25">
+      <c r="A26" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="R26" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="S26" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="T26" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="U26" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="V26" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="W26" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="X26" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z26" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE26" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF26" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG26" s="5"/>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ26" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK26" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL26" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM26" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN26" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP26" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR26" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS26" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT26" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU26" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV26" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW26" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX26" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AZ26" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="BA26" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB26" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC26" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="BD26" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE26" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG26" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="BH26" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI26" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="BJ26" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK26" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="BL26" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="BM26" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="BN26" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="BO26" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BP26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BQ26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="BR26" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="BS26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BT26" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="BU26" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="BV26" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BW26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BX26" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BY26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BZ26" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CA26" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="CB26" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="CC26" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CD26" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="CE26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="CF26" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CG26" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="CH26" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="CI26" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="CJ26" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CL26" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="CM26" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CO26" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:102" s="4" customFormat="1" ht="45">
+      <c r="A27" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="M27" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="R27" s="11"/>
+      <c r="S27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T27" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="U27" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="V27" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="W27" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="X27" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA27" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB27" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD27" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE27" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF27" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG27" s="11"/>
+      <c r="AH27" s="11"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL27" s="3"/>
+      <c r="AM27" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN27" s="3"/>
+      <c r="AO27" s="11"/>
+      <c r="AP27" s="3"/>
+      <c r="AR27" s="3"/>
+      <c r="AS27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT27" s="11"/>
+      <c r="AU27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW27" s="3"/>
+      <c r="AX27" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="AY27" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA27" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB27" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="BC27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="BD27" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="BE27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="BF27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="BH27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="BI27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BJ27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK27" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BL27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="BM27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="BN27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BO27" s="3"/>
+      <c r="BP27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BQ27" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:102" s="10" customFormat="1">
+      <c r="A28" s="9"/>
+      <c r="B28" s="17"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+      <c r="AA28" s="9"/>
+      <c r="AB28" s="9"/>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9"/>
+      <c r="AF28" s="9"/>
+      <c r="AG28" s="9"/>
+      <c r="AH28" s="9"/>
+      <c r="AJ28" s="9"/>
+      <c r="AK28" s="9"/>
+      <c r="AL28" s="9"/>
+      <c r="AM28" s="9"/>
+      <c r="AN28" s="9"/>
+      <c r="AO28" s="9"/>
+      <c r="AP28" s="9"/>
+      <c r="AR28" s="9"/>
+      <c r="AT28" s="9"/>
+      <c r="AU28" s="9"/>
+      <c r="AV28" s="9"/>
+      <c r="AW28" s="9"/>
+      <c r="AX28" s="9"/>
+      <c r="BH28" s="9"/>
+      <c r="BJ28" s="9"/>
+      <c r="BK28" s="9"/>
+      <c r="BL28" s="9"/>
+      <c r="BM28" s="9"/>
+      <c r="BN28" s="9"/>
+      <c r="BO28" s="9"/>
+      <c r="BP28" s="9"/>
+      <c r="BQ28" s="9"/>
+    </row>
+    <row r="29" spans="1:102" s="10" customFormat="1">
       <c r="A29" s="9"/>
       <c r="B29" s="17"/>
       <c r="E29" s="9"/>
@@ -5612,7 +5926,7 @@
       <c r="BP29" s="9"/>
       <c r="BQ29" s="9"/>
     </row>
-    <row r="30" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="30" spans="1:102" s="10" customFormat="1">
       <c r="A30" s="9"/>
       <c r="B30" s="17"/>
       <c r="E30" s="9"/>
@@ -5663,160 +5977,214 @@
       <c r="BP30" s="9"/>
       <c r="BQ30" s="9"/>
     </row>
-    <row r="31" spans="1:102" s="10" customFormat="1" ht="409.6">
-      <c r="A31" s="9"/>
-      <c r="B31" s="17"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="29"/>
-      <c r="R31" s="29"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="9"/>
-      <c r="Y31" s="9"/>
-      <c r="Z31" s="9"/>
-      <c r="AA31" s="9"/>
-      <c r="AB31" s="9"/>
-      <c r="AC31" s="9"/>
-      <c r="AD31" s="9"/>
-      <c r="AE31" s="9"/>
-      <c r="AF31" s="9"/>
-      <c r="AG31" s="9"/>
-      <c r="AH31" s="9"/>
-      <c r="AJ31" s="9"/>
-      <c r="AK31" s="9"/>
-      <c r="AL31" s="9"/>
-      <c r="AM31" s="9"/>
-      <c r="AN31" s="9"/>
-      <c r="AO31" s="9"/>
-      <c r="AP31" s="9"/>
-      <c r="AR31" s="9"/>
-      <c r="AT31" s="9"/>
-      <c r="AU31" s="9"/>
-      <c r="AV31" s="9"/>
-      <c r="AW31" s="9"/>
-      <c r="AX31" s="9"/>
-      <c r="BH31" s="9"/>
-      <c r="BJ31" s="9"/>
-      <c r="BK31" s="9"/>
-      <c r="BL31" s="9"/>
-      <c r="BM31" s="9"/>
-      <c r="BN31" s="9"/>
-      <c r="BO31" s="9"/>
-      <c r="BP31" s="9"/>
-      <c r="BQ31" s="9"/>
-    </row>
-    <row r="32" spans="1:102" s="10" customFormat="1" ht="409.6">
-      <c r="A32" s="9"/>
-      <c r="B32" s="17"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="29"/>
-      <c r="R32" s="29"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-      <c r="AA32" s="9"/>
-      <c r="AB32" s="9"/>
-      <c r="AC32" s="9"/>
-      <c r="AD32" s="9"/>
-      <c r="AE32" s="9"/>
-      <c r="AF32" s="9"/>
-      <c r="AG32" s="9"/>
-      <c r="AH32" s="9"/>
-      <c r="AJ32" s="9"/>
-      <c r="AK32" s="9"/>
-      <c r="AL32" s="9"/>
-      <c r="AM32" s="9"/>
-      <c r="AN32" s="9"/>
-      <c r="AO32" s="9"/>
-      <c r="AP32" s="9"/>
-      <c r="AR32" s="9"/>
-      <c r="AT32" s="9"/>
-      <c r="AU32" s="9"/>
-      <c r="AV32" s="9"/>
-      <c r="AW32" s="9"/>
-      <c r="AX32" s="9"/>
-      <c r="BH32" s="9"/>
-      <c r="BJ32" s="9"/>
-      <c r="BK32" s="9"/>
-      <c r="BL32" s="9"/>
-      <c r="BM32" s="9"/>
-      <c r="BN32" s="9"/>
-      <c r="BO32" s="9"/>
-      <c r="BP32" s="9"/>
-      <c r="BQ32" s="9"/>
-    </row>
-    <row r="33" spans="1:102" s="10" customFormat="1" ht="409.6">
-      <c r="A33" s="9"/>
-      <c r="B33" s="17"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="29"/>
-      <c r="R33" s="29"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
-      <c r="X33" s="9"/>
-      <c r="Y33" s="9"/>
-      <c r="Z33" s="9"/>
-      <c r="AA33" s="9"/>
-      <c r="AB33" s="9"/>
-      <c r="AC33" s="9"/>
-      <c r="AD33" s="9"/>
-      <c r="AE33" s="9"/>
-      <c r="AF33" s="9"/>
-      <c r="AG33" s="9"/>
-      <c r="AH33" s="9"/>
-      <c r="AJ33" s="9"/>
-      <c r="AK33" s="9"/>
-      <c r="AL33" s="9"/>
-      <c r="AM33" s="9"/>
-      <c r="AN33" s="9"/>
-      <c r="AO33" s="9"/>
-      <c r="AP33" s="9"/>
-      <c r="AR33" s="9"/>
-      <c r="AT33" s="9"/>
-      <c r="AU33" s="9"/>
-      <c r="AV33" s="9"/>
-      <c r="AW33" s="9"/>
-      <c r="AX33" s="9"/>
-      <c r="BH33" s="9"/>
-      <c r="BJ33" s="9"/>
-      <c r="BK33" s="9"/>
-      <c r="BL33" s="9"/>
-      <c r="BM33" s="9"/>
-      <c r="BN33" s="9"/>
-      <c r="BO33" s="9"/>
-      <c r="BP33" s="9"/>
-      <c r="BQ33" s="9"/>
-    </row>
-    <row r="34" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="31" spans="1:102" s="25" customFormat="1">
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
+      <c r="U31" s="24"/>
+      <c r="V31" s="24"/>
+      <c r="W31" s="24"/>
+      <c r="X31" s="24"/>
+      <c r="Y31" s="24"/>
+      <c r="Z31" s="24"/>
+      <c r="AA31" s="24"/>
+      <c r="AB31" s="24"/>
+      <c r="AC31" s="24"/>
+      <c r="AD31" s="24"/>
+      <c r="AE31" s="24"/>
+      <c r="AF31" s="24"/>
+      <c r="AG31" s="24"/>
+      <c r="AH31" s="24"/>
+      <c r="AJ31" s="22"/>
+      <c r="AK31" s="22"/>
+      <c r="AL31" s="22"/>
+      <c r="AM31" s="22"/>
+      <c r="AN31" s="22"/>
+      <c r="AO31" s="24"/>
+      <c r="AP31" s="22"/>
+      <c r="AR31" s="22"/>
+      <c r="AS31" s="22"/>
+      <c r="AT31" s="24"/>
+      <c r="AU31" s="22"/>
+      <c r="AV31" s="22"/>
+      <c r="AW31" s="22"/>
+      <c r="AX31" s="22"/>
+      <c r="AY31" s="22"/>
+      <c r="AZ31" s="22"/>
+      <c r="BA31" s="22"/>
+      <c r="BB31" s="24"/>
+      <c r="BC31" s="24"/>
+      <c r="BD31" s="24"/>
+      <c r="BE31" s="22"/>
+      <c r="BF31" s="22"/>
+      <c r="BG31" s="22"/>
+      <c r="BH31" s="22"/>
+      <c r="BI31" s="22"/>
+      <c r="BJ31" s="22"/>
+      <c r="BK31" s="22"/>
+      <c r="BL31" s="22"/>
+      <c r="BM31" s="22"/>
+      <c r="BN31" s="22"/>
+      <c r="BO31" s="22"/>
+      <c r="BP31" s="24"/>
+      <c r="BQ31" s="24"/>
+    </row>
+    <row r="32" spans="1:102" s="25" customFormat="1">
+      <c r="A32" s="22"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="24"/>
+      <c r="V32" s="24"/>
+      <c r="W32" s="24"/>
+      <c r="X32" s="24"/>
+      <c r="Y32" s="24"/>
+      <c r="Z32" s="24"/>
+      <c r="AA32" s="24"/>
+      <c r="AB32" s="24"/>
+      <c r="AC32" s="24"/>
+      <c r="AD32" s="24"/>
+      <c r="AE32" s="24"/>
+      <c r="AF32" s="24"/>
+      <c r="AG32" s="24"/>
+      <c r="AH32" s="24"/>
+      <c r="AJ32" s="22"/>
+      <c r="AK32" s="22"/>
+      <c r="AL32" s="22"/>
+      <c r="AM32" s="22"/>
+      <c r="AN32" s="22"/>
+      <c r="AO32" s="24"/>
+      <c r="AP32" s="22"/>
+      <c r="AR32" s="22"/>
+      <c r="AS32" s="22"/>
+      <c r="AT32" s="24"/>
+      <c r="AU32" s="22"/>
+      <c r="AV32" s="22"/>
+      <c r="AW32" s="22"/>
+      <c r="AX32" s="22"/>
+      <c r="AY32" s="22"/>
+      <c r="AZ32" s="22"/>
+      <c r="BA32" s="22"/>
+      <c r="BB32" s="24"/>
+      <c r="BC32" s="24"/>
+      <c r="BD32" s="24"/>
+      <c r="BE32" s="22"/>
+      <c r="BF32" s="22"/>
+      <c r="BG32" s="22"/>
+      <c r="BH32" s="22"/>
+      <c r="BI32" s="22"/>
+      <c r="BJ32" s="22"/>
+      <c r="BK32" s="22"/>
+      <c r="BL32" s="22"/>
+      <c r="BM32" s="22"/>
+      <c r="BN32" s="22"/>
+      <c r="BO32" s="22"/>
+      <c r="BP32" s="24"/>
+      <c r="BQ32" s="24"/>
+    </row>
+    <row r="33" spans="1:102" s="25" customFormat="1">
+      <c r="A33" s="22"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="24"/>
+      <c r="W33" s="24"/>
+      <c r="X33" s="24"/>
+      <c r="Y33" s="24"/>
+      <c r="Z33" s="24"/>
+      <c r="AA33" s="24"/>
+      <c r="AB33" s="24"/>
+      <c r="AC33" s="24"/>
+      <c r="AD33" s="24"/>
+      <c r="AE33" s="24"/>
+      <c r="AF33" s="24"/>
+      <c r="AG33" s="24"/>
+      <c r="AH33" s="24"/>
+      <c r="AJ33" s="22"/>
+      <c r="AK33" s="22"/>
+      <c r="AL33" s="22"/>
+      <c r="AM33" s="22"/>
+      <c r="AN33" s="22"/>
+      <c r="AO33" s="24"/>
+      <c r="AP33" s="22"/>
+      <c r="AR33" s="22"/>
+      <c r="AS33" s="22"/>
+      <c r="AT33" s="24"/>
+      <c r="AU33" s="22"/>
+      <c r="AV33" s="22"/>
+      <c r="AW33" s="22"/>
+      <c r="AX33" s="22"/>
+      <c r="AY33" s="22"/>
+      <c r="AZ33" s="22"/>
+      <c r="BA33" s="22"/>
+      <c r="BB33" s="24"/>
+      <c r="BC33" s="24"/>
+      <c r="BD33" s="24"/>
+      <c r="BE33" s="22"/>
+      <c r="BF33" s="22"/>
+      <c r="BG33" s="22"/>
+      <c r="BH33" s="22"/>
+      <c r="BI33" s="22"/>
+      <c r="BJ33" s="22"/>
+      <c r="BK33" s="22"/>
+      <c r="BL33" s="22"/>
+      <c r="BM33" s="22"/>
+      <c r="BN33" s="22"/>
+      <c r="BO33" s="22"/>
+      <c r="BP33" s="24"/>
+      <c r="BQ33" s="24"/>
+    </row>
+    <row r="34" spans="1:102" s="10" customFormat="1">
       <c r="A34" s="9"/>
       <c r="B34" s="17"/>
       <c r="E34" s="9"/>
@@ -5867,7 +6235,7 @@
       <c r="BP34" s="9"/>
       <c r="BQ34" s="9"/>
     </row>
-    <row r="35" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="35" spans="1:102" s="10" customFormat="1">
       <c r="A35" s="9"/>
       <c r="B35" s="17"/>
       <c r="E35" s="9"/>
@@ -5918,7 +6286,7 @@
       <c r="BP35" s="9"/>
       <c r="BQ35" s="9"/>
     </row>
-    <row r="36" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="36" spans="1:102" s="10" customFormat="1">
       <c r="A36" s="9"/>
       <c r="B36" s="17"/>
       <c r="E36" s="9"/>
@@ -5969,7 +6337,7 @@
       <c r="BP36" s="9"/>
       <c r="BQ36" s="9"/>
     </row>
-    <row r="37" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="37" spans="1:102" s="10" customFormat="1">
       <c r="A37" s="9"/>
       <c r="B37" s="17"/>
       <c r="E37" s="9"/>
@@ -6020,7 +6388,7 @@
       <c r="BP37" s="9"/>
       <c r="BQ37" s="9"/>
     </row>
-    <row r="38" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="38" spans="1:102" s="10" customFormat="1">
       <c r="A38" s="9"/>
       <c r="B38" s="17"/>
       <c r="E38" s="9"/>
@@ -6071,7 +6439,7 @@
       <c r="BP38" s="9"/>
       <c r="BQ38" s="9"/>
     </row>
-    <row r="39" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="39" spans="1:102" s="10" customFormat="1">
       <c r="A39" s="9"/>
       <c r="B39" s="17"/>
       <c r="E39" s="9"/>
@@ -6122,7 +6490,7 @@
       <c r="BP39" s="9"/>
       <c r="BQ39" s="9"/>
     </row>
-    <row r="40" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="40" spans="1:102" s="10" customFormat="1">
       <c r="A40" s="9"/>
       <c r="B40" s="17"/>
       <c r="E40" s="9"/>
@@ -6173,7 +6541,7 @@
       <c r="BP40" s="9"/>
       <c r="BQ40" s="9"/>
     </row>
-    <row r="41" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="41" spans="1:102" s="10" customFormat="1">
       <c r="A41" s="9"/>
       <c r="B41" s="17"/>
       <c r="E41" s="9"/>
@@ -6224,7 +6592,7 @@
       <c r="BP41" s="9"/>
       <c r="BQ41" s="9"/>
     </row>
-    <row r="42" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="42" spans="1:102" s="10" customFormat="1">
       <c r="A42" s="9"/>
       <c r="B42" s="17"/>
       <c r="E42" s="9"/>
@@ -17954,6 +18322,261 @@
       <c r="BP271" s="9"/>
       <c r="BQ271" s="9"/>
     </row>
+    <row r="272" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A272" s="9"/>
+      <c r="B272" s="17"/>
+      <c r="E272" s="9"/>
+      <c r="F272" s="9"/>
+      <c r="G272" s="9"/>
+      <c r="K272" s="28"/>
+      <c r="L272" s="9"/>
+      <c r="M272" s="9"/>
+      <c r="N272" s="9"/>
+      <c r="O272" s="9"/>
+      <c r="P272" s="9"/>
+      <c r="Q272" s="29"/>
+      <c r="R272" s="29"/>
+      <c r="U272" s="9"/>
+      <c r="V272" s="9"/>
+      <c r="W272" s="9"/>
+      <c r="X272" s="9"/>
+      <c r="Y272" s="9"/>
+      <c r="Z272" s="9"/>
+      <c r="AA272" s="9"/>
+      <c r="AB272" s="9"/>
+      <c r="AC272" s="9"/>
+      <c r="AD272" s="9"/>
+      <c r="AE272" s="9"/>
+      <c r="AF272" s="9"/>
+      <c r="AG272" s="9"/>
+      <c r="AH272" s="9"/>
+      <c r="AJ272" s="9"/>
+      <c r="AK272" s="9"/>
+      <c r="AL272" s="9"/>
+      <c r="AM272" s="9"/>
+      <c r="AN272" s="9"/>
+      <c r="AO272" s="9"/>
+      <c r="AP272" s="9"/>
+      <c r="AR272" s="9"/>
+      <c r="AT272" s="9"/>
+      <c r="AU272" s="9"/>
+      <c r="AV272" s="9"/>
+      <c r="AW272" s="9"/>
+      <c r="AX272" s="9"/>
+      <c r="BH272" s="9"/>
+      <c r="BJ272" s="9"/>
+      <c r="BK272" s="9"/>
+      <c r="BL272" s="9"/>
+      <c r="BM272" s="9"/>
+      <c r="BN272" s="9"/>
+      <c r="BO272" s="9"/>
+      <c r="BP272" s="9"/>
+      <c r="BQ272" s="9"/>
+    </row>
+    <row r="273" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A273" s="9"/>
+      <c r="B273" s="17"/>
+      <c r="E273" s="9"/>
+      <c r="F273" s="9"/>
+      <c r="G273" s="9"/>
+      <c r="K273" s="28"/>
+      <c r="L273" s="9"/>
+      <c r="M273" s="9"/>
+      <c r="N273" s="9"/>
+      <c r="O273" s="9"/>
+      <c r="P273" s="9"/>
+      <c r="Q273" s="29"/>
+      <c r="R273" s="29"/>
+      <c r="U273" s="9"/>
+      <c r="V273" s="9"/>
+      <c r="W273" s="9"/>
+      <c r="X273" s="9"/>
+      <c r="Y273" s="9"/>
+      <c r="Z273" s="9"/>
+      <c r="AA273" s="9"/>
+      <c r="AB273" s="9"/>
+      <c r="AC273" s="9"/>
+      <c r="AD273" s="9"/>
+      <c r="AE273" s="9"/>
+      <c r="AF273" s="9"/>
+      <c r="AG273" s="9"/>
+      <c r="AH273" s="9"/>
+      <c r="AJ273" s="9"/>
+      <c r="AK273" s="9"/>
+      <c r="AL273" s="9"/>
+      <c r="AM273" s="9"/>
+      <c r="AN273" s="9"/>
+      <c r="AO273" s="9"/>
+      <c r="AP273" s="9"/>
+      <c r="AR273" s="9"/>
+      <c r="AT273" s="9"/>
+      <c r="AU273" s="9"/>
+      <c r="AV273" s="9"/>
+      <c r="AW273" s="9"/>
+      <c r="AX273" s="9"/>
+      <c r="BH273" s="9"/>
+      <c r="BJ273" s="9"/>
+      <c r="BK273" s="9"/>
+      <c r="BL273" s="9"/>
+      <c r="BM273" s="9"/>
+      <c r="BN273" s="9"/>
+      <c r="BO273" s="9"/>
+      <c r="BP273" s="9"/>
+      <c r="BQ273" s="9"/>
+    </row>
+    <row r="274" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A274" s="9"/>
+      <c r="B274" s="17"/>
+      <c r="E274" s="9"/>
+      <c r="F274" s="9"/>
+      <c r="G274" s="9"/>
+      <c r="K274" s="28"/>
+      <c r="L274" s="9"/>
+      <c r="M274" s="9"/>
+      <c r="N274" s="9"/>
+      <c r="O274" s="9"/>
+      <c r="P274" s="9"/>
+      <c r="Q274" s="29"/>
+      <c r="R274" s="29"/>
+      <c r="U274" s="9"/>
+      <c r="V274" s="9"/>
+      <c r="W274" s="9"/>
+      <c r="X274" s="9"/>
+      <c r="Y274" s="9"/>
+      <c r="Z274" s="9"/>
+      <c r="AA274" s="9"/>
+      <c r="AB274" s="9"/>
+      <c r="AC274" s="9"/>
+      <c r="AD274" s="9"/>
+      <c r="AE274" s="9"/>
+      <c r="AF274" s="9"/>
+      <c r="AG274" s="9"/>
+      <c r="AH274" s="9"/>
+      <c r="AJ274" s="9"/>
+      <c r="AK274" s="9"/>
+      <c r="AL274" s="9"/>
+      <c r="AM274" s="9"/>
+      <c r="AN274" s="9"/>
+      <c r="AO274" s="9"/>
+      <c r="AP274" s="9"/>
+      <c r="AR274" s="9"/>
+      <c r="AT274" s="9"/>
+      <c r="AU274" s="9"/>
+      <c r="AV274" s="9"/>
+      <c r="AW274" s="9"/>
+      <c r="AX274" s="9"/>
+      <c r="BH274" s="9"/>
+      <c r="BJ274" s="9"/>
+      <c r="BK274" s="9"/>
+      <c r="BL274" s="9"/>
+      <c r="BM274" s="9"/>
+      <c r="BN274" s="9"/>
+      <c r="BO274" s="9"/>
+      <c r="BP274" s="9"/>
+      <c r="BQ274" s="9"/>
+    </row>
+    <row r="275" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A275" s="9"/>
+      <c r="B275" s="17"/>
+      <c r="E275" s="9"/>
+      <c r="F275" s="9"/>
+      <c r="G275" s="9"/>
+      <c r="K275" s="28"/>
+      <c r="L275" s="9"/>
+      <c r="M275" s="9"/>
+      <c r="N275" s="9"/>
+      <c r="O275" s="9"/>
+      <c r="P275" s="9"/>
+      <c r="Q275" s="29"/>
+      <c r="R275" s="29"/>
+      <c r="U275" s="9"/>
+      <c r="V275" s="9"/>
+      <c r="W275" s="9"/>
+      <c r="X275" s="9"/>
+      <c r="Y275" s="9"/>
+      <c r="Z275" s="9"/>
+      <c r="AA275" s="9"/>
+      <c r="AB275" s="9"/>
+      <c r="AC275" s="9"/>
+      <c r="AD275" s="9"/>
+      <c r="AE275" s="9"/>
+      <c r="AF275" s="9"/>
+      <c r="AG275" s="9"/>
+      <c r="AH275" s="9"/>
+      <c r="AJ275" s="9"/>
+      <c r="AK275" s="9"/>
+      <c r="AL275" s="9"/>
+      <c r="AM275" s="9"/>
+      <c r="AN275" s="9"/>
+      <c r="AO275" s="9"/>
+      <c r="AP275" s="9"/>
+      <c r="AR275" s="9"/>
+      <c r="AT275" s="9"/>
+      <c r="AU275" s="9"/>
+      <c r="AV275" s="9"/>
+      <c r="AW275" s="9"/>
+      <c r="AX275" s="9"/>
+      <c r="BH275" s="9"/>
+      <c r="BJ275" s="9"/>
+      <c r="BK275" s="9"/>
+      <c r="BL275" s="9"/>
+      <c r="BM275" s="9"/>
+      <c r="BN275" s="9"/>
+      <c r="BO275" s="9"/>
+      <c r="BP275" s="9"/>
+      <c r="BQ275" s="9"/>
+    </row>
+    <row r="276" spans="1:102" s="10" customFormat="1" ht="409.6">
+      <c r="A276" s="9"/>
+      <c r="B276" s="17"/>
+      <c r="E276" s="9"/>
+      <c r="F276" s="9"/>
+      <c r="G276" s="9"/>
+      <c r="K276" s="28"/>
+      <c r="L276" s="9"/>
+      <c r="M276" s="9"/>
+      <c r="N276" s="9"/>
+      <c r="O276" s="9"/>
+      <c r="P276" s="9"/>
+      <c r="Q276" s="29"/>
+      <c r="R276" s="29"/>
+      <c r="U276" s="9"/>
+      <c r="V276" s="9"/>
+      <c r="W276" s="9"/>
+      <c r="X276" s="9"/>
+      <c r="Y276" s="9"/>
+      <c r="Z276" s="9"/>
+      <c r="AA276" s="9"/>
+      <c r="AB276" s="9"/>
+      <c r="AC276" s="9"/>
+      <c r="AD276" s="9"/>
+      <c r="AE276" s="9"/>
+      <c r="AF276" s="9"/>
+      <c r="AG276" s="9"/>
+      <c r="AH276" s="9"/>
+      <c r="AJ276" s="9"/>
+      <c r="AK276" s="9"/>
+      <c r="AL276" s="9"/>
+      <c r="AM276" s="9"/>
+      <c r="AN276" s="9"/>
+      <c r="AO276" s="9"/>
+      <c r="AP276" s="9"/>
+      <c r="AR276" s="9"/>
+      <c r="AT276" s="9"/>
+      <c r="AU276" s="9"/>
+      <c r="AV276" s="9"/>
+      <c r="AW276" s="9"/>
+      <c r="AX276" s="9"/>
+      <c r="BH276" s="9"/>
+      <c r="BJ276" s="9"/>
+      <c r="BK276" s="9"/>
+      <c r="BL276" s="9"/>
+      <c r="BM276" s="9"/>
+      <c r="BN276" s="9"/>
+      <c r="BO276" s="9"/>
+      <c r="BP276" s="9"/>
+      <c r="BQ276" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="X19" r:id="rId1" display="BOILERSOIL@GMAIL.COM :: Oil Burner Installer :: CONTROLLED PLBG CO., INC"/>
@@ -17972,8 +18595,13 @@
     <hyperlink ref="E11" r:id="rId14"/>
     <hyperlink ref="AA15" r:id="rId15"/>
     <hyperlink ref="AB15" r:id="rId16"/>
+    <hyperlink ref="X27" r:id="rId17" display="BOILERSOIL@GMAIL.COM :: Oil Burner Installer :: CONTROLLED PLBG CO., INC"/>
+    <hyperlink ref="T27" r:id="rId18"/>
+    <hyperlink ref="AA27" r:id="rId19"/>
+    <hyperlink ref="AB27" r:id="rId20"/>
+    <hyperlink ref="E27" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
latest data files as of 2019-01-18
latest data files as of 2019-01-18
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases BEMSST.xlsx
+++ b/src/com/data/Test Cases BEMSST.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="22095" windowHeight="10200" tabRatio="152" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="22095" windowHeight="9960" tabRatio="152" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A5:J22"/>
+  <oleSize ref="A19:J39"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="167">
   <si>
     <t>TCID</t>
   </si>
@@ -496,6 +496,27 @@
   </si>
   <si>
     <t>Boiler Equipment - Replacement - Standard</t>
+  </si>
+  <si>
+    <t>device</t>
+  </si>
+  <si>
+    <t>3 :: 10000230076N1111</t>
+  </si>
+  <si>
+    <t>1 :: 0 :: N :: N :: N :: N :: N :: N :: N :: N :: N :: N</t>
+  </si>
+  <si>
+    <t>3 :: 10000230074Y1111</t>
+  </si>
+  <si>
+    <t>Boiler Equipment - Modification - Standard</t>
+  </si>
+  <si>
+    <t>AJOETEST@GMAIL.COM :: Mechanical Work :: 2 :: 3 :: 1</t>
+  </si>
+  <si>
+    <t>BeNewStdMod</t>
   </si>
 </sst>
 </file>
@@ -1747,7 +1768,7 @@
   <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="12.75"/>
@@ -1824,9 +1845,13 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1">
-      <c r="A8" s="30"/>
+      <c r="A8" s="34" t="s">
+        <v>166</v>
+      </c>
       <c r="B8" s="30"/>
-      <c r="C8" s="33"/>
+      <c r="C8" s="32" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1">
       <c r="A9" s="30"/>
@@ -2181,11 +2206,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CX276"/>
+  <dimension ref="A1:CX279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J27" sqref="J27"/>
+      <selection pane="topRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -2697,7 +2722,9 @@
       <c r="AF6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AG6" s="5"/>
+      <c r="AG6" s="12" t="s">
+        <v>160</v>
+      </c>
       <c r="AH6" s="5"/>
       <c r="AI6" s="12" t="s">
         <v>82</v>
@@ -3251,7 +3278,9 @@
       <c r="AF10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AG10" s="5"/>
+      <c r="AG10" s="12" t="s">
+        <v>160</v>
+      </c>
       <c r="AH10" s="5"/>
       <c r="AI10" s="12" t="s">
         <v>82</v>
@@ -3805,7 +3834,9 @@
       <c r="AF14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AG14" s="5"/>
+      <c r="AG14" s="12" t="s">
+        <v>160</v>
+      </c>
       <c r="AH14" s="5"/>
       <c r="AI14" s="12" t="s">
         <v>82</v>
@@ -4357,7 +4388,9 @@
       <c r="AF18" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AG18" s="5"/>
+      <c r="AG18" s="12" t="s">
+        <v>160</v>
+      </c>
       <c r="AH18" s="5"/>
       <c r="AI18" s="12" t="s">
         <v>82</v>
@@ -4913,7 +4946,9 @@
       <c r="AF22" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AG22" s="5"/>
+      <c r="AG22" s="12" t="s">
+        <v>160</v>
+      </c>
       <c r="AH22" s="5"/>
       <c r="AI22" s="12" t="s">
         <v>82</v>
@@ -5469,7 +5504,9 @@
       <c r="AF26" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AG26" s="5"/>
+      <c r="AG26" s="12" t="s">
+        <v>160</v>
+      </c>
       <c r="AH26" s="5"/>
       <c r="AI26" s="12" t="s">
         <v>82</v>
@@ -5665,14 +5702,11 @@
       <c r="E27" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="G27" s="4" t="s">
         <v>108</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>3</v>
@@ -5740,7 +5774,9 @@
       <c r="AF27" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AG27" s="11"/>
+      <c r="AG27" s="4" t="s">
+        <v>161</v>
+      </c>
       <c r="AH27" s="11"/>
       <c r="AJ27" s="3"/>
       <c r="AK27" s="3" t="s">
@@ -5875,467 +5911,820 @@
       <c r="BP28" s="9"/>
       <c r="BQ28" s="9"/>
     </row>
-    <row r="29" spans="1:102" s="10" customFormat="1">
-      <c r="A29" s="9"/>
-      <c r="B29" s="17"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="29"/>
-      <c r="R29" s="29"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-      <c r="X29" s="9"/>
-      <c r="Y29" s="9"/>
-      <c r="Z29" s="9"/>
-      <c r="AA29" s="9"/>
-      <c r="AB29" s="9"/>
-      <c r="AC29" s="9"/>
-      <c r="AD29" s="9"/>
-      <c r="AE29" s="9"/>
-      <c r="AF29" s="9"/>
-      <c r="AG29" s="9"/>
-      <c r="AH29" s="9"/>
-      <c r="AJ29" s="9"/>
-      <c r="AK29" s="9"/>
-      <c r="AL29" s="9"/>
-      <c r="AM29" s="9"/>
-      <c r="AN29" s="9"/>
-      <c r="AO29" s="9"/>
-      <c r="AP29" s="9"/>
-      <c r="AR29" s="9"/>
-      <c r="AT29" s="9"/>
-      <c r="AU29" s="9"/>
-      <c r="AV29" s="9"/>
-      <c r="AW29" s="9"/>
-      <c r="AX29" s="9"/>
-      <c r="BH29" s="9"/>
-      <c r="BJ29" s="9"/>
-      <c r="BK29" s="9"/>
-      <c r="BL29" s="9"/>
-      <c r="BM29" s="9"/>
-      <c r="BN29" s="9"/>
-      <c r="BO29" s="9"/>
-      <c r="BP29" s="9"/>
-      <c r="BQ29" s="9"/>
-    </row>
-    <row r="30" spans="1:102" s="10" customFormat="1">
-      <c r="A30" s="9"/>
-      <c r="B30" s="17"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="29"/>
-      <c r="R30" s="29"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
-      <c r="X30" s="9"/>
-      <c r="Y30" s="9"/>
-      <c r="Z30" s="9"/>
-      <c r="AA30" s="9"/>
-      <c r="AB30" s="9"/>
-      <c r="AC30" s="9"/>
-      <c r="AD30" s="9"/>
-      <c r="AE30" s="9"/>
-      <c r="AF30" s="9"/>
-      <c r="AG30" s="9"/>
-      <c r="AH30" s="9"/>
-      <c r="AJ30" s="9"/>
-      <c r="AK30" s="9"/>
-      <c r="AL30" s="9"/>
-      <c r="AM30" s="9"/>
-      <c r="AN30" s="9"/>
-      <c r="AO30" s="9"/>
-      <c r="AP30" s="9"/>
-      <c r="AR30" s="9"/>
-      <c r="AT30" s="9"/>
-      <c r="AU30" s="9"/>
-      <c r="AV30" s="9"/>
-      <c r="AW30" s="9"/>
-      <c r="AX30" s="9"/>
-      <c r="BH30" s="9"/>
-      <c r="BJ30" s="9"/>
-      <c r="BK30" s="9"/>
-      <c r="BL30" s="9"/>
-      <c r="BM30" s="9"/>
-      <c r="BN30" s="9"/>
-      <c r="BO30" s="9"/>
-      <c r="BP30" s="9"/>
-      <c r="BQ30" s="9"/>
-    </row>
-    <row r="31" spans="1:102" s="25" customFormat="1">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="22"/>
-      <c r="T31" s="22"/>
-      <c r="U31" s="24"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="24"/>
-      <c r="X31" s="24"/>
-      <c r="Y31" s="24"/>
-      <c r="Z31" s="24"/>
-      <c r="AA31" s="24"/>
-      <c r="AB31" s="24"/>
-      <c r="AC31" s="24"/>
-      <c r="AD31" s="24"/>
-      <c r="AE31" s="24"/>
-      <c r="AF31" s="24"/>
-      <c r="AG31" s="24"/>
-      <c r="AH31" s="24"/>
-      <c r="AJ31" s="22"/>
-      <c r="AK31" s="22"/>
-      <c r="AL31" s="22"/>
-      <c r="AM31" s="22"/>
-      <c r="AN31" s="22"/>
-      <c r="AO31" s="24"/>
-      <c r="AP31" s="22"/>
-      <c r="AR31" s="22"/>
-      <c r="AS31" s="22"/>
-      <c r="AT31" s="24"/>
-      <c r="AU31" s="22"/>
-      <c r="AV31" s="22"/>
-      <c r="AW31" s="22"/>
-      <c r="AX31" s="22"/>
-      <c r="AY31" s="22"/>
-      <c r="AZ31" s="22"/>
-      <c r="BA31" s="22"/>
-      <c r="BB31" s="24"/>
-      <c r="BC31" s="24"/>
-      <c r="BD31" s="24"/>
-      <c r="BE31" s="22"/>
-      <c r="BF31" s="22"/>
-      <c r="BG31" s="22"/>
-      <c r="BH31" s="22"/>
-      <c r="BI31" s="22"/>
-      <c r="BJ31" s="22"/>
-      <c r="BK31" s="22"/>
-      <c r="BL31" s="22"/>
-      <c r="BM31" s="22"/>
-      <c r="BN31" s="22"/>
-      <c r="BO31" s="22"/>
-      <c r="BP31" s="24"/>
-      <c r="BQ31" s="24"/>
-    </row>
-    <row r="32" spans="1:102" s="25" customFormat="1">
-      <c r="A32" s="22"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
-      <c r="S32" s="22"/>
-      <c r="T32" s="22"/>
-      <c r="U32" s="24"/>
-      <c r="V32" s="24"/>
-      <c r="W32" s="24"/>
-      <c r="X32" s="24"/>
-      <c r="Y32" s="24"/>
-      <c r="Z32" s="24"/>
-      <c r="AA32" s="24"/>
-      <c r="AB32" s="24"/>
-      <c r="AC32" s="24"/>
-      <c r="AD32" s="24"/>
-      <c r="AE32" s="24"/>
-      <c r="AF32" s="24"/>
-      <c r="AG32" s="24"/>
-      <c r="AH32" s="24"/>
-      <c r="AJ32" s="22"/>
-      <c r="AK32" s="22"/>
-      <c r="AL32" s="22"/>
-      <c r="AM32" s="22"/>
-      <c r="AN32" s="22"/>
-      <c r="AO32" s="24"/>
-      <c r="AP32" s="22"/>
-      <c r="AR32" s="22"/>
-      <c r="AS32" s="22"/>
-      <c r="AT32" s="24"/>
-      <c r="AU32" s="22"/>
-      <c r="AV32" s="22"/>
-      <c r="AW32" s="22"/>
-      <c r="AX32" s="22"/>
-      <c r="AY32" s="22"/>
-      <c r="AZ32" s="22"/>
-      <c r="BA32" s="22"/>
-      <c r="BB32" s="24"/>
-      <c r="BC32" s="24"/>
-      <c r="BD32" s="24"/>
-      <c r="BE32" s="22"/>
-      <c r="BF32" s="22"/>
-      <c r="BG32" s="22"/>
-      <c r="BH32" s="22"/>
-      <c r="BI32" s="22"/>
-      <c r="BJ32" s="22"/>
-      <c r="BK32" s="22"/>
-      <c r="BL32" s="22"/>
-      <c r="BM32" s="22"/>
-      <c r="BN32" s="22"/>
-      <c r="BO32" s="22"/>
-      <c r="BP32" s="24"/>
-      <c r="BQ32" s="24"/>
-    </row>
-    <row r="33" spans="1:102" s="25" customFormat="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="24"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="22"/>
-      <c r="T33" s="22"/>
-      <c r="U33" s="24"/>
-      <c r="V33" s="24"/>
-      <c r="W33" s="24"/>
-      <c r="X33" s="24"/>
-      <c r="Y33" s="24"/>
-      <c r="Z33" s="24"/>
-      <c r="AA33" s="24"/>
-      <c r="AB33" s="24"/>
-      <c r="AC33" s="24"/>
-      <c r="AD33" s="24"/>
-      <c r="AE33" s="24"/>
-      <c r="AF33" s="24"/>
-      <c r="AG33" s="24"/>
-      <c r="AH33" s="24"/>
-      <c r="AJ33" s="22"/>
-      <c r="AK33" s="22"/>
-      <c r="AL33" s="22"/>
-      <c r="AM33" s="22"/>
-      <c r="AN33" s="22"/>
-      <c r="AO33" s="24"/>
-      <c r="AP33" s="22"/>
-      <c r="AR33" s="22"/>
-      <c r="AS33" s="22"/>
-      <c r="AT33" s="24"/>
-      <c r="AU33" s="22"/>
-      <c r="AV33" s="22"/>
-      <c r="AW33" s="22"/>
-      <c r="AX33" s="22"/>
-      <c r="AY33" s="22"/>
-      <c r="AZ33" s="22"/>
-      <c r="BA33" s="22"/>
-      <c r="BB33" s="24"/>
-      <c r="BC33" s="24"/>
-      <c r="BD33" s="24"/>
-      <c r="BE33" s="22"/>
-      <c r="BF33" s="22"/>
-      <c r="BG33" s="22"/>
-      <c r="BH33" s="22"/>
-      <c r="BI33" s="22"/>
-      <c r="BJ33" s="22"/>
-      <c r="BK33" s="22"/>
-      <c r="BL33" s="22"/>
-      <c r="BM33" s="22"/>
-      <c r="BN33" s="22"/>
-      <c r="BO33" s="22"/>
-      <c r="BP33" s="24"/>
-      <c r="BQ33" s="24"/>
-    </row>
-    <row r="34" spans="1:102" s="10" customFormat="1">
-      <c r="A34" s="9"/>
-      <c r="B34" s="17"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="29"/>
-      <c r="R34" s="29"/>
-      <c r="U34" s="9"/>
-      <c r="V34" s="9"/>
-      <c r="W34" s="9"/>
-      <c r="X34" s="9"/>
-      <c r="Y34" s="9"/>
-      <c r="Z34" s="9"/>
-      <c r="AA34" s="9"/>
-      <c r="AB34" s="9"/>
-      <c r="AC34" s="9"/>
-      <c r="AD34" s="9"/>
-      <c r="AE34" s="9"/>
-      <c r="AF34" s="9"/>
-      <c r="AG34" s="9"/>
-      <c r="AH34" s="9"/>
-      <c r="AJ34" s="9"/>
-      <c r="AK34" s="9"/>
-      <c r="AL34" s="9"/>
-      <c r="AM34" s="9"/>
-      <c r="AN34" s="9"/>
-      <c r="AO34" s="9"/>
-      <c r="AP34" s="9"/>
-      <c r="AR34" s="9"/>
-      <c r="AT34" s="9"/>
-      <c r="AU34" s="9"/>
-      <c r="AV34" s="9"/>
-      <c r="AW34" s="9"/>
-      <c r="AX34" s="9"/>
-      <c r="BH34" s="9"/>
-      <c r="BJ34" s="9"/>
-      <c r="BK34" s="9"/>
-      <c r="BL34" s="9"/>
-      <c r="BM34" s="9"/>
-      <c r="BN34" s="9"/>
-      <c r="BO34" s="9"/>
-      <c r="BP34" s="9"/>
-      <c r="BQ34" s="9"/>
-    </row>
-    <row r="35" spans="1:102" s="10" customFormat="1">
-      <c r="A35" s="9"/>
-      <c r="B35" s="17"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="K35" s="28"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="29"/>
-      <c r="R35" s="29"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="9"/>
-      <c r="Y35" s="9"/>
-      <c r="Z35" s="9"/>
-      <c r="AA35" s="9"/>
-      <c r="AB35" s="9"/>
-      <c r="AC35" s="9"/>
-      <c r="AD35" s="9"/>
-      <c r="AE35" s="9"/>
-      <c r="AF35" s="9"/>
-      <c r="AG35" s="9"/>
-      <c r="AH35" s="9"/>
-      <c r="AJ35" s="9"/>
-      <c r="AK35" s="9"/>
-      <c r="AL35" s="9"/>
-      <c r="AM35" s="9"/>
-      <c r="AN35" s="9"/>
-      <c r="AO35" s="9"/>
-      <c r="AP35" s="9"/>
-      <c r="AR35" s="9"/>
-      <c r="AT35" s="9"/>
-      <c r="AU35" s="9"/>
-      <c r="AV35" s="9"/>
-      <c r="AW35" s="9"/>
-      <c r="AX35" s="9"/>
-      <c r="BH35" s="9"/>
-      <c r="BJ35" s="9"/>
-      <c r="BK35" s="9"/>
-      <c r="BL35" s="9"/>
-      <c r="BM35" s="9"/>
-      <c r="BN35" s="9"/>
-      <c r="BO35" s="9"/>
-      <c r="BP35" s="9"/>
-      <c r="BQ35" s="9"/>
-    </row>
-    <row r="36" spans="1:102" s="10" customFormat="1">
-      <c r="A36" s="9"/>
-      <c r="B36" s="17"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="29"/>
-      <c r="R36" s="29"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="9"/>
-      <c r="W36" s="9"/>
-      <c r="X36" s="9"/>
-      <c r="Y36" s="9"/>
-      <c r="Z36" s="9"/>
-      <c r="AA36" s="9"/>
-      <c r="AB36" s="9"/>
-      <c r="AC36" s="9"/>
-      <c r="AD36" s="9"/>
-      <c r="AE36" s="9"/>
-      <c r="AF36" s="9"/>
-      <c r="AG36" s="9"/>
-      <c r="AH36" s="9"/>
-      <c r="AJ36" s="9"/>
-      <c r="AK36" s="9"/>
-      <c r="AL36" s="9"/>
-      <c r="AM36" s="9"/>
-      <c r="AN36" s="9"/>
-      <c r="AO36" s="9"/>
-      <c r="AP36" s="9"/>
-      <c r="AR36" s="9"/>
-      <c r="AT36" s="9"/>
-      <c r="AU36" s="9"/>
-      <c r="AV36" s="9"/>
-      <c r="AW36" s="9"/>
-      <c r="AX36" s="9"/>
-      <c r="BH36" s="9"/>
-      <c r="BJ36" s="9"/>
-      <c r="BK36" s="9"/>
-      <c r="BL36" s="9"/>
-      <c r="BM36" s="9"/>
-      <c r="BN36" s="9"/>
-      <c r="BO36" s="9"/>
-      <c r="BP36" s="9"/>
-      <c r="BQ36" s="9"/>
+    <row r="29" spans="1:102" s="7" customFormat="1">
+      <c r="A29" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="6"/>
+      <c r="Z29" s="6"/>
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="6"/>
+      <c r="AC29" s="6"/>
+      <c r="AD29" s="6"/>
+      <c r="AE29" s="6"/>
+      <c r="AF29" s="6"/>
+      <c r="AG29" s="6"/>
+      <c r="AH29" s="6"/>
+      <c r="AJ29" s="6"/>
+      <c r="AK29" s="6"/>
+      <c r="AL29" s="6"/>
+      <c r="AM29" s="6"/>
+      <c r="AN29" s="6"/>
+      <c r="AO29" s="6"/>
+      <c r="AP29" s="6"/>
+      <c r="AR29" s="6"/>
+      <c r="AT29" s="6"/>
+      <c r="AU29" s="6"/>
+      <c r="AV29" s="6"/>
+      <c r="AW29" s="6"/>
+      <c r="AX29" s="6"/>
+      <c r="BH29" s="6"/>
+      <c r="BJ29" s="6"/>
+      <c r="BK29" s="6"/>
+      <c r="BL29" s="6"/>
+      <c r="BM29" s="6"/>
+      <c r="BN29" s="6"/>
+      <c r="BO29" s="6"/>
+      <c r="BP29" s="6"/>
+      <c r="BQ29" s="6"/>
+    </row>
+    <row r="30" spans="1:102" s="8" customFormat="1" ht="38.25">
+      <c r="A30" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O30" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="R30" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="S30" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="T30" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="U30" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="V30" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="W30" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="X30" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y30" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z30" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE30" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF30" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG30" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH30" s="5"/>
+      <c r="AI30" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ30" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK30" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL30" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM30" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN30" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP30" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR30" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS30" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU30" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV30" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW30" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX30" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY30" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AZ30" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="BA30" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB30" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC30" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="BD30" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE30" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF30" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="BG30" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="BH30" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI30" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="BJ30" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK30" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="BL30" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="BM30" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="BN30" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="BO30" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BP30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BQ30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="BR30" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="BS30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BT30" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="BU30" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="BV30" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BW30" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BX30" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BY30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BZ30" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CA30" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="CB30" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="CC30" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="CD30" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="CE30" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="CF30" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CG30" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="CH30" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="CI30" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="CJ30" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK30" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="CL30" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="CM30" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN30" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CO30" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:102" s="4" customFormat="1" ht="45">
+      <c r="A31" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="N31" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q31" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="R31" s="11"/>
+      <c r="S31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T31" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="U31" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="V31" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="W31" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="X31" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA31" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB31" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC31" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD31" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE31" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF31" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG31" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AH31" s="11"/>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL31" s="3"/>
+      <c r="AM31" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN31" s="3"/>
+      <c r="AO31" s="11"/>
+      <c r="AP31" s="3"/>
+      <c r="AR31" s="3"/>
+      <c r="AS31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT31" s="11"/>
+      <c r="AU31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW31" s="3"/>
+      <c r="AX31" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="AY31" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA31" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB31" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="BC31" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="BD31" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="BE31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="BF31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="BH31" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="BI31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BJ31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BL31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="BM31" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="BN31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BO31" s="3"/>
+      <c r="BP31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BQ31" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:102" s="10" customFormat="1">
+      <c r="A32" s="9"/>
+      <c r="B32" s="17"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="29"/>
+      <c r="R32" s="29"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="9"/>
+      <c r="Z32" s="9"/>
+      <c r="AA32" s="9"/>
+      <c r="AB32" s="9"/>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="9"/>
+      <c r="AG32" s="9"/>
+      <c r="AH32" s="9"/>
+      <c r="AJ32" s="9"/>
+      <c r="AK32" s="9"/>
+      <c r="AL32" s="9"/>
+      <c r="AM32" s="9"/>
+      <c r="AN32" s="9"/>
+      <c r="AO32" s="9"/>
+      <c r="AP32" s="9"/>
+      <c r="AR32" s="9"/>
+      <c r="AT32" s="9"/>
+      <c r="AU32" s="9"/>
+      <c r="AV32" s="9"/>
+      <c r="AW32" s="9"/>
+      <c r="AX32" s="9"/>
+      <c r="BH32" s="9"/>
+      <c r="BJ32" s="9"/>
+      <c r="BK32" s="9"/>
+      <c r="BL32" s="9"/>
+      <c r="BM32" s="9"/>
+      <c r="BN32" s="9"/>
+      <c r="BO32" s="9"/>
+      <c r="BP32" s="9"/>
+      <c r="BQ32" s="9"/>
+    </row>
+    <row r="33" spans="1:102" s="10" customFormat="1">
+      <c r="A33" s="9"/>
+      <c r="B33" s="17"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="29"/>
+      <c r="R33" s="29"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="9"/>
+      <c r="X33" s="9"/>
+      <c r="Y33" s="9"/>
+      <c r="Z33" s="9"/>
+      <c r="AA33" s="9"/>
+      <c r="AB33" s="9"/>
+      <c r="AC33" s="9"/>
+      <c r="AD33" s="9"/>
+      <c r="AE33" s="9"/>
+      <c r="AF33" s="9"/>
+      <c r="AG33" s="9"/>
+      <c r="AH33" s="9"/>
+      <c r="AJ33" s="9"/>
+      <c r="AK33" s="9"/>
+      <c r="AL33" s="9"/>
+      <c r="AM33" s="9"/>
+      <c r="AN33" s="9"/>
+      <c r="AO33" s="9"/>
+      <c r="AP33" s="9"/>
+      <c r="AR33" s="9"/>
+      <c r="AT33" s="9"/>
+      <c r="AU33" s="9"/>
+      <c r="AV33" s="9"/>
+      <c r="AW33" s="9"/>
+      <c r="AX33" s="9"/>
+      <c r="BH33" s="9"/>
+      <c r="BJ33" s="9"/>
+      <c r="BK33" s="9"/>
+      <c r="BL33" s="9"/>
+      <c r="BM33" s="9"/>
+      <c r="BN33" s="9"/>
+      <c r="BO33" s="9"/>
+      <c r="BP33" s="9"/>
+      <c r="BQ33" s="9"/>
+    </row>
+    <row r="34" spans="1:102" s="25" customFormat="1">
+      <c r="A34" s="22"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+      <c r="U34" s="24"/>
+      <c r="V34" s="24"/>
+      <c r="W34" s="24"/>
+      <c r="X34" s="24"/>
+      <c r="Y34" s="24"/>
+      <c r="Z34" s="24"/>
+      <c r="AA34" s="24"/>
+      <c r="AB34" s="24"/>
+      <c r="AC34" s="24"/>
+      <c r="AD34" s="24"/>
+      <c r="AE34" s="24"/>
+      <c r="AF34" s="24"/>
+      <c r="AG34" s="24"/>
+      <c r="AH34" s="24"/>
+      <c r="AJ34" s="22"/>
+      <c r="AK34" s="22"/>
+      <c r="AL34" s="22"/>
+      <c r="AM34" s="22"/>
+      <c r="AN34" s="22"/>
+      <c r="AO34" s="24"/>
+      <c r="AP34" s="22"/>
+      <c r="AR34" s="22"/>
+      <c r="AS34" s="22"/>
+      <c r="AT34" s="24"/>
+      <c r="AU34" s="22"/>
+      <c r="AV34" s="22"/>
+      <c r="AW34" s="22"/>
+      <c r="AX34" s="22"/>
+      <c r="AY34" s="22"/>
+      <c r="AZ34" s="22"/>
+      <c r="BA34" s="22"/>
+      <c r="BB34" s="24"/>
+      <c r="BC34" s="24"/>
+      <c r="BD34" s="24"/>
+      <c r="BE34" s="22"/>
+      <c r="BF34" s="22"/>
+      <c r="BG34" s="22"/>
+      <c r="BH34" s="22"/>
+      <c r="BI34" s="22"/>
+      <c r="BJ34" s="22"/>
+      <c r="BK34" s="22"/>
+      <c r="BL34" s="22"/>
+      <c r="BM34" s="22"/>
+      <c r="BN34" s="22"/>
+      <c r="BO34" s="22"/>
+      <c r="BP34" s="24"/>
+      <c r="BQ34" s="24"/>
+    </row>
+    <row r="35" spans="1:102" s="25" customFormat="1">
+      <c r="A35" s="22"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+      <c r="U35" s="24"/>
+      <c r="V35" s="24"/>
+      <c r="W35" s="24"/>
+      <c r="X35" s="24"/>
+      <c r="Y35" s="24"/>
+      <c r="Z35" s="24"/>
+      <c r="AA35" s="24"/>
+      <c r="AB35" s="24"/>
+      <c r="AC35" s="24"/>
+      <c r="AD35" s="24"/>
+      <c r="AE35" s="24"/>
+      <c r="AF35" s="24"/>
+      <c r="AG35" s="24"/>
+      <c r="AH35" s="24"/>
+      <c r="AJ35" s="22"/>
+      <c r="AK35" s="22"/>
+      <c r="AL35" s="22"/>
+      <c r="AM35" s="22"/>
+      <c r="AN35" s="22"/>
+      <c r="AO35" s="24"/>
+      <c r="AP35" s="22"/>
+      <c r="AR35" s="22"/>
+      <c r="AS35" s="22"/>
+      <c r="AT35" s="24"/>
+      <c r="AU35" s="22"/>
+      <c r="AV35" s="22"/>
+      <c r="AW35" s="22"/>
+      <c r="AX35" s="22"/>
+      <c r="AY35" s="22"/>
+      <c r="AZ35" s="22"/>
+      <c r="BA35" s="22"/>
+      <c r="BB35" s="24"/>
+      <c r="BC35" s="24"/>
+      <c r="BD35" s="24"/>
+      <c r="BE35" s="22"/>
+      <c r="BF35" s="22"/>
+      <c r="BG35" s="22"/>
+      <c r="BH35" s="22"/>
+      <c r="BI35" s="22"/>
+      <c r="BJ35" s="22"/>
+      <c r="BK35" s="22"/>
+      <c r="BL35" s="22"/>
+      <c r="BM35" s="22"/>
+      <c r="BN35" s="22"/>
+      <c r="BO35" s="22"/>
+      <c r="BP35" s="24"/>
+      <c r="BQ35" s="24"/>
+    </row>
+    <row r="36" spans="1:102" s="25" customFormat="1">
+      <c r="A36" s="22"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="24"/>
+      <c r="V36" s="24"/>
+      <c r="W36" s="24"/>
+      <c r="X36" s="24"/>
+      <c r="Y36" s="24"/>
+      <c r="Z36" s="24"/>
+      <c r="AA36" s="24"/>
+      <c r="AB36" s="24"/>
+      <c r="AC36" s="24"/>
+      <c r="AD36" s="24"/>
+      <c r="AE36" s="24"/>
+      <c r="AF36" s="24"/>
+      <c r="AG36" s="24"/>
+      <c r="AH36" s="24"/>
+      <c r="AJ36" s="22"/>
+      <c r="AK36" s="22"/>
+      <c r="AL36" s="22"/>
+      <c r="AM36" s="22"/>
+      <c r="AN36" s="22"/>
+      <c r="AO36" s="24"/>
+      <c r="AP36" s="22"/>
+      <c r="AR36" s="22"/>
+      <c r="AS36" s="22"/>
+      <c r="AT36" s="24"/>
+      <c r="AU36" s="22"/>
+      <c r="AV36" s="22"/>
+      <c r="AW36" s="22"/>
+      <c r="AX36" s="22"/>
+      <c r="AY36" s="22"/>
+      <c r="AZ36" s="22"/>
+      <c r="BA36" s="22"/>
+      <c r="BB36" s="24"/>
+      <c r="BC36" s="24"/>
+      <c r="BD36" s="24"/>
+      <c r="BE36" s="22"/>
+      <c r="BF36" s="22"/>
+      <c r="BG36" s="22"/>
+      <c r="BH36" s="22"/>
+      <c r="BI36" s="22"/>
+      <c r="BJ36" s="22"/>
+      <c r="BK36" s="22"/>
+      <c r="BL36" s="22"/>
+      <c r="BM36" s="22"/>
+      <c r="BN36" s="22"/>
+      <c r="BO36" s="22"/>
+      <c r="BP36" s="24"/>
+      <c r="BQ36" s="24"/>
     </row>
     <row r="37" spans="1:102" s="10" customFormat="1">
       <c r="A37" s="9"/>
@@ -6643,7 +7032,7 @@
       <c r="BP42" s="9"/>
       <c r="BQ42" s="9"/>
     </row>
-    <row r="43" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="43" spans="1:102" s="10" customFormat="1">
       <c r="A43" s="9"/>
       <c r="B43" s="17"/>
       <c r="E43" s="9"/>
@@ -6694,7 +7083,7 @@
       <c r="BP43" s="9"/>
       <c r="BQ43" s="9"/>
     </row>
-    <row r="44" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="44" spans="1:102" s="10" customFormat="1">
       <c r="A44" s="9"/>
       <c r="B44" s="17"/>
       <c r="E44" s="9"/>
@@ -6745,7 +7134,7 @@
       <c r="BP44" s="9"/>
       <c r="BQ44" s="9"/>
     </row>
-    <row r="45" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="45" spans="1:102" s="10" customFormat="1">
       <c r="A45" s="9"/>
       <c r="B45" s="17"/>
       <c r="E45" s="9"/>
@@ -6796,7 +7185,7 @@
       <c r="BP45" s="9"/>
       <c r="BQ45" s="9"/>
     </row>
-    <row r="46" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="46" spans="1:102" s="10" customFormat="1">
       <c r="A46" s="9"/>
       <c r="B46" s="17"/>
       <c r="E46" s="9"/>
@@ -6847,7 +7236,7 @@
       <c r="BP46" s="9"/>
       <c r="BQ46" s="9"/>
     </row>
-    <row r="47" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="47" spans="1:102" s="10" customFormat="1">
       <c r="A47" s="9"/>
       <c r="B47" s="17"/>
       <c r="E47" s="9"/>
@@ -6898,7 +7287,7 @@
       <c r="BP47" s="9"/>
       <c r="BQ47" s="9"/>
     </row>
-    <row r="48" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="48" spans="1:102" s="10" customFormat="1">
       <c r="A48" s="9"/>
       <c r="B48" s="17"/>
       <c r="E48" s="9"/>
@@ -6949,7 +7338,7 @@
       <c r="BP48" s="9"/>
       <c r="BQ48" s="9"/>
     </row>
-    <row r="49" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="49" spans="1:102" s="10" customFormat="1">
       <c r="A49" s="9"/>
       <c r="B49" s="17"/>
       <c r="E49" s="9"/>
@@ -7000,7 +7389,7 @@
       <c r="BP49" s="9"/>
       <c r="BQ49" s="9"/>
     </row>
-    <row r="50" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="50" spans="1:102" s="10" customFormat="1">
       <c r="A50" s="9"/>
       <c r="B50" s="17"/>
       <c r="E50" s="9"/>
@@ -7051,7 +7440,7 @@
       <c r="BP50" s="9"/>
       <c r="BQ50" s="9"/>
     </row>
-    <row r="51" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="51" spans="1:102" s="10" customFormat="1">
       <c r="A51" s="9"/>
       <c r="B51" s="17"/>
       <c r="E51" s="9"/>
@@ -7102,7 +7491,7 @@
       <c r="BP51" s="9"/>
       <c r="BQ51" s="9"/>
     </row>
-    <row r="52" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="52" spans="1:102" s="10" customFormat="1">
       <c r="A52" s="9"/>
       <c r="B52" s="17"/>
       <c r="E52" s="9"/>
@@ -7153,7 +7542,7 @@
       <c r="BP52" s="9"/>
       <c r="BQ52" s="9"/>
     </row>
-    <row r="53" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="53" spans="1:102" s="10" customFormat="1">
       <c r="A53" s="9"/>
       <c r="B53" s="17"/>
       <c r="E53" s="9"/>
@@ -7204,7 +7593,7 @@
       <c r="BP53" s="9"/>
       <c r="BQ53" s="9"/>
     </row>
-    <row r="54" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="54" spans="1:102" s="10" customFormat="1">
       <c r="A54" s="9"/>
       <c r="B54" s="17"/>
       <c r="E54" s="9"/>
@@ -7255,7 +7644,7 @@
       <c r="BP54" s="9"/>
       <c r="BQ54" s="9"/>
     </row>
-    <row r="55" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="55" spans="1:102" s="10" customFormat="1">
       <c r="A55" s="9"/>
       <c r="B55" s="17"/>
       <c r="E55" s="9"/>
@@ -7306,7 +7695,7 @@
       <c r="BP55" s="9"/>
       <c r="BQ55" s="9"/>
     </row>
-    <row r="56" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="56" spans="1:102" s="10" customFormat="1">
       <c r="A56" s="9"/>
       <c r="B56" s="17"/>
       <c r="E56" s="9"/>
@@ -7357,7 +7746,7 @@
       <c r="BP56" s="9"/>
       <c r="BQ56" s="9"/>
     </row>
-    <row r="57" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="57" spans="1:102" s="10" customFormat="1">
       <c r="A57" s="9"/>
       <c r="B57" s="17"/>
       <c r="E57" s="9"/>
@@ -7408,7 +7797,7 @@
       <c r="BP57" s="9"/>
       <c r="BQ57" s="9"/>
     </row>
-    <row r="58" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="58" spans="1:102" s="10" customFormat="1">
       <c r="A58" s="9"/>
       <c r="B58" s="17"/>
       <c r="E58" s="9"/>
@@ -7459,7 +7848,7 @@
       <c r="BP58" s="9"/>
       <c r="BQ58" s="9"/>
     </row>
-    <row r="59" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="59" spans="1:102" s="10" customFormat="1">
       <c r="A59" s="9"/>
       <c r="B59" s="17"/>
       <c r="E59" s="9"/>
@@ -7510,7 +7899,7 @@
       <c r="BP59" s="9"/>
       <c r="BQ59" s="9"/>
     </row>
-    <row r="60" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="60" spans="1:102" s="10" customFormat="1">
       <c r="A60" s="9"/>
       <c r="B60" s="17"/>
       <c r="E60" s="9"/>
@@ -7561,7 +7950,7 @@
       <c r="BP60" s="9"/>
       <c r="BQ60" s="9"/>
     </row>
-    <row r="61" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="61" spans="1:102" s="10" customFormat="1">
       <c r="A61" s="9"/>
       <c r="B61" s="17"/>
       <c r="E61" s="9"/>
@@ -7612,7 +8001,7 @@
       <c r="BP61" s="9"/>
       <c r="BQ61" s="9"/>
     </row>
-    <row r="62" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="62" spans="1:102" s="10" customFormat="1">
       <c r="A62" s="9"/>
       <c r="B62" s="17"/>
       <c r="E62" s="9"/>
@@ -7663,7 +8052,7 @@
       <c r="BP62" s="9"/>
       <c r="BQ62" s="9"/>
     </row>
-    <row r="63" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="63" spans="1:102" s="10" customFormat="1">
       <c r="A63" s="9"/>
       <c r="B63" s="17"/>
       <c r="E63" s="9"/>
@@ -7714,7 +8103,7 @@
       <c r="BP63" s="9"/>
       <c r="BQ63" s="9"/>
     </row>
-    <row r="64" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="64" spans="1:102" s="10" customFormat="1">
       <c r="A64" s="9"/>
       <c r="B64" s="17"/>
       <c r="E64" s="9"/>
@@ -7765,7 +8154,7 @@
       <c r="BP64" s="9"/>
       <c r="BQ64" s="9"/>
     </row>
-    <row r="65" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="65" spans="1:102" s="10" customFormat="1">
       <c r="A65" s="9"/>
       <c r="B65" s="17"/>
       <c r="E65" s="9"/>
@@ -7816,7 +8205,7 @@
       <c r="BP65" s="9"/>
       <c r="BQ65" s="9"/>
     </row>
-    <row r="66" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="66" spans="1:102" s="10" customFormat="1">
       <c r="A66" s="9"/>
       <c r="B66" s="17"/>
       <c r="E66" s="9"/>
@@ -7867,7 +8256,7 @@
       <c r="BP66" s="9"/>
       <c r="BQ66" s="9"/>
     </row>
-    <row r="67" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="67" spans="1:102" s="10" customFormat="1">
       <c r="A67" s="9"/>
       <c r="B67" s="17"/>
       <c r="E67" s="9"/>
@@ -7918,7 +8307,7 @@
       <c r="BP67" s="9"/>
       <c r="BQ67" s="9"/>
     </row>
-    <row r="68" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="68" spans="1:102" s="10" customFormat="1">
       <c r="A68" s="9"/>
       <c r="B68" s="17"/>
       <c r="E68" s="9"/>
@@ -7969,7 +8358,7 @@
       <c r="BP68" s="9"/>
       <c r="BQ68" s="9"/>
     </row>
-    <row r="69" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="69" spans="1:102" s="10" customFormat="1">
       <c r="A69" s="9"/>
       <c r="B69" s="17"/>
       <c r="E69" s="9"/>
@@ -8020,7 +8409,7 @@
       <c r="BP69" s="9"/>
       <c r="BQ69" s="9"/>
     </row>
-    <row r="70" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="70" spans="1:102" s="10" customFormat="1">
       <c r="A70" s="9"/>
       <c r="B70" s="17"/>
       <c r="E70" s="9"/>
@@ -8071,7 +8460,7 @@
       <c r="BP70" s="9"/>
       <c r="BQ70" s="9"/>
     </row>
-    <row r="71" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="71" spans="1:102" s="10" customFormat="1">
       <c r="A71" s="9"/>
       <c r="B71" s="17"/>
       <c r="E71" s="9"/>
@@ -8122,7 +8511,7 @@
       <c r="BP71" s="9"/>
       <c r="BQ71" s="9"/>
     </row>
-    <row r="72" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="72" spans="1:102" s="10" customFormat="1">
       <c r="A72" s="9"/>
       <c r="B72" s="17"/>
       <c r="E72" s="9"/>
@@ -8173,7 +8562,7 @@
       <c r="BP72" s="9"/>
       <c r="BQ72" s="9"/>
     </row>
-    <row r="73" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="73" spans="1:102" s="10" customFormat="1">
       <c r="A73" s="9"/>
       <c r="B73" s="17"/>
       <c r="E73" s="9"/>
@@ -8224,7 +8613,7 @@
       <c r="BP73" s="9"/>
       <c r="BQ73" s="9"/>
     </row>
-    <row r="74" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="74" spans="1:102" s="10" customFormat="1">
       <c r="A74" s="9"/>
       <c r="B74" s="17"/>
       <c r="E74" s="9"/>
@@ -8275,7 +8664,7 @@
       <c r="BP74" s="9"/>
       <c r="BQ74" s="9"/>
     </row>
-    <row r="75" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="75" spans="1:102" s="10" customFormat="1">
       <c r="A75" s="9"/>
       <c r="B75" s="17"/>
       <c r="E75" s="9"/>
@@ -8326,7 +8715,7 @@
       <c r="BP75" s="9"/>
       <c r="BQ75" s="9"/>
     </row>
-    <row r="76" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="76" spans="1:102" s="10" customFormat="1">
       <c r="A76" s="9"/>
       <c r="B76" s="17"/>
       <c r="E76" s="9"/>
@@ -8377,7 +8766,7 @@
       <c r="BP76" s="9"/>
       <c r="BQ76" s="9"/>
     </row>
-    <row r="77" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="77" spans="1:102" s="10" customFormat="1">
       <c r="A77" s="9"/>
       <c r="B77" s="17"/>
       <c r="E77" s="9"/>
@@ -8428,7 +8817,7 @@
       <c r="BP77" s="9"/>
       <c r="BQ77" s="9"/>
     </row>
-    <row r="78" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="78" spans="1:102" s="10" customFormat="1">
       <c r="A78" s="9"/>
       <c r="B78" s="17"/>
       <c r="E78" s="9"/>
@@ -8479,7 +8868,7 @@
       <c r="BP78" s="9"/>
       <c r="BQ78" s="9"/>
     </row>
-    <row r="79" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="79" spans="1:102" s="10" customFormat="1">
       <c r="A79" s="9"/>
       <c r="B79" s="17"/>
       <c r="E79" s="9"/>
@@ -8530,7 +8919,7 @@
       <c r="BP79" s="9"/>
       <c r="BQ79" s="9"/>
     </row>
-    <row r="80" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="80" spans="1:102" s="10" customFormat="1">
       <c r="A80" s="9"/>
       <c r="B80" s="17"/>
       <c r="E80" s="9"/>
@@ -8581,7 +8970,7 @@
       <c r="BP80" s="9"/>
       <c r="BQ80" s="9"/>
     </row>
-    <row r="81" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="81" spans="1:102" s="10" customFormat="1">
       <c r="A81" s="9"/>
       <c r="B81" s="17"/>
       <c r="E81" s="9"/>
@@ -8632,7 +9021,7 @@
       <c r="BP81" s="9"/>
       <c r="BQ81" s="9"/>
     </row>
-    <row r="82" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="82" spans="1:102" s="10" customFormat="1">
       <c r="A82" s="9"/>
       <c r="B82" s="17"/>
       <c r="E82" s="9"/>
@@ -8683,7 +9072,7 @@
       <c r="BP82" s="9"/>
       <c r="BQ82" s="9"/>
     </row>
-    <row r="83" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="83" spans="1:102" s="10" customFormat="1">
       <c r="A83" s="9"/>
       <c r="B83" s="17"/>
       <c r="E83" s="9"/>
@@ -8734,7 +9123,7 @@
       <c r="BP83" s="9"/>
       <c r="BQ83" s="9"/>
     </row>
-    <row r="84" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="84" spans="1:102" s="10" customFormat="1">
       <c r="A84" s="9"/>
       <c r="B84" s="17"/>
       <c r="E84" s="9"/>
@@ -8785,7 +9174,7 @@
       <c r="BP84" s="9"/>
       <c r="BQ84" s="9"/>
     </row>
-    <row r="85" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="85" spans="1:102" s="10" customFormat="1">
       <c r="A85" s="9"/>
       <c r="B85" s="17"/>
       <c r="E85" s="9"/>
@@ -8836,7 +9225,7 @@
       <c r="BP85" s="9"/>
       <c r="BQ85" s="9"/>
     </row>
-    <row r="86" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="86" spans="1:102" s="10" customFormat="1">
       <c r="A86" s="9"/>
       <c r="B86" s="17"/>
       <c r="E86" s="9"/>
@@ -8887,7 +9276,7 @@
       <c r="BP86" s="9"/>
       <c r="BQ86" s="9"/>
     </row>
-    <row r="87" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="87" spans="1:102" s="10" customFormat="1">
       <c r="A87" s="9"/>
       <c r="B87" s="17"/>
       <c r="E87" s="9"/>
@@ -8938,7 +9327,7 @@
       <c r="BP87" s="9"/>
       <c r="BQ87" s="9"/>
     </row>
-    <row r="88" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="88" spans="1:102" s="10" customFormat="1">
       <c r="A88" s="9"/>
       <c r="B88" s="17"/>
       <c r="E88" s="9"/>
@@ -8989,7 +9378,7 @@
       <c r="BP88" s="9"/>
       <c r="BQ88" s="9"/>
     </row>
-    <row r="89" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="89" spans="1:102" s="10" customFormat="1">
       <c r="A89" s="9"/>
       <c r="B89" s="17"/>
       <c r="E89" s="9"/>
@@ -9040,7 +9429,7 @@
       <c r="BP89" s="9"/>
       <c r="BQ89" s="9"/>
     </row>
-    <row r="90" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="90" spans="1:102" s="10" customFormat="1">
       <c r="A90" s="9"/>
       <c r="B90" s="17"/>
       <c r="E90" s="9"/>
@@ -9091,7 +9480,7 @@
       <c r="BP90" s="9"/>
       <c r="BQ90" s="9"/>
     </row>
-    <row r="91" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="91" spans="1:102" s="10" customFormat="1">
       <c r="A91" s="9"/>
       <c r="B91" s="17"/>
       <c r="E91" s="9"/>
@@ -9142,7 +9531,7 @@
       <c r="BP91" s="9"/>
       <c r="BQ91" s="9"/>
     </row>
-    <row r="92" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="92" spans="1:102" s="10" customFormat="1">
       <c r="A92" s="9"/>
       <c r="B92" s="17"/>
       <c r="E92" s="9"/>
@@ -9193,7 +9582,7 @@
       <c r="BP92" s="9"/>
       <c r="BQ92" s="9"/>
     </row>
-    <row r="93" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="93" spans="1:102" s="10" customFormat="1">
       <c r="A93" s="9"/>
       <c r="B93" s="17"/>
       <c r="E93" s="9"/>
@@ -9244,7 +9633,7 @@
       <c r="BP93" s="9"/>
       <c r="BQ93" s="9"/>
     </row>
-    <row r="94" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="94" spans="1:102" s="10" customFormat="1">
       <c r="A94" s="9"/>
       <c r="B94" s="17"/>
       <c r="E94" s="9"/>
@@ -9295,7 +9684,7 @@
       <c r="BP94" s="9"/>
       <c r="BQ94" s="9"/>
     </row>
-    <row r="95" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="95" spans="1:102" s="10" customFormat="1">
       <c r="A95" s="9"/>
       <c r="B95" s="17"/>
       <c r="E95" s="9"/>
@@ -9346,7 +9735,7 @@
       <c r="BP95" s="9"/>
       <c r="BQ95" s="9"/>
     </row>
-    <row r="96" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="96" spans="1:102" s="10" customFormat="1">
       <c r="A96" s="9"/>
       <c r="B96" s="17"/>
       <c r="E96" s="9"/>
@@ -9397,7 +9786,7 @@
       <c r="BP96" s="9"/>
       <c r="BQ96" s="9"/>
     </row>
-    <row r="97" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="97" spans="1:102" s="10" customFormat="1">
       <c r="A97" s="9"/>
       <c r="B97" s="17"/>
       <c r="E97" s="9"/>
@@ -9448,7 +9837,7 @@
       <c r="BP97" s="9"/>
       <c r="BQ97" s="9"/>
     </row>
-    <row r="98" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="98" spans="1:102" s="10" customFormat="1">
       <c r="A98" s="9"/>
       <c r="B98" s="17"/>
       <c r="E98" s="9"/>
@@ -9499,7 +9888,7 @@
       <c r="BP98" s="9"/>
       <c r="BQ98" s="9"/>
     </row>
-    <row r="99" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="99" spans="1:102" s="10" customFormat="1">
       <c r="A99" s="9"/>
       <c r="B99" s="17"/>
       <c r="E99" s="9"/>
@@ -9550,7 +9939,7 @@
       <c r="BP99" s="9"/>
       <c r="BQ99" s="9"/>
     </row>
-    <row r="100" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="100" spans="1:102" s="10" customFormat="1">
       <c r="A100" s="9"/>
       <c r="B100" s="17"/>
       <c r="E100" s="9"/>
@@ -9601,7 +9990,7 @@
       <c r="BP100" s="9"/>
       <c r="BQ100" s="9"/>
     </row>
-    <row r="101" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="101" spans="1:102" s="10" customFormat="1">
       <c r="A101" s="9"/>
       <c r="B101" s="17"/>
       <c r="E101" s="9"/>
@@ -9652,7 +10041,7 @@
       <c r="BP101" s="9"/>
       <c r="BQ101" s="9"/>
     </row>
-    <row r="102" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="102" spans="1:102" s="10" customFormat="1">
       <c r="A102" s="9"/>
       <c r="B102" s="17"/>
       <c r="E102" s="9"/>
@@ -9703,7 +10092,7 @@
       <c r="BP102" s="9"/>
       <c r="BQ102" s="9"/>
     </row>
-    <row r="103" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="103" spans="1:102" s="10" customFormat="1">
       <c r="A103" s="9"/>
       <c r="B103" s="17"/>
       <c r="E103" s="9"/>
@@ -9754,7 +10143,7 @@
       <c r="BP103" s="9"/>
       <c r="BQ103" s="9"/>
     </row>
-    <row r="104" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="104" spans="1:102" s="10" customFormat="1">
       <c r="A104" s="9"/>
       <c r="B104" s="17"/>
       <c r="E104" s="9"/>
@@ -9805,7 +10194,7 @@
       <c r="BP104" s="9"/>
       <c r="BQ104" s="9"/>
     </row>
-    <row r="105" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="105" spans="1:102" s="10" customFormat="1">
       <c r="A105" s="9"/>
       <c r="B105" s="17"/>
       <c r="E105" s="9"/>
@@ -9856,7 +10245,7 @@
       <c r="BP105" s="9"/>
       <c r="BQ105" s="9"/>
     </row>
-    <row r="106" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="106" spans="1:102" s="10" customFormat="1">
       <c r="A106" s="9"/>
       <c r="B106" s="17"/>
       <c r="E106" s="9"/>
@@ -9907,7 +10296,7 @@
       <c r="BP106" s="9"/>
       <c r="BQ106" s="9"/>
     </row>
-    <row r="107" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="107" spans="1:102" s="10" customFormat="1">
       <c r="A107" s="9"/>
       <c r="B107" s="17"/>
       <c r="E107" s="9"/>
@@ -9958,7 +10347,7 @@
       <c r="BP107" s="9"/>
       <c r="BQ107" s="9"/>
     </row>
-    <row r="108" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="108" spans="1:102" s="10" customFormat="1">
       <c r="A108" s="9"/>
       <c r="B108" s="17"/>
       <c r="E108" s="9"/>
@@ -10009,7 +10398,7 @@
       <c r="BP108" s="9"/>
       <c r="BQ108" s="9"/>
     </row>
-    <row r="109" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="109" spans="1:102" s="10" customFormat="1">
       <c r="A109" s="9"/>
       <c r="B109" s="17"/>
       <c r="E109" s="9"/>
@@ -10060,7 +10449,7 @@
       <c r="BP109" s="9"/>
       <c r="BQ109" s="9"/>
     </row>
-    <row r="110" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="110" spans="1:102" s="10" customFormat="1">
       <c r="A110" s="9"/>
       <c r="B110" s="17"/>
       <c r="E110" s="9"/>
@@ -10111,7 +10500,7 @@
       <c r="BP110" s="9"/>
       <c r="BQ110" s="9"/>
     </row>
-    <row r="111" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="111" spans="1:102" s="10" customFormat="1">
       <c r="A111" s="9"/>
       <c r="B111" s="17"/>
       <c r="E111" s="9"/>
@@ -10162,7 +10551,7 @@
       <c r="BP111" s="9"/>
       <c r="BQ111" s="9"/>
     </row>
-    <row r="112" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="112" spans="1:102" s="10" customFormat="1">
       <c r="A112" s="9"/>
       <c r="B112" s="17"/>
       <c r="E112" s="9"/>
@@ -10213,7 +10602,7 @@
       <c r="BP112" s="9"/>
       <c r="BQ112" s="9"/>
     </row>
-    <row r="113" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="113" spans="1:102" s="10" customFormat="1">
       <c r="A113" s="9"/>
       <c r="B113" s="17"/>
       <c r="E113" s="9"/>
@@ -10264,7 +10653,7 @@
       <c r="BP113" s="9"/>
       <c r="BQ113" s="9"/>
     </row>
-    <row r="114" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="114" spans="1:102" s="10" customFormat="1">
       <c r="A114" s="9"/>
       <c r="B114" s="17"/>
       <c r="E114" s="9"/>
@@ -10315,7 +10704,7 @@
       <c r="BP114" s="9"/>
       <c r="BQ114" s="9"/>
     </row>
-    <row r="115" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="115" spans="1:102" s="10" customFormat="1">
       <c r="A115" s="9"/>
       <c r="B115" s="17"/>
       <c r="E115" s="9"/>
@@ -10366,7 +10755,7 @@
       <c r="BP115" s="9"/>
       <c r="BQ115" s="9"/>
     </row>
-    <row r="116" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="116" spans="1:102" s="10" customFormat="1">
       <c r="A116" s="9"/>
       <c r="B116" s="17"/>
       <c r="E116" s="9"/>
@@ -10417,7 +10806,7 @@
       <c r="BP116" s="9"/>
       <c r="BQ116" s="9"/>
     </row>
-    <row r="117" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="117" spans="1:102" s="10" customFormat="1">
       <c r="A117" s="9"/>
       <c r="B117" s="17"/>
       <c r="E117" s="9"/>
@@ -10468,7 +10857,7 @@
       <c r="BP117" s="9"/>
       <c r="BQ117" s="9"/>
     </row>
-    <row r="118" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="118" spans="1:102" s="10" customFormat="1">
       <c r="A118" s="9"/>
       <c r="B118" s="17"/>
       <c r="E118" s="9"/>
@@ -10519,7 +10908,7 @@
       <c r="BP118" s="9"/>
       <c r="BQ118" s="9"/>
     </row>
-    <row r="119" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="119" spans="1:102" s="10" customFormat="1">
       <c r="A119" s="9"/>
       <c r="B119" s="17"/>
       <c r="E119" s="9"/>
@@ -10570,7 +10959,7 @@
       <c r="BP119" s="9"/>
       <c r="BQ119" s="9"/>
     </row>
-    <row r="120" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="120" spans="1:102" s="10" customFormat="1">
       <c r="A120" s="9"/>
       <c r="B120" s="17"/>
       <c r="E120" s="9"/>
@@ -10621,7 +11010,7 @@
       <c r="BP120" s="9"/>
       <c r="BQ120" s="9"/>
     </row>
-    <row r="121" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="121" spans="1:102" s="10" customFormat="1">
       <c r="A121" s="9"/>
       <c r="B121" s="17"/>
       <c r="E121" s="9"/>
@@ -10672,7 +11061,7 @@
       <c r="BP121" s="9"/>
       <c r="BQ121" s="9"/>
     </row>
-    <row r="122" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="122" spans="1:102" s="10" customFormat="1">
       <c r="A122" s="9"/>
       <c r="B122" s="17"/>
       <c r="E122" s="9"/>
@@ -10723,7 +11112,7 @@
       <c r="BP122" s="9"/>
       <c r="BQ122" s="9"/>
     </row>
-    <row r="123" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="123" spans="1:102" s="10" customFormat="1">
       <c r="A123" s="9"/>
       <c r="B123" s="17"/>
       <c r="E123" s="9"/>
@@ -10774,7 +11163,7 @@
       <c r="BP123" s="9"/>
       <c r="BQ123" s="9"/>
     </row>
-    <row r="124" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="124" spans="1:102" s="10" customFormat="1">
       <c r="A124" s="9"/>
       <c r="B124" s="17"/>
       <c r="E124" s="9"/>
@@ -10825,7 +11214,7 @@
       <c r="BP124" s="9"/>
       <c r="BQ124" s="9"/>
     </row>
-    <row r="125" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="125" spans="1:102" s="10" customFormat="1">
       <c r="A125" s="9"/>
       <c r="B125" s="17"/>
       <c r="E125" s="9"/>
@@ -10876,7 +11265,7 @@
       <c r="BP125" s="9"/>
       <c r="BQ125" s="9"/>
     </row>
-    <row r="126" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="126" spans="1:102" s="10" customFormat="1">
       <c r="A126" s="9"/>
       <c r="B126" s="17"/>
       <c r="E126" s="9"/>
@@ -10927,7 +11316,7 @@
       <c r="BP126" s="9"/>
       <c r="BQ126" s="9"/>
     </row>
-    <row r="127" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="127" spans="1:102" s="10" customFormat="1">
       <c r="A127" s="9"/>
       <c r="B127" s="17"/>
       <c r="E127" s="9"/>
@@ -10978,7 +11367,7 @@
       <c r="BP127" s="9"/>
       <c r="BQ127" s="9"/>
     </row>
-    <row r="128" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="128" spans="1:102" s="10" customFormat="1">
       <c r="A128" s="9"/>
       <c r="B128" s="17"/>
       <c r="E128" s="9"/>
@@ -11029,7 +11418,7 @@
       <c r="BP128" s="9"/>
       <c r="BQ128" s="9"/>
     </row>
-    <row r="129" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="129" spans="1:102" s="10" customFormat="1">
       <c r="A129" s="9"/>
       <c r="B129" s="17"/>
       <c r="E129" s="9"/>
@@ -11080,7 +11469,7 @@
       <c r="BP129" s="9"/>
       <c r="BQ129" s="9"/>
     </row>
-    <row r="130" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="130" spans="1:102" s="10" customFormat="1">
       <c r="A130" s="9"/>
       <c r="B130" s="17"/>
       <c r="E130" s="9"/>
@@ -11131,7 +11520,7 @@
       <c r="BP130" s="9"/>
       <c r="BQ130" s="9"/>
     </row>
-    <row r="131" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="131" spans="1:102" s="10" customFormat="1">
       <c r="A131" s="9"/>
       <c r="B131" s="17"/>
       <c r="E131" s="9"/>
@@ -11182,7 +11571,7 @@
       <c r="BP131" s="9"/>
       <c r="BQ131" s="9"/>
     </row>
-    <row r="132" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="132" spans="1:102" s="10" customFormat="1">
       <c r="A132" s="9"/>
       <c r="B132" s="17"/>
       <c r="E132" s="9"/>
@@ -11233,7 +11622,7 @@
       <c r="BP132" s="9"/>
       <c r="BQ132" s="9"/>
     </row>
-    <row r="133" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="133" spans="1:102" s="10" customFormat="1">
       <c r="A133" s="9"/>
       <c r="B133" s="17"/>
       <c r="E133" s="9"/>
@@ -11284,7 +11673,7 @@
       <c r="BP133" s="9"/>
       <c r="BQ133" s="9"/>
     </row>
-    <row r="134" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="134" spans="1:102" s="10" customFormat="1">
       <c r="A134" s="9"/>
       <c r="B134" s="17"/>
       <c r="E134" s="9"/>
@@ -11335,7 +11724,7 @@
       <c r="BP134" s="9"/>
       <c r="BQ134" s="9"/>
     </row>
-    <row r="135" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="135" spans="1:102" s="10" customFormat="1">
       <c r="A135" s="9"/>
       <c r="B135" s="17"/>
       <c r="E135" s="9"/>
@@ -11386,7 +11775,7 @@
       <c r="BP135" s="9"/>
       <c r="BQ135" s="9"/>
     </row>
-    <row r="136" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="136" spans="1:102" s="10" customFormat="1">
       <c r="A136" s="9"/>
       <c r="B136" s="17"/>
       <c r="E136" s="9"/>
@@ -11437,7 +11826,7 @@
       <c r="BP136" s="9"/>
       <c r="BQ136" s="9"/>
     </row>
-    <row r="137" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="137" spans="1:102" s="10" customFormat="1">
       <c r="A137" s="9"/>
       <c r="B137" s="17"/>
       <c r="E137" s="9"/>
@@ -11488,7 +11877,7 @@
       <c r="BP137" s="9"/>
       <c r="BQ137" s="9"/>
     </row>
-    <row r="138" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="138" spans="1:102" s="10" customFormat="1">
       <c r="A138" s="9"/>
       <c r="B138" s="17"/>
       <c r="E138" s="9"/>
@@ -11539,7 +11928,7 @@
       <c r="BP138" s="9"/>
       <c r="BQ138" s="9"/>
     </row>
-    <row r="139" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="139" spans="1:102" s="10" customFormat="1">
       <c r="A139" s="9"/>
       <c r="B139" s="17"/>
       <c r="E139" s="9"/>
@@ -11590,7 +11979,7 @@
       <c r="BP139" s="9"/>
       <c r="BQ139" s="9"/>
     </row>
-    <row r="140" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="140" spans="1:102" s="10" customFormat="1">
       <c r="A140" s="9"/>
       <c r="B140" s="17"/>
       <c r="E140" s="9"/>
@@ -11641,7 +12030,7 @@
       <c r="BP140" s="9"/>
       <c r="BQ140" s="9"/>
     </row>
-    <row r="141" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="141" spans="1:102" s="10" customFormat="1">
       <c r="A141" s="9"/>
       <c r="B141" s="17"/>
       <c r="E141" s="9"/>
@@ -11692,7 +12081,7 @@
       <c r="BP141" s="9"/>
       <c r="BQ141" s="9"/>
     </row>
-    <row r="142" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="142" spans="1:102" s="10" customFormat="1">
       <c r="A142" s="9"/>
       <c r="B142" s="17"/>
       <c r="E142" s="9"/>
@@ -11743,7 +12132,7 @@
       <c r="BP142" s="9"/>
       <c r="BQ142" s="9"/>
     </row>
-    <row r="143" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="143" spans="1:102" s="10" customFormat="1">
       <c r="A143" s="9"/>
       <c r="B143" s="17"/>
       <c r="E143" s="9"/>
@@ -11794,7 +12183,7 @@
       <c r="BP143" s="9"/>
       <c r="BQ143" s="9"/>
     </row>
-    <row r="144" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="144" spans="1:102" s="10" customFormat="1">
       <c r="A144" s="9"/>
       <c r="B144" s="17"/>
       <c r="E144" s="9"/>
@@ -11845,7 +12234,7 @@
       <c r="BP144" s="9"/>
       <c r="BQ144" s="9"/>
     </row>
-    <row r="145" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="145" spans="1:102" s="10" customFormat="1">
       <c r="A145" s="9"/>
       <c r="B145" s="17"/>
       <c r="E145" s="9"/>
@@ -11896,7 +12285,7 @@
       <c r="BP145" s="9"/>
       <c r="BQ145" s="9"/>
     </row>
-    <row r="146" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="146" spans="1:102" s="10" customFormat="1">
       <c r="A146" s="9"/>
       <c r="B146" s="17"/>
       <c r="E146" s="9"/>
@@ -11947,7 +12336,7 @@
       <c r="BP146" s="9"/>
       <c r="BQ146" s="9"/>
     </row>
-    <row r="147" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="147" spans="1:102" s="10" customFormat="1">
       <c r="A147" s="9"/>
       <c r="B147" s="17"/>
       <c r="E147" s="9"/>
@@ -11998,7 +12387,7 @@
       <c r="BP147" s="9"/>
       <c r="BQ147" s="9"/>
     </row>
-    <row r="148" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="148" spans="1:102" s="10" customFormat="1">
       <c r="A148" s="9"/>
       <c r="B148" s="17"/>
       <c r="E148" s="9"/>
@@ -12049,7 +12438,7 @@
       <c r="BP148" s="9"/>
       <c r="BQ148" s="9"/>
     </row>
-    <row r="149" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="149" spans="1:102" s="10" customFormat="1">
       <c r="A149" s="9"/>
       <c r="B149" s="17"/>
       <c r="E149" s="9"/>
@@ -12100,7 +12489,7 @@
       <c r="BP149" s="9"/>
       <c r="BQ149" s="9"/>
     </row>
-    <row r="150" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="150" spans="1:102" s="10" customFormat="1">
       <c r="A150" s="9"/>
       <c r="B150" s="17"/>
       <c r="E150" s="9"/>
@@ -12151,7 +12540,7 @@
       <c r="BP150" s="9"/>
       <c r="BQ150" s="9"/>
     </row>
-    <row r="151" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="151" spans="1:102" s="10" customFormat="1">
       <c r="A151" s="9"/>
       <c r="B151" s="17"/>
       <c r="E151" s="9"/>
@@ -12202,7 +12591,7 @@
       <c r="BP151" s="9"/>
       <c r="BQ151" s="9"/>
     </row>
-    <row r="152" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="152" spans="1:102" s="10" customFormat="1">
       <c r="A152" s="9"/>
       <c r="B152" s="17"/>
       <c r="E152" s="9"/>
@@ -12253,7 +12642,7 @@
       <c r="BP152" s="9"/>
       <c r="BQ152" s="9"/>
     </row>
-    <row r="153" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="153" spans="1:102" s="10" customFormat="1">
       <c r="A153" s="9"/>
       <c r="B153" s="17"/>
       <c r="E153" s="9"/>
@@ -12304,7 +12693,7 @@
       <c r="BP153" s="9"/>
       <c r="BQ153" s="9"/>
     </row>
-    <row r="154" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="154" spans="1:102" s="10" customFormat="1">
       <c r="A154" s="9"/>
       <c r="B154" s="17"/>
       <c r="E154" s="9"/>
@@ -12355,7 +12744,7 @@
       <c r="BP154" s="9"/>
       <c r="BQ154" s="9"/>
     </row>
-    <row r="155" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="155" spans="1:102" s="10" customFormat="1">
       <c r="A155" s="9"/>
       <c r="B155" s="17"/>
       <c r="E155" s="9"/>
@@ -12406,7 +12795,7 @@
       <c r="BP155" s="9"/>
       <c r="BQ155" s="9"/>
     </row>
-    <row r="156" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="156" spans="1:102" s="10" customFormat="1">
       <c r="A156" s="9"/>
       <c r="B156" s="17"/>
       <c r="E156" s="9"/>
@@ -12457,7 +12846,7 @@
       <c r="BP156" s="9"/>
       <c r="BQ156" s="9"/>
     </row>
-    <row r="157" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="157" spans="1:102" s="10" customFormat="1">
       <c r="A157" s="9"/>
       <c r="B157" s="17"/>
       <c r="E157" s="9"/>
@@ -12508,7 +12897,7 @@
       <c r="BP157" s="9"/>
       <c r="BQ157" s="9"/>
     </row>
-    <row r="158" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="158" spans="1:102" s="10" customFormat="1">
       <c r="A158" s="9"/>
       <c r="B158" s="17"/>
       <c r="E158" s="9"/>
@@ -12559,7 +12948,7 @@
       <c r="BP158" s="9"/>
       <c r="BQ158" s="9"/>
     </row>
-    <row r="159" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="159" spans="1:102" s="10" customFormat="1">
       <c r="A159" s="9"/>
       <c r="B159" s="17"/>
       <c r="E159" s="9"/>
@@ -12610,7 +12999,7 @@
       <c r="BP159" s="9"/>
       <c r="BQ159" s="9"/>
     </row>
-    <row r="160" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="160" spans="1:102" s="10" customFormat="1">
       <c r="A160" s="9"/>
       <c r="B160" s="17"/>
       <c r="E160" s="9"/>
@@ -12661,7 +13050,7 @@
       <c r="BP160" s="9"/>
       <c r="BQ160" s="9"/>
     </row>
-    <row r="161" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="161" spans="1:102" s="10" customFormat="1">
       <c r="A161" s="9"/>
       <c r="B161" s="17"/>
       <c r="E161" s="9"/>
@@ -12712,7 +13101,7 @@
       <c r="BP161" s="9"/>
       <c r="BQ161" s="9"/>
     </row>
-    <row r="162" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="162" spans="1:102" s="10" customFormat="1">
       <c r="A162" s="9"/>
       <c r="B162" s="17"/>
       <c r="E162" s="9"/>
@@ -12763,7 +13152,7 @@
       <c r="BP162" s="9"/>
       <c r="BQ162" s="9"/>
     </row>
-    <row r="163" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="163" spans="1:102" s="10" customFormat="1">
       <c r="A163" s="9"/>
       <c r="B163" s="17"/>
       <c r="E163" s="9"/>
@@ -12814,7 +13203,7 @@
       <c r="BP163" s="9"/>
       <c r="BQ163" s="9"/>
     </row>
-    <row r="164" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="164" spans="1:102" s="10" customFormat="1">
       <c r="A164" s="9"/>
       <c r="B164" s="17"/>
       <c r="E164" s="9"/>
@@ -12865,7 +13254,7 @@
       <c r="BP164" s="9"/>
       <c r="BQ164" s="9"/>
     </row>
-    <row r="165" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="165" spans="1:102" s="10" customFormat="1">
       <c r="A165" s="9"/>
       <c r="B165" s="17"/>
       <c r="E165" s="9"/>
@@ -12916,7 +13305,7 @@
       <c r="BP165" s="9"/>
       <c r="BQ165" s="9"/>
     </row>
-    <row r="166" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="166" spans="1:102" s="10" customFormat="1">
       <c r="A166" s="9"/>
       <c r="B166" s="17"/>
       <c r="E166" s="9"/>
@@ -12967,7 +13356,7 @@
       <c r="BP166" s="9"/>
       <c r="BQ166" s="9"/>
     </row>
-    <row r="167" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="167" spans="1:102" s="10" customFormat="1">
       <c r="A167" s="9"/>
       <c r="B167" s="17"/>
       <c r="E167" s="9"/>
@@ -13018,7 +13407,7 @@
       <c r="BP167" s="9"/>
       <c r="BQ167" s="9"/>
     </row>
-    <row r="168" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="168" spans="1:102" s="10" customFormat="1">
       <c r="A168" s="9"/>
       <c r="B168" s="17"/>
       <c r="E168" s="9"/>
@@ -13069,7 +13458,7 @@
       <c r="BP168" s="9"/>
       <c r="BQ168" s="9"/>
     </row>
-    <row r="169" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="169" spans="1:102" s="10" customFormat="1">
       <c r="A169" s="9"/>
       <c r="B169" s="17"/>
       <c r="E169" s="9"/>
@@ -13120,7 +13509,7 @@
       <c r="BP169" s="9"/>
       <c r="BQ169" s="9"/>
     </row>
-    <row r="170" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="170" spans="1:102" s="10" customFormat="1">
       <c r="A170" s="9"/>
       <c r="B170" s="17"/>
       <c r="E170" s="9"/>
@@ -13171,7 +13560,7 @@
       <c r="BP170" s="9"/>
       <c r="BQ170" s="9"/>
     </row>
-    <row r="171" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="171" spans="1:102" s="10" customFormat="1">
       <c r="A171" s="9"/>
       <c r="B171" s="17"/>
       <c r="E171" s="9"/>
@@ -13222,7 +13611,7 @@
       <c r="BP171" s="9"/>
       <c r="BQ171" s="9"/>
     </row>
-    <row r="172" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="172" spans="1:102" s="10" customFormat="1">
       <c r="A172" s="9"/>
       <c r="B172" s="17"/>
       <c r="E172" s="9"/>
@@ -13273,7 +13662,7 @@
       <c r="BP172" s="9"/>
       <c r="BQ172" s="9"/>
     </row>
-    <row r="173" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="173" spans="1:102" s="10" customFormat="1">
       <c r="A173" s="9"/>
       <c r="B173" s="17"/>
       <c r="E173" s="9"/>
@@ -13324,7 +13713,7 @@
       <c r="BP173" s="9"/>
       <c r="BQ173" s="9"/>
     </row>
-    <row r="174" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="174" spans="1:102" s="10" customFormat="1">
       <c r="A174" s="9"/>
       <c r="B174" s="17"/>
       <c r="E174" s="9"/>
@@ -13375,7 +13764,7 @@
       <c r="BP174" s="9"/>
       <c r="BQ174" s="9"/>
     </row>
-    <row r="175" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="175" spans="1:102" s="10" customFormat="1">
       <c r="A175" s="9"/>
       <c r="B175" s="17"/>
       <c r="E175" s="9"/>
@@ -13426,7 +13815,7 @@
       <c r="BP175" s="9"/>
       <c r="BQ175" s="9"/>
     </row>
-    <row r="176" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="176" spans="1:102" s="10" customFormat="1">
       <c r="A176" s="9"/>
       <c r="B176" s="17"/>
       <c r="E176" s="9"/>
@@ -13477,7 +13866,7 @@
       <c r="BP176" s="9"/>
       <c r="BQ176" s="9"/>
     </row>
-    <row r="177" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="177" spans="1:102" s="10" customFormat="1">
       <c r="A177" s="9"/>
       <c r="B177" s="17"/>
       <c r="E177" s="9"/>
@@ -13528,7 +13917,7 @@
       <c r="BP177" s="9"/>
       <c r="BQ177" s="9"/>
     </row>
-    <row r="178" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="178" spans="1:102" s="10" customFormat="1">
       <c r="A178" s="9"/>
       <c r="B178" s="17"/>
       <c r="E178" s="9"/>
@@ -13579,7 +13968,7 @@
       <c r="BP178" s="9"/>
       <c r="BQ178" s="9"/>
     </row>
-    <row r="179" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="179" spans="1:102" s="10" customFormat="1">
       <c r="A179" s="9"/>
       <c r="B179" s="17"/>
       <c r="E179" s="9"/>
@@ -13630,7 +14019,7 @@
       <c r="BP179" s="9"/>
       <c r="BQ179" s="9"/>
     </row>
-    <row r="180" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="180" spans="1:102" s="10" customFormat="1">
       <c r="A180" s="9"/>
       <c r="B180" s="17"/>
       <c r="E180" s="9"/>
@@ -13681,7 +14070,7 @@
       <c r="BP180" s="9"/>
       <c r="BQ180" s="9"/>
     </row>
-    <row r="181" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="181" spans="1:102" s="10" customFormat="1">
       <c r="A181" s="9"/>
       <c r="B181" s="17"/>
       <c r="E181" s="9"/>
@@ -13732,7 +14121,7 @@
       <c r="BP181" s="9"/>
       <c r="BQ181" s="9"/>
     </row>
-    <row r="182" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="182" spans="1:102" s="10" customFormat="1">
       <c r="A182" s="9"/>
       <c r="B182" s="17"/>
       <c r="E182" s="9"/>
@@ -13783,7 +14172,7 @@
       <c r="BP182" s="9"/>
       <c r="BQ182" s="9"/>
     </row>
-    <row r="183" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="183" spans="1:102" s="10" customFormat="1">
       <c r="A183" s="9"/>
       <c r="B183" s="17"/>
       <c r="E183" s="9"/>
@@ -13834,7 +14223,7 @@
       <c r="BP183" s="9"/>
       <c r="BQ183" s="9"/>
     </row>
-    <row r="184" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="184" spans="1:102" s="10" customFormat="1">
       <c r="A184" s="9"/>
       <c r="B184" s="17"/>
       <c r="E184" s="9"/>
@@ -13885,7 +14274,7 @@
       <c r="BP184" s="9"/>
       <c r="BQ184" s="9"/>
     </row>
-    <row r="185" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="185" spans="1:102" s="10" customFormat="1">
       <c r="A185" s="9"/>
       <c r="B185" s="17"/>
       <c r="E185" s="9"/>
@@ -13936,7 +14325,7 @@
       <c r="BP185" s="9"/>
       <c r="BQ185" s="9"/>
     </row>
-    <row r="186" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="186" spans="1:102" s="10" customFormat="1">
       <c r="A186" s="9"/>
       <c r="B186" s="17"/>
       <c r="E186" s="9"/>
@@ -13987,7 +14376,7 @@
       <c r="BP186" s="9"/>
       <c r="BQ186" s="9"/>
     </row>
-    <row r="187" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="187" spans="1:102" s="10" customFormat="1">
       <c r="A187" s="9"/>
       <c r="B187" s="17"/>
       <c r="E187" s="9"/>
@@ -14038,7 +14427,7 @@
       <c r="BP187" s="9"/>
       <c r="BQ187" s="9"/>
     </row>
-    <row r="188" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="188" spans="1:102" s="10" customFormat="1">
       <c r="A188" s="9"/>
       <c r="B188" s="17"/>
       <c r="E188" s="9"/>
@@ -14089,7 +14478,7 @@
       <c r="BP188" s="9"/>
       <c r="BQ188" s="9"/>
     </row>
-    <row r="189" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="189" spans="1:102" s="10" customFormat="1">
       <c r="A189" s="9"/>
       <c r="B189" s="17"/>
       <c r="E189" s="9"/>
@@ -14140,7 +14529,7 @@
       <c r="BP189" s="9"/>
       <c r="BQ189" s="9"/>
     </row>
-    <row r="190" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="190" spans="1:102" s="10" customFormat="1">
       <c r="A190" s="9"/>
       <c r="B190" s="17"/>
       <c r="E190" s="9"/>
@@ -14191,7 +14580,7 @@
       <c r="BP190" s="9"/>
       <c r="BQ190" s="9"/>
     </row>
-    <row r="191" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="191" spans="1:102" s="10" customFormat="1">
       <c r="A191" s="9"/>
       <c r="B191" s="17"/>
       <c r="E191" s="9"/>
@@ -14242,7 +14631,7 @@
       <c r="BP191" s="9"/>
       <c r="BQ191" s="9"/>
     </row>
-    <row r="192" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="192" spans="1:102" s="10" customFormat="1">
       <c r="A192" s="9"/>
       <c r="B192" s="17"/>
       <c r="E192" s="9"/>
@@ -14293,7 +14682,7 @@
       <c r="BP192" s="9"/>
       <c r="BQ192" s="9"/>
     </row>
-    <row r="193" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="193" spans="1:102" s="10" customFormat="1">
       <c r="A193" s="9"/>
       <c r="B193" s="17"/>
       <c r="E193" s="9"/>
@@ -14344,7 +14733,7 @@
       <c r="BP193" s="9"/>
       <c r="BQ193" s="9"/>
     </row>
-    <row r="194" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="194" spans="1:102" s="10" customFormat="1">
       <c r="A194" s="9"/>
       <c r="B194" s="17"/>
       <c r="E194" s="9"/>
@@ -14395,7 +14784,7 @@
       <c r="BP194" s="9"/>
       <c r="BQ194" s="9"/>
     </row>
-    <row r="195" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="195" spans="1:102" s="10" customFormat="1">
       <c r="A195" s="9"/>
       <c r="B195" s="17"/>
       <c r="E195" s="9"/>
@@ -14446,7 +14835,7 @@
       <c r="BP195" s="9"/>
       <c r="BQ195" s="9"/>
     </row>
-    <row r="196" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="196" spans="1:102" s="10" customFormat="1">
       <c r="A196" s="9"/>
       <c r="B196" s="17"/>
       <c r="E196" s="9"/>
@@ -14497,7 +14886,7 @@
       <c r="BP196" s="9"/>
       <c r="BQ196" s="9"/>
     </row>
-    <row r="197" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="197" spans="1:102" s="10" customFormat="1">
       <c r="A197" s="9"/>
       <c r="B197" s="17"/>
       <c r="E197" s="9"/>
@@ -14548,7 +14937,7 @@
       <c r="BP197" s="9"/>
       <c r="BQ197" s="9"/>
     </row>
-    <row r="198" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="198" spans="1:102" s="10" customFormat="1">
       <c r="A198" s="9"/>
       <c r="B198" s="17"/>
       <c r="E198" s="9"/>
@@ -14599,7 +14988,7 @@
       <c r="BP198" s="9"/>
       <c r="BQ198" s="9"/>
     </row>
-    <row r="199" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="199" spans="1:102" s="10" customFormat="1">
       <c r="A199" s="9"/>
       <c r="B199" s="17"/>
       <c r="E199" s="9"/>
@@ -14650,7 +15039,7 @@
       <c r="BP199" s="9"/>
       <c r="BQ199" s="9"/>
     </row>
-    <row r="200" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="200" spans="1:102" s="10" customFormat="1">
       <c r="A200" s="9"/>
       <c r="B200" s="17"/>
       <c r="E200" s="9"/>
@@ -14701,7 +15090,7 @@
       <c r="BP200" s="9"/>
       <c r="BQ200" s="9"/>
     </row>
-    <row r="201" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="201" spans="1:102" s="10" customFormat="1">
       <c r="A201" s="9"/>
       <c r="B201" s="17"/>
       <c r="E201" s="9"/>
@@ -14752,7 +15141,7 @@
       <c r="BP201" s="9"/>
       <c r="BQ201" s="9"/>
     </row>
-    <row r="202" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="202" spans="1:102" s="10" customFormat="1">
       <c r="A202" s="9"/>
       <c r="B202" s="17"/>
       <c r="E202" s="9"/>
@@ -14803,7 +15192,7 @@
       <c r="BP202" s="9"/>
       <c r="BQ202" s="9"/>
     </row>
-    <row r="203" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="203" spans="1:102" s="10" customFormat="1">
       <c r="A203" s="9"/>
       <c r="B203" s="17"/>
       <c r="E203" s="9"/>
@@ -14854,7 +15243,7 @@
       <c r="BP203" s="9"/>
       <c r="BQ203" s="9"/>
     </row>
-    <row r="204" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="204" spans="1:102" s="10" customFormat="1">
       <c r="A204" s="9"/>
       <c r="B204" s="17"/>
       <c r="E204" s="9"/>
@@ -14905,7 +15294,7 @@
       <c r="BP204" s="9"/>
       <c r="BQ204" s="9"/>
     </row>
-    <row r="205" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="205" spans="1:102" s="10" customFormat="1">
       <c r="A205" s="9"/>
       <c r="B205" s="17"/>
       <c r="E205" s="9"/>
@@ -14956,7 +15345,7 @@
       <c r="BP205" s="9"/>
       <c r="BQ205" s="9"/>
     </row>
-    <row r="206" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="206" spans="1:102" s="10" customFormat="1">
       <c r="A206" s="9"/>
       <c r="B206" s="17"/>
       <c r="E206" s="9"/>
@@ -15007,7 +15396,7 @@
       <c r="BP206" s="9"/>
       <c r="BQ206" s="9"/>
     </row>
-    <row r="207" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="207" spans="1:102" s="10" customFormat="1">
       <c r="A207" s="9"/>
       <c r="B207" s="17"/>
       <c r="E207" s="9"/>
@@ -15058,7 +15447,7 @@
       <c r="BP207" s="9"/>
       <c r="BQ207" s="9"/>
     </row>
-    <row r="208" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="208" spans="1:102" s="10" customFormat="1">
       <c r="A208" s="9"/>
       <c r="B208" s="17"/>
       <c r="E208" s="9"/>
@@ -15109,7 +15498,7 @@
       <c r="BP208" s="9"/>
       <c r="BQ208" s="9"/>
     </row>
-    <row r="209" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="209" spans="1:102" s="10" customFormat="1">
       <c r="A209" s="9"/>
       <c r="B209" s="17"/>
       <c r="E209" s="9"/>
@@ -15160,7 +15549,7 @@
       <c r="BP209" s="9"/>
       <c r="BQ209" s="9"/>
     </row>
-    <row r="210" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="210" spans="1:102" s="10" customFormat="1">
       <c r="A210" s="9"/>
       <c r="B210" s="17"/>
       <c r="E210" s="9"/>
@@ -15211,7 +15600,7 @@
       <c r="BP210" s="9"/>
       <c r="BQ210" s="9"/>
     </row>
-    <row r="211" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="211" spans="1:102" s="10" customFormat="1">
       <c r="A211" s="9"/>
       <c r="B211" s="17"/>
       <c r="E211" s="9"/>
@@ -15262,7 +15651,7 @@
       <c r="BP211" s="9"/>
       <c r="BQ211" s="9"/>
     </row>
-    <row r="212" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="212" spans="1:102" s="10" customFormat="1">
       <c r="A212" s="9"/>
       <c r="B212" s="17"/>
       <c r="E212" s="9"/>
@@ -15313,7 +15702,7 @@
       <c r="BP212" s="9"/>
       <c r="BQ212" s="9"/>
     </row>
-    <row r="213" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="213" spans="1:102" s="10" customFormat="1">
       <c r="A213" s="9"/>
       <c r="B213" s="17"/>
       <c r="E213" s="9"/>
@@ -15364,7 +15753,7 @@
       <c r="BP213" s="9"/>
       <c r="BQ213" s="9"/>
     </row>
-    <row r="214" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="214" spans="1:102" s="10" customFormat="1">
       <c r="A214" s="9"/>
       <c r="B214" s="17"/>
       <c r="E214" s="9"/>
@@ -15415,7 +15804,7 @@
       <c r="BP214" s="9"/>
       <c r="BQ214" s="9"/>
     </row>
-    <row r="215" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="215" spans="1:102" s="10" customFormat="1">
       <c r="A215" s="9"/>
       <c r="B215" s="17"/>
       <c r="E215" s="9"/>
@@ -15466,7 +15855,7 @@
       <c r="BP215" s="9"/>
       <c r="BQ215" s="9"/>
     </row>
-    <row r="216" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="216" spans="1:102" s="10" customFormat="1">
       <c r="A216" s="9"/>
       <c r="B216" s="17"/>
       <c r="E216" s="9"/>
@@ -15517,7 +15906,7 @@
       <c r="BP216" s="9"/>
       <c r="BQ216" s="9"/>
     </row>
-    <row r="217" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="217" spans="1:102" s="10" customFormat="1">
       <c r="A217" s="9"/>
       <c r="B217" s="17"/>
       <c r="E217" s="9"/>
@@ -15568,7 +15957,7 @@
       <c r="BP217" s="9"/>
       <c r="BQ217" s="9"/>
     </row>
-    <row r="218" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="218" spans="1:102" s="10" customFormat="1">
       <c r="A218" s="9"/>
       <c r="B218" s="17"/>
       <c r="E218" s="9"/>
@@ -15619,7 +16008,7 @@
       <c r="BP218" s="9"/>
       <c r="BQ218" s="9"/>
     </row>
-    <row r="219" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="219" spans="1:102" s="10" customFormat="1">
       <c r="A219" s="9"/>
       <c r="B219" s="17"/>
       <c r="E219" s="9"/>
@@ -15670,7 +16059,7 @@
       <c r="BP219" s="9"/>
       <c r="BQ219" s="9"/>
     </row>
-    <row r="220" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="220" spans="1:102" s="10" customFormat="1">
       <c r="A220" s="9"/>
       <c r="B220" s="17"/>
       <c r="E220" s="9"/>
@@ -15721,7 +16110,7 @@
       <c r="BP220" s="9"/>
       <c r="BQ220" s="9"/>
     </row>
-    <row r="221" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="221" spans="1:102" s="10" customFormat="1">
       <c r="A221" s="9"/>
       <c r="B221" s="17"/>
       <c r="E221" s="9"/>
@@ -15772,7 +16161,7 @@
       <c r="BP221" s="9"/>
       <c r="BQ221" s="9"/>
     </row>
-    <row r="222" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="222" spans="1:102" s="10" customFormat="1">
       <c r="A222" s="9"/>
       <c r="B222" s="17"/>
       <c r="E222" s="9"/>
@@ -15823,7 +16212,7 @@
       <c r="BP222" s="9"/>
       <c r="BQ222" s="9"/>
     </row>
-    <row r="223" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="223" spans="1:102" s="10" customFormat="1">
       <c r="A223" s="9"/>
       <c r="B223" s="17"/>
       <c r="E223" s="9"/>
@@ -15874,7 +16263,7 @@
       <c r="BP223" s="9"/>
       <c r="BQ223" s="9"/>
     </row>
-    <row r="224" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="224" spans="1:102" s="10" customFormat="1">
       <c r="A224" s="9"/>
       <c r="B224" s="17"/>
       <c r="E224" s="9"/>
@@ -15925,7 +16314,7 @@
       <c r="BP224" s="9"/>
       <c r="BQ224" s="9"/>
     </row>
-    <row r="225" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="225" spans="1:102" s="10" customFormat="1">
       <c r="A225" s="9"/>
       <c r="B225" s="17"/>
       <c r="E225" s="9"/>
@@ -15976,7 +16365,7 @@
       <c r="BP225" s="9"/>
       <c r="BQ225" s="9"/>
     </row>
-    <row r="226" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="226" spans="1:102" s="10" customFormat="1">
       <c r="A226" s="9"/>
       <c r="B226" s="17"/>
       <c r="E226" s="9"/>
@@ -16027,7 +16416,7 @@
       <c r="BP226" s="9"/>
       <c r="BQ226" s="9"/>
     </row>
-    <row r="227" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="227" spans="1:102" s="10" customFormat="1">
       <c r="A227" s="9"/>
       <c r="B227" s="17"/>
       <c r="E227" s="9"/>
@@ -16078,7 +16467,7 @@
       <c r="BP227" s="9"/>
       <c r="BQ227" s="9"/>
     </row>
-    <row r="228" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="228" spans="1:102" s="10" customFormat="1">
       <c r="A228" s="9"/>
       <c r="B228" s="17"/>
       <c r="E228" s="9"/>
@@ -16129,7 +16518,7 @@
       <c r="BP228" s="9"/>
       <c r="BQ228" s="9"/>
     </row>
-    <row r="229" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="229" spans="1:102" s="10" customFormat="1">
       <c r="A229" s="9"/>
       <c r="B229" s="17"/>
       <c r="E229" s="9"/>
@@ -16180,7 +16569,7 @@
       <c r="BP229" s="9"/>
       <c r="BQ229" s="9"/>
     </row>
-    <row r="230" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="230" spans="1:102" s="10" customFormat="1">
       <c r="A230" s="9"/>
       <c r="B230" s="17"/>
       <c r="E230" s="9"/>
@@ -16231,7 +16620,7 @@
       <c r="BP230" s="9"/>
       <c r="BQ230" s="9"/>
     </row>
-    <row r="231" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="231" spans="1:102" s="10" customFormat="1">
       <c r="A231" s="9"/>
       <c r="B231" s="17"/>
       <c r="E231" s="9"/>
@@ -16282,7 +16671,7 @@
       <c r="BP231" s="9"/>
       <c r="BQ231" s="9"/>
     </row>
-    <row r="232" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="232" spans="1:102" s="10" customFormat="1">
       <c r="A232" s="9"/>
       <c r="B232" s="17"/>
       <c r="E232" s="9"/>
@@ -16333,7 +16722,7 @@
       <c r="BP232" s="9"/>
       <c r="BQ232" s="9"/>
     </row>
-    <row r="233" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="233" spans="1:102" s="10" customFormat="1">
       <c r="A233" s="9"/>
       <c r="B233" s="17"/>
       <c r="E233" s="9"/>
@@ -16384,7 +16773,7 @@
       <c r="BP233" s="9"/>
       <c r="BQ233" s="9"/>
     </row>
-    <row r="234" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="234" spans="1:102" s="10" customFormat="1">
       <c r="A234" s="9"/>
       <c r="B234" s="17"/>
       <c r="E234" s="9"/>
@@ -16435,7 +16824,7 @@
       <c r="BP234" s="9"/>
       <c r="BQ234" s="9"/>
     </row>
-    <row r="235" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="235" spans="1:102" s="10" customFormat="1">
       <c r="A235" s="9"/>
       <c r="B235" s="17"/>
       <c r="E235" s="9"/>
@@ -16486,7 +16875,7 @@
       <c r="BP235" s="9"/>
       <c r="BQ235" s="9"/>
     </row>
-    <row r="236" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="236" spans="1:102" s="10" customFormat="1">
       <c r="A236" s="9"/>
       <c r="B236" s="17"/>
       <c r="E236" s="9"/>
@@ -16537,7 +16926,7 @@
       <c r="BP236" s="9"/>
       <c r="BQ236" s="9"/>
     </row>
-    <row r="237" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="237" spans="1:102" s="10" customFormat="1">
       <c r="A237" s="9"/>
       <c r="B237" s="17"/>
       <c r="E237" s="9"/>
@@ -16588,7 +16977,7 @@
       <c r="BP237" s="9"/>
       <c r="BQ237" s="9"/>
     </row>
-    <row r="238" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="238" spans="1:102" s="10" customFormat="1">
       <c r="A238" s="9"/>
       <c r="B238" s="17"/>
       <c r="E238" s="9"/>
@@ -16639,7 +17028,7 @@
       <c r="BP238" s="9"/>
       <c r="BQ238" s="9"/>
     </row>
-    <row r="239" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="239" spans="1:102" s="10" customFormat="1">
       <c r="A239" s="9"/>
       <c r="B239" s="17"/>
       <c r="E239" s="9"/>
@@ -16690,7 +17079,7 @@
       <c r="BP239" s="9"/>
       <c r="BQ239" s="9"/>
     </row>
-    <row r="240" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="240" spans="1:102" s="10" customFormat="1">
       <c r="A240" s="9"/>
       <c r="B240" s="17"/>
       <c r="E240" s="9"/>
@@ -16741,7 +17130,7 @@
       <c r="BP240" s="9"/>
       <c r="BQ240" s="9"/>
     </row>
-    <row r="241" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="241" spans="1:102" s="10" customFormat="1">
       <c r="A241" s="9"/>
       <c r="B241" s="17"/>
       <c r="E241" s="9"/>
@@ -16792,7 +17181,7 @@
       <c r="BP241" s="9"/>
       <c r="BQ241" s="9"/>
     </row>
-    <row r="242" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="242" spans="1:102" s="10" customFormat="1">
       <c r="A242" s="9"/>
       <c r="B242" s="17"/>
       <c r="E242" s="9"/>
@@ -16843,7 +17232,7 @@
       <c r="BP242" s="9"/>
       <c r="BQ242" s="9"/>
     </row>
-    <row r="243" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="243" spans="1:102" s="10" customFormat="1">
       <c r="A243" s="9"/>
       <c r="B243" s="17"/>
       <c r="E243" s="9"/>
@@ -16894,7 +17283,7 @@
       <c r="BP243" s="9"/>
       <c r="BQ243" s="9"/>
     </row>
-    <row r="244" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="244" spans="1:102" s="10" customFormat="1">
       <c r="A244" s="9"/>
       <c r="B244" s="17"/>
       <c r="E244" s="9"/>
@@ -16945,7 +17334,7 @@
       <c r="BP244" s="9"/>
       <c r="BQ244" s="9"/>
     </row>
-    <row r="245" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="245" spans="1:102" s="10" customFormat="1">
       <c r="A245" s="9"/>
       <c r="B245" s="17"/>
       <c r="E245" s="9"/>
@@ -16996,7 +17385,7 @@
       <c r="BP245" s="9"/>
       <c r="BQ245" s="9"/>
     </row>
-    <row r="246" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="246" spans="1:102" s="10" customFormat="1">
       <c r="A246" s="9"/>
       <c r="B246" s="17"/>
       <c r="E246" s="9"/>
@@ -17047,7 +17436,7 @@
       <c r="BP246" s="9"/>
       <c r="BQ246" s="9"/>
     </row>
-    <row r="247" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="247" spans="1:102" s="10" customFormat="1">
       <c r="A247" s="9"/>
       <c r="B247" s="17"/>
       <c r="E247" s="9"/>
@@ -17098,7 +17487,7 @@
       <c r="BP247" s="9"/>
       <c r="BQ247" s="9"/>
     </row>
-    <row r="248" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="248" spans="1:102" s="10" customFormat="1">
       <c r="A248" s="9"/>
       <c r="B248" s="17"/>
       <c r="E248" s="9"/>
@@ -17149,7 +17538,7 @@
       <c r="BP248" s="9"/>
       <c r="BQ248" s="9"/>
     </row>
-    <row r="249" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="249" spans="1:102" s="10" customFormat="1">
       <c r="A249" s="9"/>
       <c r="B249" s="17"/>
       <c r="E249" s="9"/>
@@ -17200,7 +17589,7 @@
       <c r="BP249" s="9"/>
       <c r="BQ249" s="9"/>
     </row>
-    <row r="250" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="250" spans="1:102" s="10" customFormat="1">
       <c r="A250" s="9"/>
       <c r="B250" s="17"/>
       <c r="E250" s="9"/>
@@ -17251,7 +17640,7 @@
       <c r="BP250" s="9"/>
       <c r="BQ250" s="9"/>
     </row>
-    <row r="251" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="251" spans="1:102" s="10" customFormat="1">
       <c r="A251" s="9"/>
       <c r="B251" s="17"/>
       <c r="E251" s="9"/>
@@ -17302,7 +17691,7 @@
       <c r="BP251" s="9"/>
       <c r="BQ251" s="9"/>
     </row>
-    <row r="252" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="252" spans="1:102" s="10" customFormat="1">
       <c r="A252" s="9"/>
       <c r="B252" s="17"/>
       <c r="E252" s="9"/>
@@ -17353,7 +17742,7 @@
       <c r="BP252" s="9"/>
       <c r="BQ252" s="9"/>
     </row>
-    <row r="253" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="253" spans="1:102" s="10" customFormat="1">
       <c r="A253" s="9"/>
       <c r="B253" s="17"/>
       <c r="E253" s="9"/>
@@ -17404,7 +17793,7 @@
       <c r="BP253" s="9"/>
       <c r="BQ253" s="9"/>
     </row>
-    <row r="254" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="254" spans="1:102" s="10" customFormat="1">
       <c r="A254" s="9"/>
       <c r="B254" s="17"/>
       <c r="E254" s="9"/>
@@ -17455,7 +17844,7 @@
       <c r="BP254" s="9"/>
       <c r="BQ254" s="9"/>
     </row>
-    <row r="255" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="255" spans="1:102" s="10" customFormat="1">
       <c r="A255" s="9"/>
       <c r="B255" s="17"/>
       <c r="E255" s="9"/>
@@ -17506,7 +17895,7 @@
       <c r="BP255" s="9"/>
       <c r="BQ255" s="9"/>
     </row>
-    <row r="256" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="256" spans="1:102" s="10" customFormat="1">
       <c r="A256" s="9"/>
       <c r="B256" s="17"/>
       <c r="E256" s="9"/>
@@ -17557,7 +17946,7 @@
       <c r="BP256" s="9"/>
       <c r="BQ256" s="9"/>
     </row>
-    <row r="257" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="257" spans="1:102" s="10" customFormat="1">
       <c r="A257" s="9"/>
       <c r="B257" s="17"/>
       <c r="E257" s="9"/>
@@ -17608,7 +17997,7 @@
       <c r="BP257" s="9"/>
       <c r="BQ257" s="9"/>
     </row>
-    <row r="258" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="258" spans="1:102" s="10" customFormat="1">
       <c r="A258" s="9"/>
       <c r="B258" s="17"/>
       <c r="E258" s="9"/>
@@ -17659,7 +18048,7 @@
       <c r="BP258" s="9"/>
       <c r="BQ258" s="9"/>
     </row>
-    <row r="259" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="259" spans="1:102" s="10" customFormat="1">
       <c r="A259" s="9"/>
       <c r="B259" s="17"/>
       <c r="E259" s="9"/>
@@ -17710,7 +18099,7 @@
       <c r="BP259" s="9"/>
       <c r="BQ259" s="9"/>
     </row>
-    <row r="260" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="260" spans="1:102" s="10" customFormat="1">
       <c r="A260" s="9"/>
       <c r="B260" s="17"/>
       <c r="E260" s="9"/>
@@ -17761,7 +18150,7 @@
       <c r="BP260" s="9"/>
       <c r="BQ260" s="9"/>
     </row>
-    <row r="261" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="261" spans="1:102" s="10" customFormat="1">
       <c r="A261" s="9"/>
       <c r="B261" s="17"/>
       <c r="E261" s="9"/>
@@ -17812,7 +18201,7 @@
       <c r="BP261" s="9"/>
       <c r="BQ261" s="9"/>
     </row>
-    <row r="262" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="262" spans="1:102" s="10" customFormat="1">
       <c r="A262" s="9"/>
       <c r="B262" s="17"/>
       <c r="E262" s="9"/>
@@ -17863,7 +18252,7 @@
       <c r="BP262" s="9"/>
       <c r="BQ262" s="9"/>
     </row>
-    <row r="263" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="263" spans="1:102" s="10" customFormat="1">
       <c r="A263" s="9"/>
       <c r="B263" s="17"/>
       <c r="E263" s="9"/>
@@ -17914,7 +18303,7 @@
       <c r="BP263" s="9"/>
       <c r="BQ263" s="9"/>
     </row>
-    <row r="264" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="264" spans="1:102" s="10" customFormat="1">
       <c r="A264" s="9"/>
       <c r="B264" s="17"/>
       <c r="E264" s="9"/>
@@ -17965,7 +18354,7 @@
       <c r="BP264" s="9"/>
       <c r="BQ264" s="9"/>
     </row>
-    <row r="265" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="265" spans="1:102" s="10" customFormat="1">
       <c r="A265" s="9"/>
       <c r="B265" s="17"/>
       <c r="E265" s="9"/>
@@ -18016,7 +18405,7 @@
       <c r="BP265" s="9"/>
       <c r="BQ265" s="9"/>
     </row>
-    <row r="266" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="266" spans="1:102" s="10" customFormat="1">
       <c r="A266" s="9"/>
       <c r="B266" s="17"/>
       <c r="E266" s="9"/>
@@ -18067,7 +18456,7 @@
       <c r="BP266" s="9"/>
       <c r="BQ266" s="9"/>
     </row>
-    <row r="267" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="267" spans="1:102" s="10" customFormat="1">
       <c r="A267" s="9"/>
       <c r="B267" s="17"/>
       <c r="E267" s="9"/>
@@ -18118,7 +18507,7 @@
       <c r="BP267" s="9"/>
       <c r="BQ267" s="9"/>
     </row>
-    <row r="268" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="268" spans="1:102" s="10" customFormat="1">
       <c r="A268" s="9"/>
       <c r="B268" s="17"/>
       <c r="E268" s="9"/>
@@ -18169,7 +18558,7 @@
       <c r="BP268" s="9"/>
       <c r="BQ268" s="9"/>
     </row>
-    <row r="269" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="269" spans="1:102" s="10" customFormat="1">
       <c r="A269" s="9"/>
       <c r="B269" s="17"/>
       <c r="E269" s="9"/>
@@ -18220,7 +18609,7 @@
       <c r="BP269" s="9"/>
       <c r="BQ269" s="9"/>
     </row>
-    <row r="270" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="270" spans="1:102" s="10" customFormat="1">
       <c r="A270" s="9"/>
       <c r="B270" s="17"/>
       <c r="E270" s="9"/>
@@ -18271,7 +18660,7 @@
       <c r="BP270" s="9"/>
       <c r="BQ270" s="9"/>
     </row>
-    <row r="271" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="271" spans="1:102" s="10" customFormat="1">
       <c r="A271" s="9"/>
       <c r="B271" s="17"/>
       <c r="E271" s="9"/>
@@ -18322,7 +18711,7 @@
       <c r="BP271" s="9"/>
       <c r="BQ271" s="9"/>
     </row>
-    <row r="272" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="272" spans="1:102" s="10" customFormat="1">
       <c r="A272" s="9"/>
       <c r="B272" s="17"/>
       <c r="E272" s="9"/>
@@ -18373,7 +18762,7 @@
       <c r="BP272" s="9"/>
       <c r="BQ272" s="9"/>
     </row>
-    <row r="273" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="273" spans="1:102" s="10" customFormat="1">
       <c r="A273" s="9"/>
       <c r="B273" s="17"/>
       <c r="E273" s="9"/>
@@ -18424,7 +18813,7 @@
       <c r="BP273" s="9"/>
       <c r="BQ273" s="9"/>
     </row>
-    <row r="274" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="274" spans="1:102" s="10" customFormat="1">
       <c r="A274" s="9"/>
       <c r="B274" s="17"/>
       <c r="E274" s="9"/>
@@ -18475,7 +18864,7 @@
       <c r="BP274" s="9"/>
       <c r="BQ274" s="9"/>
     </row>
-    <row r="275" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="275" spans="1:102" s="10" customFormat="1">
       <c r="A275" s="9"/>
       <c r="B275" s="17"/>
       <c r="E275" s="9"/>
@@ -18526,7 +18915,7 @@
       <c r="BP275" s="9"/>
       <c r="BQ275" s="9"/>
     </row>
-    <row r="276" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="276" spans="1:102" s="10" customFormat="1">
       <c r="A276" s="9"/>
       <c r="B276" s="17"/>
       <c r="E276" s="9"/>
@@ -18577,6 +18966,159 @@
       <c r="BP276" s="9"/>
       <c r="BQ276" s="9"/>
     </row>
+    <row r="277" spans="1:102" s="10" customFormat="1">
+      <c r="A277" s="9"/>
+      <c r="B277" s="17"/>
+      <c r="E277" s="9"/>
+      <c r="F277" s="9"/>
+      <c r="G277" s="9"/>
+      <c r="K277" s="28"/>
+      <c r="L277" s="9"/>
+      <c r="M277" s="9"/>
+      <c r="N277" s="9"/>
+      <c r="O277" s="9"/>
+      <c r="P277" s="9"/>
+      <c r="Q277" s="29"/>
+      <c r="R277" s="29"/>
+      <c r="U277" s="9"/>
+      <c r="V277" s="9"/>
+      <c r="W277" s="9"/>
+      <c r="X277" s="9"/>
+      <c r="Y277" s="9"/>
+      <c r="Z277" s="9"/>
+      <c r="AA277" s="9"/>
+      <c r="AB277" s="9"/>
+      <c r="AC277" s="9"/>
+      <c r="AD277" s="9"/>
+      <c r="AE277" s="9"/>
+      <c r="AF277" s="9"/>
+      <c r="AG277" s="9"/>
+      <c r="AH277" s="9"/>
+      <c r="AJ277" s="9"/>
+      <c r="AK277" s="9"/>
+      <c r="AL277" s="9"/>
+      <c r="AM277" s="9"/>
+      <c r="AN277" s="9"/>
+      <c r="AO277" s="9"/>
+      <c r="AP277" s="9"/>
+      <c r="AR277" s="9"/>
+      <c r="AT277" s="9"/>
+      <c r="AU277" s="9"/>
+      <c r="AV277" s="9"/>
+      <c r="AW277" s="9"/>
+      <c r="AX277" s="9"/>
+      <c r="BH277" s="9"/>
+      <c r="BJ277" s="9"/>
+      <c r="BK277" s="9"/>
+      <c r="BL277" s="9"/>
+      <c r="BM277" s="9"/>
+      <c r="BN277" s="9"/>
+      <c r="BO277" s="9"/>
+      <c r="BP277" s="9"/>
+      <c r="BQ277" s="9"/>
+    </row>
+    <row r="278" spans="1:102" s="10" customFormat="1">
+      <c r="A278" s="9"/>
+      <c r="B278" s="17"/>
+      <c r="E278" s="9"/>
+      <c r="F278" s="9"/>
+      <c r="G278" s="9"/>
+      <c r="K278" s="28"/>
+      <c r="L278" s="9"/>
+      <c r="M278" s="9"/>
+      <c r="N278" s="9"/>
+      <c r="O278" s="9"/>
+      <c r="P278" s="9"/>
+      <c r="Q278" s="29"/>
+      <c r="R278" s="29"/>
+      <c r="U278" s="9"/>
+      <c r="V278" s="9"/>
+      <c r="W278" s="9"/>
+      <c r="X278" s="9"/>
+      <c r="Y278" s="9"/>
+      <c r="Z278" s="9"/>
+      <c r="AA278" s="9"/>
+      <c r="AB278" s="9"/>
+      <c r="AC278" s="9"/>
+      <c r="AD278" s="9"/>
+      <c r="AE278" s="9"/>
+      <c r="AF278" s="9"/>
+      <c r="AG278" s="9"/>
+      <c r="AH278" s="9"/>
+      <c r="AJ278" s="9"/>
+      <c r="AK278" s="9"/>
+      <c r="AL278" s="9"/>
+      <c r="AM278" s="9"/>
+      <c r="AN278" s="9"/>
+      <c r="AO278" s="9"/>
+      <c r="AP278" s="9"/>
+      <c r="AR278" s="9"/>
+      <c r="AT278" s="9"/>
+      <c r="AU278" s="9"/>
+      <c r="AV278" s="9"/>
+      <c r="AW278" s="9"/>
+      <c r="AX278" s="9"/>
+      <c r="BH278" s="9"/>
+      <c r="BJ278" s="9"/>
+      <c r="BK278" s="9"/>
+      <c r="BL278" s="9"/>
+      <c r="BM278" s="9"/>
+      <c r="BN278" s="9"/>
+      <c r="BO278" s="9"/>
+      <c r="BP278" s="9"/>
+      <c r="BQ278" s="9"/>
+    </row>
+    <row r="279" spans="1:102" s="10" customFormat="1">
+      <c r="A279" s="9"/>
+      <c r="B279" s="17"/>
+      <c r="E279" s="9"/>
+      <c r="F279" s="9"/>
+      <c r="G279" s="9"/>
+      <c r="K279" s="28"/>
+      <c r="L279" s="9"/>
+      <c r="M279" s="9"/>
+      <c r="N279" s="9"/>
+      <c r="O279" s="9"/>
+      <c r="P279" s="9"/>
+      <c r="Q279" s="29"/>
+      <c r="R279" s="29"/>
+      <c r="U279" s="9"/>
+      <c r="V279" s="9"/>
+      <c r="W279" s="9"/>
+      <c r="X279" s="9"/>
+      <c r="Y279" s="9"/>
+      <c r="Z279" s="9"/>
+      <c r="AA279" s="9"/>
+      <c r="AB279" s="9"/>
+      <c r="AC279" s="9"/>
+      <c r="AD279" s="9"/>
+      <c r="AE279" s="9"/>
+      <c r="AF279" s="9"/>
+      <c r="AG279" s="9"/>
+      <c r="AH279" s="9"/>
+      <c r="AJ279" s="9"/>
+      <c r="AK279" s="9"/>
+      <c r="AL279" s="9"/>
+      <c r="AM279" s="9"/>
+      <c r="AN279" s="9"/>
+      <c r="AO279" s="9"/>
+      <c r="AP279" s="9"/>
+      <c r="AR279" s="9"/>
+      <c r="AT279" s="9"/>
+      <c r="AU279" s="9"/>
+      <c r="AV279" s="9"/>
+      <c r="AW279" s="9"/>
+      <c r="AX279" s="9"/>
+      <c r="BH279" s="9"/>
+      <c r="BJ279" s="9"/>
+      <c r="BK279" s="9"/>
+      <c r="BL279" s="9"/>
+      <c r="BM279" s="9"/>
+      <c r="BN279" s="9"/>
+      <c r="BO279" s="9"/>
+      <c r="BP279" s="9"/>
+      <c r="BQ279" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="X19" r:id="rId1" display="BOILERSOIL@GMAIL.COM :: Oil Burner Installer :: CONTROLLED PLBG CO., INC"/>
@@ -18600,8 +19142,13 @@
     <hyperlink ref="AA27" r:id="rId19"/>
     <hyperlink ref="AB27" r:id="rId20"/>
     <hyperlink ref="E27" r:id="rId21"/>
+    <hyperlink ref="X31" r:id="rId22" display="BOILERSOIL@GMAIL.COM :: Oil Burner Installer :: CONTROLLED PLBG CO., INC"/>
+    <hyperlink ref="T31" r:id="rId23"/>
+    <hyperlink ref="AA31" r:id="rId24"/>
+    <hyperlink ref="AB31" r:id="rId25"/>
+    <hyperlink ref="E31" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
latest data files as of 2019-01-24c
latest data files as of 2019-01-24c - 1 file
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases BEMSST.xlsx
+++ b/src/com/data/Test Cases BEMSST.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1185" windowWidth="23115" windowHeight="11520" tabRatio="152" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1185" windowWidth="22185" windowHeight="11250" tabRatio="152" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="186">
   <si>
     <t>TCID</t>
   </si>
@@ -402,9 +402,6 @@
     <t>Professional Certification</t>
   </si>
   <si>
-    <t>BOILERPLUMBER@GMAIL.COM :: Master Plumber :: THE PLUMBING COMPANY INC :: APPLEROME16@GMAIL.COM</t>
-  </si>
-  <si>
     <t>AJOETEST@GMAIL.COM :: Mechanical Work :: 2 :: 1 :: 1</t>
   </si>
   <si>
@@ -415,9 +412,6 @@
   </si>
   <si>
     <t>AJOETEST@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>AJOETEST@GMAIL.COM :: Professional Engineer :: JA&amp; LLC :: APPLEROME16@GMAIL.COM</t>
   </si>
   <si>
     <t>boiler :: AJOETEST@GMAIL.COM</t>
@@ -444,12 +438,6 @@
     <t>AJOETEST@GMAIL.COM :: Structural :: 0 :: 0 :: 1</t>
   </si>
   <si>
-    <t>280 :: BROADWAY :: MANHATTAN :: 153 :: 1 :: BES</t>
-  </si>
-  <si>
-    <t>280 :: BROADWAY :: MANHATTAN :: 153 :: 1 :: BEP</t>
-  </si>
-  <si>
     <t>111 :: FIRST AVENUE :: MANHATTAN :: 448 :: 28 :: STS</t>
   </si>
   <si>
@@ -460,9 +448,6 @@
   </si>
   <si>
     <t>AJOETEST@GMAIL.COM :: Mechanical Work :: 1 :: 0 :: 1</t>
-  </si>
-  <si>
-    <t>BOILERSTEST1@GMAIL.COM :: Master Plumber :: SAMUEL &amp; SONS P &amp; H INC :: APPLEROME16@GMAIL.COM :: AJOETEST@GMAIL.COM</t>
   </si>
   <si>
     <t>1 :: AJOETEST@GMAIL.COM :: Professional Engineer :: 005546 :: Fuel-Oil Storage and Fuel-Oil Piping Systems</t>
@@ -531,9 +516,6 @@
     <t>a :: DOBTESTING123@GMAIL.COM :: Professional Engineer :: 005551 :: Fuel-Oil Storage and Fuel-Oil Piping Systems</t>
   </si>
   <si>
-    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2 :: 123456789 :: Track12345 :: APPLEROME16@GMAIL.COM :: AJOETEST2@GMAIL.COM</t>
-  </si>
-  <si>
     <t>1 :: Electrical Motors :: DOBTESTING123@GMAIL.COM :: Professional Engineer</t>
   </si>
   <si>
@@ -577,6 +559,21 @@
   </si>
   <si>
     <t>a :: AJOETEST@GMAIL.COM :: Professional Engineer :: 005546 :: Fire-resistant Penetrations and Joints :: Lowest Floor Elevation</t>
+  </si>
+  <si>
+    <t>20 :: VESEY STREET :: MANHATTAN :: 88 :: 5 :: BeNewPro</t>
+  </si>
+  <si>
+    <t>20 :: VESEY STREET :: MANHATTAN :: 88 :: 5 :: BeNewProPw2</t>
+  </si>
+  <si>
+    <t>20 :: VESEY STREET :: MANHATTAN :: 88 :: 5 :: BeNewStd</t>
+  </si>
+  <si>
+    <t>BOILERPLUMBER@GMAIL.COM :: Master Plumber :: THE PLUMBING COMPANY INC :: 123456789 :: Track12345 :: APPLEROME16@GMAIL.COM :: AJOETEST@GMAIL.COM :: skip insurance :: skip insurance :: skip insurance</t>
+  </si>
+  <si>
+    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2 :: 123456789 :: Track12345 :: APPLEROME16@GMAIL.COM :: AJOETEST@GMAIL.COM :: Liability Insurance Co. :: Worker's Comp Insurance Co. :: Disability Insurance Co.</t>
   </si>
 </sst>
 </file>
@@ -1876,7 +1873,7 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1">
       <c r="A2" s="34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="32" t="s">
@@ -1885,7 +1882,7 @@
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1">
       <c r="A3" s="34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="32" t="s">
@@ -1894,7 +1891,7 @@
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1">
       <c r="A4" s="34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B4" s="30"/>
       <c r="C4" s="32" t="s">
@@ -1903,7 +1900,7 @@
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">
       <c r="A5" s="34" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="32" t="s">
@@ -1912,7 +1909,7 @@
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1">
       <c r="A6" s="34" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="32" t="s">
@@ -1921,7 +1918,7 @@
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1">
       <c r="A7" s="34" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="32" t="s">
@@ -1930,7 +1927,7 @@
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1">
       <c r="A8" s="34" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="32" t="s">
@@ -1939,7 +1936,7 @@
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1">
       <c r="A9" s="34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="32" t="s">
@@ -1948,7 +1945,7 @@
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1">
       <c r="A10" s="34" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="32" t="s">
@@ -1957,7 +1954,7 @@
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1">
       <c r="A11" s="34" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="32" t="s">
@@ -1966,7 +1963,7 @@
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1">
       <c r="A12" s="34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="32" t="s">
@@ -2323,9 +2320,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W21" sqref="W21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -2552,7 +2549,7 @@
     </row>
     <row r="3" spans="1:102" s="7" customFormat="1">
       <c r="A3" s="34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" s="6"/>
       <c r="E3" s="3"/>
@@ -2702,7 +2699,7 @@
         <v>12</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AH4" s="5"/>
       <c r="AI4" s="12" t="s">
@@ -2888,19 +2885,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>127</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>143</v>
+        <v>181</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>108</v>
@@ -2915,7 +2912,7 @@
         <v>115</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>124</v>
@@ -2938,27 +2935,27 @@
         <v>3</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U5" s="4" t="s">
         <v>122</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="W5" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X5" s="3"/>
       <c r="Y5" s="11"/>
       <c r="Z5" s="39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC5" s="11" t="s">
         <v>3</v>
@@ -3110,7 +3107,7 @@
     </row>
     <row r="7" spans="1:102" s="7" customFormat="1">
       <c r="A7" s="34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B7" s="6"/>
       <c r="E7" s="3"/>
@@ -3260,7 +3257,7 @@
         <v>12</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AH8" s="5"/>
       <c r="AI8" s="12" t="s">
@@ -3441,24 +3438,24 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:102" s="4" customFormat="1" ht="38.25">
+    <row r="9" spans="1:102" s="4" customFormat="1" ht="51">
       <c r="A9" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>127</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>108</v>
@@ -3473,7 +3470,7 @@
         <v>115</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L9" s="11" t="s">
         <v>124</v>
@@ -3496,29 +3493,29 @@
         <v>3</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U9" s="4" t="s">
         <v>122</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="W9" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="Y9" s="11"/>
       <c r="Z9" s="39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB9" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC9" s="11" t="s">
         <v>3</v>
@@ -3670,7 +3667,7 @@
     </row>
     <row r="11" spans="1:102" s="7" customFormat="1">
       <c r="A11" s="34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B11" s="6"/>
       <c r="E11" s="3"/>
@@ -3820,7 +3817,7 @@
         <v>12</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AH12" s="5"/>
       <c r="AI12" s="12" t="s">
@@ -4006,19 +4003,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>116</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>129</v>
+        <v>163</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>108</v>
@@ -4033,7 +4030,7 @@
         <v>115</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L13" s="11" t="s">
         <v>124</v>
@@ -4056,29 +4053,27 @@
         <v>3</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>122</v>
       </c>
       <c r="V13" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="W13" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>128</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="X13" s="3"/>
       <c r="Y13" s="11"/>
       <c r="Z13" s="39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AA13" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB13" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC13" s="11" t="s">
         <v>3</v>
@@ -4230,7 +4225,7 @@
     </row>
     <row r="15" spans="1:102" s="7" customFormat="1">
       <c r="A15" s="34" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B15" s="6"/>
       <c r="E15" s="3"/>
@@ -4380,7 +4375,7 @@
         <v>12</v>
       </c>
       <c r="AG16" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AH16" s="5"/>
       <c r="AI16" s="12" t="s">
@@ -4566,22 +4561,22 @@
         <v>3</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>116</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>156</v>
+        <v>163</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>108</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>3</v>
@@ -4590,7 +4585,7 @@
         <v>115</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L17" s="11" t="s">
         <v>124</v>
@@ -4613,29 +4608,27 @@
         <v>3</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U17" s="4" t="s">
         <v>122</v>
       </c>
       <c r="V17" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="W17" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="X17" s="3" t="s">
-        <v>128</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="X17" s="3"/>
       <c r="Y17" s="11"/>
       <c r="Z17" s="39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AA17" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB17" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC17" s="11" t="s">
         <v>3</v>
@@ -4650,7 +4643,7 @@
         <v>57</v>
       </c>
       <c r="AG17" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="AH17" s="11"/>
       <c r="AJ17" s="3"/>
@@ -4789,7 +4782,7 @@
     </row>
     <row r="19" spans="1:102" s="7" customFormat="1">
       <c r="A19" s="34" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B19" s="6"/>
       <c r="E19" s="3"/>
@@ -4939,7 +4932,7 @@
         <v>12</v>
       </c>
       <c r="AG20" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AH20" s="5"/>
       <c r="AI20" s="12" t="s">
@@ -5125,22 +5118,22 @@
         <v>3</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>116</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E21" s="35" t="s">
-        <v>151</v>
+        <v>163</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>108</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>3</v>
@@ -5149,7 +5142,7 @@
         <v>115</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L21" s="11" t="s">
         <v>124</v>
@@ -5172,29 +5165,27 @@
         <v>3</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U21" s="4" t="s">
         <v>122</v>
       </c>
       <c r="V21" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="W21" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="X21" s="3" t="s">
-        <v>128</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="X21" s="3"/>
       <c r="Y21" s="11"/>
       <c r="Z21" s="39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AA21" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB21" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC21" s="11" t="s">
         <v>3</v>
@@ -5209,7 +5200,7 @@
         <v>57</v>
       </c>
       <c r="AG21" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="AH21" s="11"/>
       <c r="AJ21" s="3"/>
@@ -5348,7 +5339,7 @@
     </row>
     <row r="23" spans="1:102" s="7" customFormat="1">
       <c r="A23" s="34" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B23" s="6"/>
       <c r="E23" s="3"/>
@@ -5498,7 +5489,7 @@
         <v>12</v>
       </c>
       <c r="AG24" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AH24" s="5"/>
       <c r="AI24" s="12" t="s">
@@ -5679,24 +5670,24 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:102" s="4" customFormat="1" ht="25.5">
+    <row r="25" spans="1:102" s="4" customFormat="1" ht="38.25">
       <c r="A25" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>127</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>162</v>
+        <v>163</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>108</v>
@@ -5711,7 +5702,7 @@
         <v>115</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L25" s="11" t="s">
         <v>123</v>
@@ -5748,13 +5739,13 @@
       <c r="X25" s="3"/>
       <c r="Y25" s="11"/>
       <c r="Z25" s="39" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="AA25" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB25" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC25" s="11" t="s">
         <v>3</v>
@@ -5906,7 +5897,7 @@
     </row>
     <row r="27" spans="1:102" s="7" customFormat="1">
       <c r="A27" s="34" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B27" s="6"/>
       <c r="E27" s="3"/>
@@ -6056,7 +6047,7 @@
         <v>12</v>
       </c>
       <c r="AG28" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AH28" s="5"/>
       <c r="AI28" s="12" t="s">
@@ -6237,24 +6228,24 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:102" s="4" customFormat="1" ht="38.25">
+    <row r="29" spans="1:102" s="4" customFormat="1" ht="51">
       <c r="A29" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>127</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>108</v>
@@ -6269,7 +6260,7 @@
         <v>115</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L29" s="11" t="s">
         <v>124</v>
@@ -6298,23 +6289,23 @@
         <v>119</v>
       </c>
       <c r="V29" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="W29" s="11" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="X29" s="3" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="Y29" s="11"/>
       <c r="Z29" s="39" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="AA29" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AB29" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AC29" s="11" t="s">
         <v>3</v>
@@ -6466,7 +6457,7 @@
     </row>
     <row r="31" spans="1:102" s="7" customFormat="1">
       <c r="A31" s="34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B31" s="6"/>
       <c r="E31" s="3"/>
@@ -6616,7 +6607,7 @@
         <v>12</v>
       </c>
       <c r="AG32" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AH32" s="5"/>
       <c r="AI32" s="12" t="s">
@@ -6802,19 +6793,19 @@
         <v>3</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>116</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E33" s="35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>108</v>
@@ -6829,7 +6820,7 @@
         <v>115</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L33" s="11" t="s">
         <v>123</v>
@@ -6866,13 +6857,13 @@
       <c r="X33" s="3"/>
       <c r="Y33" s="11"/>
       <c r="Z33" s="39" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="AA33" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB33" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC33" s="11" t="s">
         <v>3</v>
@@ -7024,7 +7015,7 @@
     </row>
     <row r="35" spans="1:102" s="7" customFormat="1">
       <c r="A35" s="34" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B35" s="6"/>
       <c r="E35" s="3"/>
@@ -7174,7 +7165,7 @@
         <v>12</v>
       </c>
       <c r="AG36" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AH36" s="5"/>
       <c r="AI36" s="12" t="s">
@@ -7355,24 +7346,24 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:102" s="4" customFormat="1" ht="25.5">
+    <row r="37" spans="1:102" s="4" customFormat="1" ht="38.25">
       <c r="A37" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>127</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>108</v>
@@ -7387,7 +7378,7 @@
         <v>115</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L37" s="11" t="s">
         <v>123</v>
@@ -7416,19 +7407,19 @@
         <v>118</v>
       </c>
       <c r="V37" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="W37" s="11"/>
       <c r="X37" s="3"/>
       <c r="Y37" s="11"/>
       <c r="Z37" s="39" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="AA37" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB37" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC37" s="11" t="s">
         <v>3</v>
@@ -7526,7 +7517,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="38" spans="1:102" s="10" customFormat="1">
       <c r="A38" s="9"/>
       <c r="B38" s="17"/>
       <c r="E38" s="29"/>
@@ -7578,9 +7569,9 @@
       <c r="BP38" s="9"/>
       <c r="BQ38" s="9"/>
     </row>
-    <row r="39" spans="1:102" s="7" customFormat="1" ht="409.6">
+    <row r="39" spans="1:102" s="7" customFormat="1">
       <c r="A39" s="34" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B39" s="6"/>
       <c r="E39" s="3"/>
@@ -7730,7 +7721,7 @@
         <v>12</v>
       </c>
       <c r="AG40" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AH40" s="5"/>
       <c r="AI40" s="12" t="s">
@@ -7911,24 +7902,24 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:102" s="4" customFormat="1" ht="38.25">
+    <row r="41" spans="1:102" s="4" customFormat="1" ht="51">
       <c r="A41" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>127</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>108</v>
@@ -7943,7 +7934,7 @@
         <v>115</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L41" s="11" t="s">
         <v>123</v>
@@ -7972,23 +7963,23 @@
         <v>119</v>
       </c>
       <c r="V41" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="W41" s="11" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="X41" s="3" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="Y41" s="11"/>
       <c r="Z41" s="39" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="AA41" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AB41" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AC41" s="11" t="s">
         <v>3</v>
@@ -8086,7 +8077,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="42" spans="1:102" s="10" customFormat="1">
       <c r="A42" s="9"/>
       <c r="B42" s="17"/>
       <c r="E42" s="29"/>
@@ -8138,9 +8129,9 @@
       <c r="BP42" s="9"/>
       <c r="BQ42" s="9"/>
     </row>
-    <row r="43" spans="1:102" s="7" customFormat="1" ht="409.6">
+    <row r="43" spans="1:102" s="7" customFormat="1">
       <c r="A43" s="34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B43" s="6"/>
       <c r="E43" s="3"/>
@@ -8290,7 +8281,7 @@
         <v>12</v>
       </c>
       <c r="AG44" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AH44" s="5"/>
       <c r="AI44" s="12" t="s">
@@ -8476,19 +8467,19 @@
         <v>3</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C45" s="20" t="s">
         <v>116</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>108</v>
@@ -8503,7 +8494,7 @@
         <v>115</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>123</v>
@@ -8532,19 +8523,19 @@
         <v>118</v>
       </c>
       <c r="V45" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="W45" s="11"/>
       <c r="X45" s="3"/>
       <c r="Y45" s="11"/>
       <c r="Z45" s="39" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="AA45" s="40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB45" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC45" s="11" t="s">
         <v>3</v>
@@ -8642,7 +8633,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="46" spans="1:102" s="10" customFormat="1">
       <c r="A46" s="9"/>
       <c r="B46" s="17"/>
       <c r="E46" s="29"/>
@@ -8694,7 +8685,7 @@
       <c r="BP46" s="9"/>
       <c r="BQ46" s="9"/>
     </row>
-    <row r="47" spans="1:102" s="25" customFormat="1" ht="409.6">
+    <row r="47" spans="1:102" s="25" customFormat="1">
       <c r="A47" s="22"/>
       <c r="B47" s="23"/>
       <c r="C47" s="22"/>
@@ -8763,7 +8754,7 @@
       <c r="BP47" s="24"/>
       <c r="BQ47" s="24"/>
     </row>
-    <row r="48" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="48" spans="1:102" s="10" customFormat="1">
       <c r="A48" s="9"/>
       <c r="B48" s="17"/>
       <c r="E48" s="29"/>
@@ -8815,7 +8806,7 @@
       <c r="BP48" s="9"/>
       <c r="BQ48" s="9"/>
     </row>
-    <row r="49" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="49" spans="1:102" s="10" customFormat="1">
       <c r="A49" s="9"/>
       <c r="B49" s="17"/>
       <c r="E49" s="29"/>
@@ -8867,7 +8858,7 @@
       <c r="BP49" s="9"/>
       <c r="BQ49" s="9"/>
     </row>
-    <row r="50" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="50" spans="1:102" s="10" customFormat="1">
       <c r="A50" s="9"/>
       <c r="B50" s="17"/>
       <c r="E50" s="29"/>
@@ -8919,7 +8910,7 @@
       <c r="BP50" s="9"/>
       <c r="BQ50" s="9"/>
     </row>
-    <row r="51" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="51" spans="1:102" s="10" customFormat="1">
       <c r="A51" s="9"/>
       <c r="B51" s="17"/>
       <c r="E51" s="29"/>
@@ -8971,7 +8962,7 @@
       <c r="BP51" s="9"/>
       <c r="BQ51" s="9"/>
     </row>
-    <row r="52" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="52" spans="1:102" s="10" customFormat="1">
       <c r="A52" s="9"/>
       <c r="B52" s="17"/>
       <c r="E52" s="29"/>
@@ -9023,7 +9014,7 @@
       <c r="BP52" s="9"/>
       <c r="BQ52" s="9"/>
     </row>
-    <row r="53" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="53" spans="1:102" s="10" customFormat="1">
       <c r="A53" s="9"/>
       <c r="B53" s="17"/>
       <c r="E53" s="29"/>
@@ -9075,7 +9066,7 @@
       <c r="BP53" s="9"/>
       <c r="BQ53" s="9"/>
     </row>
-    <row r="54" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="54" spans="1:102" s="10" customFormat="1">
       <c r="A54" s="9"/>
       <c r="B54" s="17"/>
       <c r="E54" s="29"/>
@@ -9127,7 +9118,7 @@
       <c r="BP54" s="9"/>
       <c r="BQ54" s="9"/>
     </row>
-    <row r="55" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="55" spans="1:102" s="10" customFormat="1">
       <c r="A55" s="9"/>
       <c r="B55" s="17"/>
       <c r="E55" s="29"/>
@@ -9179,7 +9170,7 @@
       <c r="BP55" s="9"/>
       <c r="BQ55" s="9"/>
     </row>
-    <row r="56" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="56" spans="1:102" s="10" customFormat="1">
       <c r="A56" s="9"/>
       <c r="B56" s="17"/>
       <c r="E56" s="29"/>
@@ -9231,7 +9222,7 @@
       <c r="BP56" s="9"/>
       <c r="BQ56" s="9"/>
     </row>
-    <row r="57" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="57" spans="1:102" s="10" customFormat="1">
       <c r="A57" s="9"/>
       <c r="B57" s="17"/>
       <c r="E57" s="29"/>
@@ -9283,7 +9274,7 @@
       <c r="BP57" s="9"/>
       <c r="BQ57" s="9"/>
     </row>
-    <row r="58" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="58" spans="1:102" s="10" customFormat="1">
       <c r="A58" s="9"/>
       <c r="B58" s="17"/>
       <c r="E58" s="29"/>
@@ -9335,7 +9326,7 @@
       <c r="BP58" s="9"/>
       <c r="BQ58" s="9"/>
     </row>
-    <row r="59" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="59" spans="1:102" s="10" customFormat="1">
       <c r="A59" s="9"/>
       <c r="B59" s="17"/>
       <c r="E59" s="29"/>
@@ -9387,7 +9378,7 @@
       <c r="BP59" s="9"/>
       <c r="BQ59" s="9"/>
     </row>
-    <row r="60" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="60" spans="1:102" s="10" customFormat="1">
       <c r="A60" s="9"/>
       <c r="B60" s="17"/>
       <c r="E60" s="29"/>
@@ -9439,7 +9430,7 @@
       <c r="BP60" s="9"/>
       <c r="BQ60" s="9"/>
     </row>
-    <row r="61" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="61" spans="1:102" s="10" customFormat="1">
       <c r="A61" s="9"/>
       <c r="B61" s="17"/>
       <c r="E61" s="29"/>
@@ -9491,7 +9482,7 @@
       <c r="BP61" s="9"/>
       <c r="BQ61" s="9"/>
     </row>
-    <row r="62" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="62" spans="1:102" s="10" customFormat="1">
       <c r="A62" s="9"/>
       <c r="B62" s="17"/>
       <c r="E62" s="29"/>
@@ -9543,7 +9534,7 @@
       <c r="BP62" s="9"/>
       <c r="BQ62" s="9"/>
     </row>
-    <row r="63" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="63" spans="1:102" s="10" customFormat="1">
       <c r="A63" s="9"/>
       <c r="B63" s="17"/>
       <c r="E63" s="29"/>
@@ -9595,7 +9586,7 @@
       <c r="BP63" s="9"/>
       <c r="BQ63" s="9"/>
     </row>
-    <row r="64" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="64" spans="1:102" s="10" customFormat="1">
       <c r="A64" s="9"/>
       <c r="B64" s="17"/>
       <c r="E64" s="29"/>
@@ -9647,7 +9638,7 @@
       <c r="BP64" s="9"/>
       <c r="BQ64" s="9"/>
     </row>
-    <row r="65" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="65" spans="1:102" s="10" customFormat="1">
       <c r="A65" s="9"/>
       <c r="B65" s="17"/>
       <c r="E65" s="29"/>
@@ -9699,7 +9690,7 @@
       <c r="BP65" s="9"/>
       <c r="BQ65" s="9"/>
     </row>
-    <row r="66" spans="1:102" s="10" customFormat="1" ht="409.6">
+    <row r="66" spans="1:102" s="10" customFormat="1">
       <c r="A66" s="9"/>
       <c r="B66" s="17"/>
       <c r="E66" s="29"/>

</xml_diff>